<commit_message>
info phase documentation and update time table
</commit_message>
<xml_diff>
--- a/documentation/Zeitplan.xlsx
+++ b/documentation/Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp8\htdocs\IPA\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0DFB46-053B-42DF-98E0-4E5433967A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D9484D-496C-4F6E-8094-E933390BD5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
   <si>
     <t>Projekttitel</t>
   </si>
@@ -961,7 +961,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1138,44 +1138,143 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="40" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1237,125 +1336,32 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1643,8 +1649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,27 +1663,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:59" ht="44.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="152" t="s">
+      <c r="A1" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
-      <c r="H1" s="152"/>
-      <c r="I1" s="152"/>
-      <c r="J1" s="152"/>
-      <c r="K1" s="152"/>
-      <c r="L1" s="152"/>
-      <c r="M1" s="152"/>
-      <c r="N1" s="152"/>
-      <c r="O1" s="152"/>
-      <c r="P1" s="152"/>
-      <c r="Q1" s="152"/>
-      <c r="R1" s="152"/>
-      <c r="S1" s="152"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
@@ -2309,86 +2315,86 @@
       <c r="BG10" s="3"/>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="101"/>
-      <c r="C11" s="95" t="s">
+      <c r="B11" s="134"/>
+      <c r="C11" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="96"/>
-      <c r="E11" s="95" t="s">
+      <c r="D11" s="129"/>
+      <c r="E11" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="96"/>
-      <c r="G11" s="140" t="s">
+      <c r="F11" s="129"/>
+      <c r="G11" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="141"/>
-      <c r="I11" s="141"/>
-      <c r="J11" s="142"/>
-      <c r="K11" s="140" t="s">
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="L11" s="141"/>
-      <c r="M11" s="141"/>
-      <c r="N11" s="142"/>
-      <c r="O11" s="140" t="s">
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="P11" s="141"/>
-      <c r="Q11" s="141"/>
-      <c r="R11" s="142"/>
-      <c r="S11" s="140" t="s">
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="87"/>
+      <c r="S11" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="T11" s="141"/>
-      <c r="U11" s="141"/>
-      <c r="V11" s="142"/>
-      <c r="W11" s="140" t="s">
+      <c r="T11" s="86"/>
+      <c r="U11" s="86"/>
+      <c r="V11" s="87"/>
+      <c r="W11" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="X11" s="141"/>
-      <c r="Y11" s="141"/>
-      <c r="Z11" s="142"/>
-      <c r="AA11" s="140" t="s">
+      <c r="X11" s="86"/>
+      <c r="Y11" s="86"/>
+      <c r="Z11" s="87"/>
+      <c r="AA11" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="AB11" s="141"/>
-      <c r="AC11" s="141"/>
-      <c r="AD11" s="142"/>
-      <c r="AE11" s="140" t="s">
+      <c r="AB11" s="86"/>
+      <c r="AC11" s="86"/>
+      <c r="AD11" s="87"/>
+      <c r="AE11" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="AF11" s="141"/>
-      <c r="AG11" s="141"/>
-      <c r="AH11" s="142"/>
-      <c r="AI11" s="140" t="s">
+      <c r="AF11" s="86"/>
+      <c r="AG11" s="86"/>
+      <c r="AH11" s="87"/>
+      <c r="AI11" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="AJ11" s="141"/>
-      <c r="AK11" s="141"/>
-      <c r="AL11" s="142"/>
-      <c r="AM11" s="140" t="s">
+      <c r="AJ11" s="86"/>
+      <c r="AK11" s="86"/>
+      <c r="AL11" s="87"/>
+      <c r="AM11" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="AN11" s="141"/>
-      <c r="AO11" s="141"/>
-      <c r="AP11" s="142"/>
-      <c r="AQ11" s="140" t="s">
+      <c r="AN11" s="86"/>
+      <c r="AO11" s="86"/>
+      <c r="AP11" s="87"/>
+      <c r="AQ11" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="AR11" s="141"/>
-      <c r="AS11" s="141"/>
-      <c r="AT11" s="142"/>
+      <c r="AR11" s="86"/>
+      <c r="AS11" s="86"/>
+      <c r="AT11" s="87"/>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A12" s="102"/>
-      <c r="B12" s="101"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="96"/>
+      <c r="A12" s="135"/>
+      <c r="B12" s="134"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="129"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="129"/>
       <c r="G12" s="10">
         <v>1</v>
       </c>
@@ -2511,12 +2517,12 @@
       </c>
     </row>
     <row r="13" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="103"/>
-      <c r="B13" s="104"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="99"/>
+      <c r="A13" s="136"/>
+      <c r="B13" s="137"/>
+      <c r="C13" s="131"/>
+      <c r="D13" s="132"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="132"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
@@ -2559,20 +2565,20 @@
       <c r="AT13" s="16"/>
     </row>
     <row r="14" spans="1:59" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="143" t="s">
+      <c r="A14" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="144"/>
-      <c r="C14" s="145">
+      <c r="B14" s="89"/>
+      <c r="C14" s="90">
         <f>SUM(C15:D16)</f>
         <v>6</v>
       </c>
-      <c r="D14" s="146"/>
-      <c r="E14" s="145">
+      <c r="D14" s="91"/>
+      <c r="E14" s="90">
         <f>SUM(E15)</f>
         <v>6</v>
       </c>
-      <c r="F14" s="146"/>
+      <c r="F14" s="91"/>
       <c r="G14" s="18"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
@@ -2624,18 +2630,18 @@
       <c r="BC14" s="24"/>
     </row>
     <row r="15" spans="1:59" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="82" t="s">
+      <c r="A15" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="147"/>
-      <c r="C15" s="150">
+      <c r="B15" s="93"/>
+      <c r="C15" s="96">
         <v>6</v>
       </c>
-      <c r="D15" s="131"/>
-      <c r="E15" s="150">
+      <c r="D15" s="97"/>
+      <c r="E15" s="96">
         <v>6</v>
       </c>
-      <c r="F15" s="131"/>
+      <c r="F15" s="97"/>
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
       <c r="I15" s="26"/>
@@ -2683,12 +2689,12 @@
       <c r="BC15" s="29"/>
     </row>
     <row r="16" spans="1:59" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="148"/>
-      <c r="B16" s="149"/>
-      <c r="C16" s="151"/>
-      <c r="D16" s="133"/>
-      <c r="E16" s="151"/>
-      <c r="F16" s="133"/>
+      <c r="A16" s="94"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="99"/>
       <c r="G16" s="30"/>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
@@ -2729,20 +2735,20 @@
       <c r="BC16" s="29"/>
     </row>
     <row r="17" spans="1:55" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="117" t="s">
+      <c r="A17" s="112" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="118"/>
-      <c r="C17" s="115">
+      <c r="B17" s="113"/>
+      <c r="C17" s="114">
         <f>SUM(C18:D25)</f>
         <v>12</v>
       </c>
-      <c r="D17" s="116"/>
-      <c r="E17" s="134">
+      <c r="D17" s="115"/>
+      <c r="E17" s="116">
         <f>SUM(E18:F25)</f>
         <v>12</v>
       </c>
-      <c r="F17" s="135"/>
+      <c r="F17" s="117"/>
       <c r="G17" s="31"/>
       <c r="H17" s="32"/>
       <c r="I17" s="32"/>
@@ -2792,18 +2798,18 @@
       <c r="BC17" s="29"/>
     </row>
     <row r="18" spans="1:55" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="82" t="s">
+      <c r="A18" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="83"/>
-      <c r="C18" s="86">
+      <c r="B18" s="105"/>
+      <c r="C18" s="104">
         <v>6</v>
       </c>
-      <c r="D18" s="83"/>
-      <c r="E18" s="86">
+      <c r="D18" s="105"/>
+      <c r="E18" s="104">
         <v>6</v>
       </c>
-      <c r="F18" s="83"/>
+      <c r="F18" s="105"/>
       <c r="G18" s="52"/>
       <c r="H18" s="53"/>
       <c r="I18" s="53"/>
@@ -2853,12 +2859,12 @@
       <c r="BC18" s="29"/>
     </row>
     <row r="19" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="84"/>
-      <c r="B19" s="85"/>
-      <c r="C19" s="87"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="85"/>
+      <c r="A19" s="118"/>
+      <c r="B19" s="107"/>
+      <c r="C19" s="106"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="106"/>
+      <c r="F19" s="107"/>
       <c r="G19" s="51"/>
       <c r="H19" s="59"/>
       <c r="I19" s="59"/>
@@ -2903,18 +2909,18 @@
       <c r="BC19" s="29"/>
     </row>
     <row r="20" spans="1:55" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="82" t="s">
+      <c r="A20" s="92" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="83"/>
-      <c r="C20" s="86">
+      <c r="B20" s="105"/>
+      <c r="C20" s="104">
         <v>2</v>
       </c>
-      <c r="D20" s="83"/>
-      <c r="E20" s="86">
+      <c r="D20" s="105"/>
+      <c r="E20" s="104">
         <v>2</v>
       </c>
-      <c r="F20" s="83"/>
+      <c r="F20" s="105"/>
       <c r="J20" s="50"/>
       <c r="K20" s="25"/>
       <c r="L20" s="26"/>
@@ -2963,15 +2969,15 @@
       <c r="BC20" s="37"/>
     </row>
     <row r="21" spans="1:55" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="84"/>
-      <c r="B21" s="85"/>
-      <c r="C21" s="87"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="85"/>
+      <c r="A21" s="118"/>
+      <c r="B21" s="107"/>
+      <c r="C21" s="106"/>
+      <c r="D21" s="107"/>
+      <c r="E21" s="106"/>
+      <c r="F21" s="107"/>
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
-      <c r="J21" s="153"/>
+      <c r="J21" s="82"/>
       <c r="K21" s="25"/>
       <c r="L21" s="26"/>
       <c r="M21" s="26"/>
@@ -3010,18 +3016,18 @@
       <c r="AT21" s="35"/>
     </row>
     <row r="22" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="119" t="s">
+      <c r="A22" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="120"/>
-      <c r="C22" s="86">
+      <c r="B22" s="101"/>
+      <c r="C22" s="104">
         <v>2</v>
       </c>
-      <c r="D22" s="83"/>
-      <c r="E22" s="86">
+      <c r="D22" s="105"/>
+      <c r="E22" s="104">
         <v>2</v>
       </c>
-      <c r="F22" s="83"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="25"/>
       <c r="J22" s="56"/>
       <c r="K22" s="61"/>
@@ -3061,14 +3067,14 @@
       <c r="AT22" s="35"/>
     </row>
     <row r="23" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="121"/>
-      <c r="B23" s="122"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="85"/>
+      <c r="A23" s="102"/>
+      <c r="B23" s="103"/>
+      <c r="C23" s="106"/>
+      <c r="D23" s="107"/>
+      <c r="E23" s="106"/>
+      <c r="F23" s="107"/>
       <c r="G23" s="25"/>
-      <c r="J23" s="154"/>
+      <c r="J23" s="83"/>
       <c r="K23" s="27"/>
       <c r="L23" s="26"/>
       <c r="M23" s="26"/>
@@ -3107,18 +3113,18 @@
       <c r="AT23" s="35"/>
     </row>
     <row r="24" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="119" t="s">
+      <c r="A24" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="120"/>
-      <c r="C24" s="86">
+      <c r="B24" s="101"/>
+      <c r="C24" s="104">
         <v>2</v>
       </c>
-      <c r="D24" s="83"/>
-      <c r="E24" s="136">
+      <c r="D24" s="105"/>
+      <c r="E24" s="108">
         <v>2</v>
       </c>
-      <c r="F24" s="137"/>
+      <c r="F24" s="109"/>
       <c r="G24" s="25"/>
       <c r="I24" s="26"/>
       <c r="J24" s="67"/>
@@ -3162,16 +3168,18 @@
       <c r="AT24" s="35"/>
     </row>
     <row r="25" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="121"/>
-      <c r="B25" s="122"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="138"/>
-      <c r="F25" s="139"/>
+      <c r="A25" s="102"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="106"/>
+      <c r="D25" s="107"/>
+      <c r="E25" s="110"/>
+      <c r="F25" s="111"/>
       <c r="G25" s="25"/>
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
-      <c r="K25" s="25"/>
+      <c r="K25" s="155" t="s">
+        <v>25</v>
+      </c>
       <c r="L25" s="26"/>
       <c r="M25" s="26"/>
       <c r="N25" s="35"/>
@@ -3209,20 +3217,20 @@
       <c r="AT25" s="35"/>
     </row>
     <row r="26" spans="1:55" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="117" t="s">
+      <c r="A26" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="118"/>
-      <c r="C26" s="115">
+      <c r="B26" s="113"/>
+      <c r="C26" s="114">
         <f>SUM(C27)</f>
         <v>2</v>
       </c>
-      <c r="D26" s="116"/>
-      <c r="E26" s="134">
+      <c r="D26" s="115"/>
+      <c r="E26" s="116">
         <f>SUM(E27)</f>
         <v>2</v>
       </c>
-      <c r="F26" s="135"/>
+      <c r="F26" s="117"/>
       <c r="G26" s="31"/>
       <c r="H26" s="32"/>
       <c r="I26" s="32"/>
@@ -3265,18 +3273,18 @@
       <c r="AT26" s="33"/>
     </row>
     <row r="27" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="82" t="s">
+      <c r="A27" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="83"/>
-      <c r="C27" s="86">
+      <c r="B27" s="105"/>
+      <c r="C27" s="104">
         <v>2</v>
       </c>
-      <c r="D27" s="83"/>
-      <c r="E27" s="86">
+      <c r="D27" s="105"/>
+      <c r="E27" s="104">
         <v>2</v>
       </c>
-      <c r="F27" s="83"/>
+      <c r="F27" s="105"/>
       <c r="G27" s="25"/>
       <c r="H27" s="26"/>
       <c r="I27" s="26"/>
@@ -3318,16 +3326,19 @@
       <c r="AT27" s="35"/>
     </row>
     <row r="28" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="84"/>
-      <c r="B28" s="85"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="85"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="85"/>
+      <c r="A28" s="118"/>
+      <c r="B28" s="107"/>
+      <c r="C28" s="106"/>
+      <c r="D28" s="107"/>
+      <c r="E28" s="106"/>
+      <c r="F28" s="107"/>
       <c r="G28" s="25"/>
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
       <c r="J28" s="35"/>
+      <c r="L28" s="156" t="s">
+        <v>29</v>
+      </c>
       <c r="M28" s="26"/>
       <c r="N28" s="35"/>
       <c r="O28" s="25"/>
@@ -3364,20 +3375,20 @@
       <c r="AT28" s="35"/>
     </row>
     <row r="29" spans="1:55" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="117" t="s">
+      <c r="A29" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="118"/>
-      <c r="C29" s="115">
+      <c r="B29" s="113"/>
+      <c r="C29" s="114">
         <f>SUM(C30:D39)</f>
         <v>12</v>
       </c>
-      <c r="D29" s="116"/>
-      <c r="E29" s="115">
+      <c r="D29" s="115"/>
+      <c r="E29" s="114">
         <f>SUM(E30:F39)</f>
         <v>12</v>
       </c>
-      <c r="F29" s="116"/>
+      <c r="F29" s="115"/>
       <c r="G29" s="31"/>
       <c r="H29" s="32"/>
       <c r="I29" s="32"/>
@@ -3420,26 +3431,24 @@
       <c r="AT29" s="33"/>
     </row>
     <row r="30" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="119" t="s">
+      <c r="A30" s="100" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="120"/>
-      <c r="C30" s="86">
+      <c r="B30" s="101"/>
+      <c r="C30" s="104">
         <v>2</v>
       </c>
-      <c r="D30" s="83"/>
-      <c r="E30" s="123">
+      <c r="D30" s="105"/>
+      <c r="E30" s="119">
         <v>2</v>
       </c>
-      <c r="F30" s="124"/>
+      <c r="F30" s="120"/>
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
       <c r="J30" s="35"/>
       <c r="K30" s="25"/>
-      <c r="N30" s="77" t="s">
-        <v>29</v>
-      </c>
+      <c r="N30" s="77"/>
       <c r="O30" s="25"/>
       <c r="P30" s="26"/>
       <c r="Q30" s="26"/>
@@ -3474,12 +3483,12 @@
       <c r="AT30" s="35"/>
     </row>
     <row r="31" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="121"/>
-      <c r="B31" s="122"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="85"/>
-      <c r="E31" s="125"/>
-      <c r="F31" s="126"/>
+      <c r="A31" s="102"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="107"/>
+      <c r="E31" s="121"/>
+      <c r="F31" s="122"/>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
@@ -3520,18 +3529,18 @@
       <c r="AT31" s="35"/>
     </row>
     <row r="32" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A32" s="119" t="s">
+      <c r="A32" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="120"/>
-      <c r="C32" s="86">
+      <c r="B32" s="101"/>
+      <c r="C32" s="104">
         <v>4</v>
       </c>
-      <c r="D32" s="83"/>
-      <c r="E32" s="86">
+      <c r="D32" s="105"/>
+      <c r="E32" s="104">
         <v>4</v>
       </c>
-      <c r="F32" s="83"/>
+      <c r="F32" s="105"/>
       <c r="G32" s="25"/>
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
@@ -3573,12 +3582,12 @@
       <c r="AT32" s="35"/>
     </row>
     <row r="33" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A33" s="121"/>
-      <c r="B33" s="122"/>
-      <c r="C33" s="87"/>
-      <c r="D33" s="85"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="85"/>
+      <c r="A33" s="102"/>
+      <c r="B33" s="103"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="107"/>
+      <c r="E33" s="106"/>
+      <c r="F33" s="107"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3620,18 +3629,18 @@
       <c r="AT33" s="35"/>
     </row>
     <row r="34" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="119" t="s">
+      <c r="A34" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="120"/>
-      <c r="C34" s="86">
+      <c r="B34" s="101"/>
+      <c r="C34" s="104">
         <v>2</v>
       </c>
-      <c r="D34" s="83"/>
-      <c r="E34" s="86">
+      <c r="D34" s="105"/>
+      <c r="E34" s="104">
         <v>2</v>
       </c>
-      <c r="F34" s="83"/>
+      <c r="F34" s="105"/>
       <c r="G34" s="25"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3673,12 +3682,12 @@
       <c r="AT34" s="35"/>
     </row>
     <row r="35" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="121"/>
-      <c r="B35" s="122"/>
-      <c r="C35" s="87"/>
-      <c r="D35" s="85"/>
-      <c r="E35" s="87"/>
-      <c r="F35" s="85"/>
+      <c r="A35" s="102"/>
+      <c r="B35" s="103"/>
+      <c r="C35" s="106"/>
+      <c r="D35" s="107"/>
+      <c r="E35" s="106"/>
+      <c r="F35" s="107"/>
       <c r="G35" s="25"/>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3720,18 +3729,18 @@
       <c r="AT35" s="35"/>
     </row>
     <row r="36" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="82" t="s">
+      <c r="A36" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="83"/>
-      <c r="C36" s="86">
+      <c r="B36" s="105"/>
+      <c r="C36" s="104">
         <v>2</v>
       </c>
-      <c r="D36" s="83"/>
-      <c r="E36" s="86">
+      <c r="D36" s="105"/>
+      <c r="E36" s="104">
         <v>2</v>
       </c>
-      <c r="F36" s="83"/>
+      <c r="F36" s="105"/>
       <c r="G36" s="25"/>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3771,12 +3780,12 @@
       <c r="AT36" s="35"/>
     </row>
     <row r="37" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A37" s="84"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="87"/>
-      <c r="D37" s="85"/>
-      <c r="E37" s="87"/>
-      <c r="F37" s="85"/>
+      <c r="A37" s="118"/>
+      <c r="B37" s="107"/>
+      <c r="C37" s="106"/>
+      <c r="D37" s="107"/>
+      <c r="E37" s="106"/>
+      <c r="F37" s="107"/>
       <c r="G37" s="25"/>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3817,18 +3826,18 @@
       <c r="AT37" s="35"/>
     </row>
     <row r="38" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="119" t="s">
+      <c r="A38" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="120"/>
-      <c r="C38" s="86">
+      <c r="B38" s="101"/>
+      <c r="C38" s="104">
         <v>2</v>
       </c>
-      <c r="D38" s="83"/>
-      <c r="E38" s="86">
+      <c r="D38" s="105"/>
+      <c r="E38" s="104">
         <v>2</v>
       </c>
-      <c r="F38" s="83"/>
+      <c r="F38" s="105"/>
       <c r="G38" s="25"/>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3870,12 +3879,12 @@
       <c r="AT38" s="35"/>
     </row>
     <row r="39" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="121"/>
-      <c r="B39" s="122"/>
-      <c r="C39" s="87"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="87"/>
-      <c r="F39" s="85"/>
+      <c r="A39" s="102"/>
+      <c r="B39" s="103"/>
+      <c r="C39" s="106"/>
+      <c r="D39" s="107"/>
+      <c r="E39" s="106"/>
+      <c r="F39" s="107"/>
       <c r="G39" s="25"/>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3917,20 +3926,20 @@
       <c r="AT39" s="35"/>
     </row>
     <row r="40" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="117" t="s">
+      <c r="A40" s="112" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="118"/>
-      <c r="C40" s="115">
+      <c r="B40" s="113"/>
+      <c r="C40" s="114">
         <f>SUM(C41:C43)</f>
         <v>3</v>
       </c>
-      <c r="D40" s="116"/>
-      <c r="E40" s="115">
+      <c r="D40" s="115"/>
+      <c r="E40" s="114">
         <f>SUM(E43+E41)</f>
         <v>3</v>
       </c>
-      <c r="F40" s="116"/>
+      <c r="F40" s="115"/>
       <c r="G40" s="31"/>
       <c r="H40" s="32"/>
       <c r="I40" s="32"/>
@@ -3973,18 +3982,18 @@
       <c r="AT40" s="33"/>
     </row>
     <row r="41" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="88" t="s">
+      <c r="A41" s="148" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="89"/>
-      <c r="C41" s="88">
+      <c r="B41" s="149"/>
+      <c r="C41" s="148">
         <v>2</v>
       </c>
-      <c r="D41" s="92"/>
-      <c r="E41" s="88">
+      <c r="D41" s="152"/>
+      <c r="E41" s="148">
         <v>2</v>
       </c>
-      <c r="F41" s="92"/>
+      <c r="F41" s="152"/>
       <c r="J41" s="54"/>
       <c r="N41" s="56"/>
       <c r="R41" s="63"/>
@@ -3999,12 +4008,12 @@
       <c r="AT41" s="56"/>
     </row>
     <row r="42" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="90"/>
-      <c r="B42" s="91"/>
-      <c r="C42" s="93"/>
-      <c r="D42" s="94"/>
-      <c r="E42" s="93"/>
-      <c r="F42" s="94"/>
+      <c r="A42" s="150"/>
+      <c r="B42" s="151"/>
+      <c r="C42" s="153"/>
+      <c r="D42" s="154"/>
+      <c r="E42" s="153"/>
+      <c r="F42" s="154"/>
       <c r="J42" s="55"/>
       <c r="N42" s="57"/>
       <c r="R42" s="63"/>
@@ -4018,18 +4027,18 @@
       <c r="AT42" s="57"/>
     </row>
     <row r="43" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A43" s="82" t="s">
+      <c r="A43" s="92" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="131"/>
-      <c r="C43" s="86">
+      <c r="B43" s="97"/>
+      <c r="C43" s="104">
         <v>1</v>
       </c>
-      <c r="D43" s="83"/>
-      <c r="E43" s="86">
+      <c r="D43" s="105"/>
+      <c r="E43" s="104">
         <v>1</v>
       </c>
-      <c r="F43" s="83"/>
+      <c r="F43" s="105"/>
       <c r="G43" s="25"/>
       <c r="H43" s="26"/>
       <c r="I43" s="26"/>
@@ -4072,12 +4081,12 @@
       <c r="AT43" s="35"/>
     </row>
     <row r="44" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="132"/>
-      <c r="B44" s="133"/>
-      <c r="C44" s="87"/>
-      <c r="D44" s="85"/>
-      <c r="E44" s="87"/>
-      <c r="F44" s="85"/>
+      <c r="A44" s="123"/>
+      <c r="B44" s="99"/>
+      <c r="C44" s="106"/>
+      <c r="D44" s="107"/>
+      <c r="E44" s="106"/>
+      <c r="F44" s="107"/>
       <c r="G44" s="25"/>
       <c r="H44" s="26"/>
       <c r="I44" s="26"/>
@@ -4120,20 +4129,20 @@
       <c r="AT44" s="35"/>
     </row>
     <row r="45" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="117" t="s">
+      <c r="A45" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="118"/>
-      <c r="C45" s="115">
+      <c r="B45" s="113"/>
+      <c r="C45" s="114">
         <f>SUM(C46:D61)</f>
         <v>19</v>
       </c>
-      <c r="D45" s="116"/>
-      <c r="E45" s="115">
+      <c r="D45" s="115"/>
+      <c r="E45" s="114">
         <f>SUM(E46:F61)</f>
         <v>19</v>
       </c>
-      <c r="F45" s="116"/>
+      <c r="F45" s="115"/>
       <c r="G45" s="31"/>
       <c r="H45" s="32"/>
       <c r="I45" s="32"/>
@@ -4176,18 +4185,18 @@
       <c r="AT45" s="33"/>
     </row>
     <row r="46" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="127" t="s">
+      <c r="A46" s="124" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="128"/>
-      <c r="C46" s="86">
+      <c r="B46" s="125"/>
+      <c r="C46" s="104">
         <v>0.5</v>
       </c>
-      <c r="D46" s="83"/>
-      <c r="E46" s="86">
+      <c r="D46" s="105"/>
+      <c r="E46" s="104">
         <v>0.5</v>
       </c>
-      <c r="F46" s="83"/>
+      <c r="F46" s="105"/>
       <c r="G46" s="25"/>
       <c r="H46" s="26"/>
       <c r="I46" s="26"/>
@@ -4227,12 +4236,12 @@
       <c r="AT46" s="35"/>
     </row>
     <row r="47" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A47" s="129"/>
-      <c r="B47" s="130"/>
-      <c r="C47" s="87"/>
-      <c r="D47" s="85"/>
-      <c r="E47" s="87"/>
-      <c r="F47" s="85"/>
+      <c r="A47" s="126"/>
+      <c r="B47" s="127"/>
+      <c r="C47" s="106"/>
+      <c r="D47" s="107"/>
+      <c r="E47" s="106"/>
+      <c r="F47" s="107"/>
       <c r="G47" s="25"/>
       <c r="H47" s="26"/>
       <c r="I47" s="26"/>
@@ -4274,18 +4283,18 @@
       <c r="AT47" s="35"/>
     </row>
     <row r="48" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="82" t="s">
+      <c r="A48" s="92" t="s">
         <v>75</v>
       </c>
-      <c r="B48" s="83"/>
-      <c r="C48" s="86">
+      <c r="B48" s="105"/>
+      <c r="C48" s="104">
         <v>0.5</v>
       </c>
-      <c r="D48" s="83"/>
-      <c r="E48" s="123">
+      <c r="D48" s="105"/>
+      <c r="E48" s="119">
         <v>0.5</v>
       </c>
-      <c r="F48" s="124"/>
+      <c r="F48" s="120"/>
       <c r="G48" s="25"/>
       <c r="H48" s="26"/>
       <c r="I48" s="26"/>
@@ -4325,12 +4334,12 @@
       <c r="AT48" s="35"/>
     </row>
     <row r="49" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="84"/>
-      <c r="B49" s="85"/>
-      <c r="C49" s="87"/>
-      <c r="D49" s="85"/>
-      <c r="E49" s="125"/>
-      <c r="F49" s="126"/>
+      <c r="A49" s="118"/>
+      <c r="B49" s="107"/>
+      <c r="C49" s="106"/>
+      <c r="D49" s="107"/>
+      <c r="E49" s="121"/>
+      <c r="F49" s="122"/>
       <c r="G49" s="25"/>
       <c r="H49" s="26"/>
       <c r="I49" s="26"/>
@@ -4372,18 +4381,18 @@
       <c r="AT49" s="35"/>
     </row>
     <row r="50" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A50" s="82" t="s">
+      <c r="A50" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="B50" s="83"/>
-      <c r="C50" s="86">
+      <c r="B50" s="105"/>
+      <c r="C50" s="104">
         <v>2</v>
       </c>
-      <c r="D50" s="83"/>
-      <c r="E50" s="123">
+      <c r="D50" s="105"/>
+      <c r="E50" s="119">
         <v>2</v>
       </c>
-      <c r="F50" s="124"/>
+      <c r="F50" s="120"/>
       <c r="G50" s="25"/>
       <c r="H50" s="26"/>
       <c r="I50" s="26"/>
@@ -4422,12 +4431,12 @@
       <c r="AT50" s="35"/>
     </row>
     <row r="51" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="84"/>
-      <c r="B51" s="85"/>
-      <c r="C51" s="87"/>
-      <c r="D51" s="85"/>
-      <c r="E51" s="125"/>
-      <c r="F51" s="126"/>
+      <c r="A51" s="118"/>
+      <c r="B51" s="107"/>
+      <c r="C51" s="106"/>
+      <c r="D51" s="107"/>
+      <c r="E51" s="121"/>
+      <c r="F51" s="122"/>
       <c r="G51" s="25"/>
       <c r="H51" s="26"/>
       <c r="I51" s="26"/>
@@ -4469,18 +4478,18 @@
       <c r="AT51" s="35"/>
     </row>
     <row r="52" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A52" s="82" t="s">
+      <c r="A52" s="92" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="83"/>
-      <c r="C52" s="86">
+      <c r="B52" s="105"/>
+      <c r="C52" s="104">
         <v>2</v>
       </c>
-      <c r="D52" s="83"/>
-      <c r="E52" s="123">
+      <c r="D52" s="105"/>
+      <c r="E52" s="119">
         <v>2</v>
       </c>
-      <c r="F52" s="124"/>
+      <c r="F52" s="120"/>
       <c r="G52" s="25"/>
       <c r="H52" s="26"/>
       <c r="I52" s="26"/>
@@ -4519,12 +4528,12 @@
       <c r="AT52" s="35"/>
     </row>
     <row r="53" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="84"/>
-      <c r="B53" s="85"/>
-      <c r="C53" s="87"/>
-      <c r="D53" s="85"/>
-      <c r="E53" s="125"/>
-      <c r="F53" s="126"/>
+      <c r="A53" s="118"/>
+      <c r="B53" s="107"/>
+      <c r="C53" s="106"/>
+      <c r="D53" s="107"/>
+      <c r="E53" s="121"/>
+      <c r="F53" s="122"/>
       <c r="G53" s="25"/>
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
@@ -4566,18 +4575,18 @@
       <c r="AT53" s="35"/>
     </row>
     <row r="54" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="119" t="s">
+      <c r="A54" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="B54" s="120"/>
-      <c r="C54" s="86">
+      <c r="B54" s="101"/>
+      <c r="C54" s="104">
         <v>2</v>
       </c>
-      <c r="D54" s="83"/>
-      <c r="E54" s="86">
+      <c r="D54" s="105"/>
+      <c r="E54" s="104">
         <v>2</v>
       </c>
-      <c r="F54" s="83"/>
+      <c r="F54" s="105"/>
       <c r="G54" s="25"/>
       <c r="H54" s="26"/>
       <c r="I54" s="26"/>
@@ -4616,12 +4625,12 @@
       <c r="AT54" s="35"/>
     </row>
     <row r="55" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="121"/>
-      <c r="B55" s="122"/>
-      <c r="C55" s="87"/>
-      <c r="D55" s="85"/>
-      <c r="E55" s="87"/>
-      <c r="F55" s="85"/>
+      <c r="A55" s="102"/>
+      <c r="B55" s="103"/>
+      <c r="C55" s="106"/>
+      <c r="D55" s="107"/>
+      <c r="E55" s="106"/>
+      <c r="F55" s="107"/>
       <c r="G55" s="25"/>
       <c r="H55" s="26"/>
       <c r="I55" s="26"/>
@@ -4662,18 +4671,18 @@
       <c r="AT55" s="35"/>
     </row>
     <row r="56" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="119" t="s">
+      <c r="A56" s="100" t="s">
         <v>79</v>
       </c>
-      <c r="B56" s="120"/>
-      <c r="C56" s="86">
+      <c r="B56" s="101"/>
+      <c r="C56" s="104">
         <v>2</v>
       </c>
-      <c r="D56" s="83"/>
-      <c r="E56" s="86">
+      <c r="D56" s="105"/>
+      <c r="E56" s="104">
         <v>2</v>
       </c>
-      <c r="F56" s="83"/>
+      <c r="F56" s="105"/>
       <c r="G56" s="25"/>
       <c r="H56" s="26"/>
       <c r="I56" s="26"/>
@@ -4714,12 +4723,12 @@
       <c r="AT56" s="35"/>
     </row>
     <row r="57" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A57" s="121"/>
-      <c r="B57" s="122"/>
-      <c r="C57" s="87"/>
-      <c r="D57" s="85"/>
-      <c r="E57" s="87"/>
-      <c r="F57" s="85"/>
+      <c r="A57" s="102"/>
+      <c r="B57" s="103"/>
+      <c r="C57" s="106"/>
+      <c r="D57" s="107"/>
+      <c r="E57" s="106"/>
+      <c r="F57" s="107"/>
       <c r="G57" s="25"/>
       <c r="H57" s="26"/>
       <c r="I57" s="26"/>
@@ -4760,18 +4769,18 @@
       <c r="AT57" s="35"/>
     </row>
     <row r="58" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A58" s="119" t="s">
+      <c r="A58" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="B58" s="120"/>
-      <c r="C58" s="86">
+      <c r="B58" s="101"/>
+      <c r="C58" s="104">
         <v>6</v>
       </c>
-      <c r="D58" s="83"/>
-      <c r="E58" s="86">
+      <c r="D58" s="105"/>
+      <c r="E58" s="104">
         <v>6</v>
       </c>
-      <c r="F58" s="83"/>
+      <c r="F58" s="105"/>
       <c r="G58" s="25"/>
       <c r="H58" s="26"/>
       <c r="I58" s="26"/>
@@ -4811,12 +4820,12 @@
       <c r="AT58" s="35"/>
     </row>
     <row r="59" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A59" s="121"/>
-      <c r="B59" s="122"/>
-      <c r="C59" s="87"/>
-      <c r="D59" s="85"/>
-      <c r="E59" s="87"/>
-      <c r="F59" s="85"/>
+      <c r="A59" s="102"/>
+      <c r="B59" s="103"/>
+      <c r="C59" s="106"/>
+      <c r="D59" s="107"/>
+      <c r="E59" s="106"/>
+      <c r="F59" s="107"/>
       <c r="G59" s="25"/>
       <c r="H59" s="26"/>
       <c r="I59" s="26"/>
@@ -4855,18 +4864,18 @@
       <c r="AT59" s="35"/>
     </row>
     <row r="60" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A60" s="119" t="s">
+      <c r="A60" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="B60" s="120"/>
-      <c r="C60" s="86">
+      <c r="B60" s="101"/>
+      <c r="C60" s="104">
         <v>4</v>
       </c>
-      <c r="D60" s="83"/>
-      <c r="E60" s="86">
+      <c r="D60" s="105"/>
+      <c r="E60" s="104">
         <v>4</v>
       </c>
-      <c r="F60" s="83"/>
+      <c r="F60" s="105"/>
       <c r="G60" s="25"/>
       <c r="H60" s="26"/>
       <c r="I60" s="26"/>
@@ -4906,12 +4915,12 @@
       <c r="AT60" s="35"/>
     </row>
     <row r="61" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A61" s="121"/>
-      <c r="B61" s="122"/>
-      <c r="C61" s="87"/>
-      <c r="D61" s="85"/>
-      <c r="E61" s="87"/>
-      <c r="F61" s="85"/>
+      <c r="A61" s="102"/>
+      <c r="B61" s="103"/>
+      <c r="C61" s="106"/>
+      <c r="D61" s="107"/>
+      <c r="E61" s="106"/>
+      <c r="F61" s="107"/>
       <c r="G61" s="25"/>
       <c r="H61" s="26"/>
       <c r="I61" s="26"/>
@@ -4952,20 +4961,20 @@
       <c r="AT61" s="35"/>
     </row>
     <row r="62" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="117" t="s">
+      <c r="A62" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="B62" s="118"/>
-      <c r="C62" s="115">
+      <c r="B62" s="113"/>
+      <c r="C62" s="114">
         <f>SUM(C63:D64)</f>
         <v>4</v>
       </c>
-      <c r="D62" s="116"/>
-      <c r="E62" s="115">
+      <c r="D62" s="115"/>
+      <c r="E62" s="114">
         <f>SUM(E63)</f>
         <v>4</v>
       </c>
-      <c r="F62" s="116"/>
+      <c r="F62" s="115"/>
       <c r="G62" s="31"/>
       <c r="H62" s="32"/>
       <c r="I62" s="32"/>
@@ -5008,18 +5017,18 @@
       <c r="AT62" s="33"/>
     </row>
     <row r="63" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A63" s="82" t="s">
+      <c r="A63" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="B63" s="83"/>
-      <c r="C63" s="86">
+      <c r="B63" s="105"/>
+      <c r="C63" s="104">
         <v>4</v>
       </c>
-      <c r="D63" s="83"/>
-      <c r="E63" s="86">
+      <c r="D63" s="105"/>
+      <c r="E63" s="104">
         <v>4</v>
       </c>
-      <c r="F63" s="83"/>
+      <c r="F63" s="105"/>
       <c r="G63" s="25"/>
       <c r="H63" s="26"/>
       <c r="I63" s="26"/>
@@ -5061,12 +5070,12 @@
       <c r="AT63" s="35"/>
     </row>
     <row r="64" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A64" s="84"/>
-      <c r="B64" s="85"/>
-      <c r="C64" s="87"/>
-      <c r="D64" s="85"/>
-      <c r="E64" s="87"/>
-      <c r="F64" s="85"/>
+      <c r="A64" s="118"/>
+      <c r="B64" s="107"/>
+      <c r="C64" s="106"/>
+      <c r="D64" s="107"/>
+      <c r="E64" s="106"/>
+      <c r="F64" s="107"/>
       <c r="G64" s="25"/>
       <c r="H64" s="26"/>
       <c r="I64" s="26"/>
@@ -5108,20 +5117,20 @@
       <c r="AT64" s="35"/>
     </row>
     <row r="65" spans="1:59" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="117" t="s">
+      <c r="A65" s="112" t="s">
         <v>42</v>
       </c>
-      <c r="B65" s="118"/>
-      <c r="C65" s="115">
+      <c r="B65" s="113"/>
+      <c r="C65" s="114">
         <f>SUM(C66:D67)</f>
         <v>4</v>
       </c>
-      <c r="D65" s="116"/>
-      <c r="E65" s="115">
+      <c r="D65" s="115"/>
+      <c r="E65" s="114">
         <f>SUM(E66)</f>
         <v>4</v>
       </c>
-      <c r="F65" s="116"/>
+      <c r="F65" s="115"/>
       <c r="G65" s="31"/>
       <c r="H65" s="32"/>
       <c r="I65" s="32"/>
@@ -5164,18 +5173,18 @@
       <c r="AT65" s="33"/>
     </row>
     <row r="66" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="82" t="s">
+      <c r="A66" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="B66" s="83"/>
-      <c r="C66" s="86">
+      <c r="B66" s="105"/>
+      <c r="C66" s="104">
         <v>4</v>
       </c>
-      <c r="D66" s="83"/>
-      <c r="E66" s="86">
+      <c r="D66" s="105"/>
+      <c r="E66" s="104">
         <v>4</v>
       </c>
-      <c r="F66" s="83"/>
+      <c r="F66" s="105"/>
       <c r="G66" s="25"/>
       <c r="H66" s="26"/>
       <c r="I66" s="26"/>
@@ -5218,12 +5227,12 @@
       <c r="AU66" s="38"/>
     </row>
     <row r="67" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A67" s="84"/>
-      <c r="B67" s="85"/>
-      <c r="C67" s="87"/>
-      <c r="D67" s="85"/>
-      <c r="E67" s="87"/>
-      <c r="F67" s="85"/>
+      <c r="A67" s="118"/>
+      <c r="B67" s="107"/>
+      <c r="C67" s="106"/>
+      <c r="D67" s="107"/>
+      <c r="E67" s="106"/>
+      <c r="F67" s="107"/>
       <c r="G67" s="25"/>
       <c r="H67" s="26"/>
       <c r="I67" s="26"/>
@@ -5265,20 +5274,20 @@
       <c r="AU67" s="39"/>
     </row>
     <row r="68" spans="1:59" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A68" s="111" t="s">
+      <c r="A68" s="144" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="112"/>
-      <c r="C68" s="113">
+      <c r="B68" s="145"/>
+      <c r="C68" s="146">
         <f>SUM(C69:D74)</f>
         <v>12</v>
       </c>
-      <c r="D68" s="114"/>
-      <c r="E68" s="115">
+      <c r="D68" s="147"/>
+      <c r="E68" s="114">
         <f>SUM(E69:F74)</f>
         <v>12</v>
       </c>
-      <c r="F68" s="116"/>
+      <c r="F68" s="115"/>
       <c r="G68" s="40"/>
       <c r="H68" s="41"/>
       <c r="I68" s="41"/>
@@ -5322,18 +5331,18 @@
       <c r="AU68" s="3"/>
     </row>
     <row r="69" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A69" s="82" t="s">
+      <c r="A69" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="B69" s="83"/>
-      <c r="C69" s="86">
+      <c r="B69" s="105"/>
+      <c r="C69" s="104">
         <v>6</v>
       </c>
-      <c r="D69" s="83"/>
-      <c r="E69" s="86">
+      <c r="D69" s="105"/>
+      <c r="E69" s="104">
         <v>6</v>
       </c>
-      <c r="F69" s="83"/>
+      <c r="F69" s="105"/>
       <c r="G69" s="25"/>
       <c r="H69" s="26"/>
       <c r="I69" s="26"/>
@@ -5373,12 +5382,12 @@
       <c r="AU69" s="3"/>
     </row>
     <row r="70" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A70" s="84"/>
-      <c r="B70" s="85"/>
-      <c r="C70" s="87"/>
-      <c r="D70" s="85"/>
-      <c r="E70" s="87"/>
-      <c r="F70" s="85"/>
+      <c r="A70" s="118"/>
+      <c r="B70" s="107"/>
+      <c r="C70" s="106"/>
+      <c r="D70" s="107"/>
+      <c r="E70" s="106"/>
+      <c r="F70" s="107"/>
       <c r="G70" s="25"/>
       <c r="H70" s="26"/>
       <c r="I70" s="26"/>
@@ -5431,18 +5440,18 @@
       <c r="BG70" s="38"/>
     </row>
     <row r="71" spans="1:59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="82" t="s">
+      <c r="A71" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="B71" s="83"/>
-      <c r="C71" s="86">
+      <c r="B71" s="105"/>
+      <c r="C71" s="104">
         <v>6</v>
       </c>
-      <c r="D71" s="83"/>
-      <c r="E71" s="86">
+      <c r="D71" s="105"/>
+      <c r="E71" s="104">
         <v>6</v>
       </c>
-      <c r="F71" s="83"/>
+      <c r="F71" s="105"/>
       <c r="G71" s="25"/>
       <c r="H71" s="26"/>
       <c r="I71" s="26"/>
@@ -5498,12 +5507,12 @@
       <c r="BG71" s="38"/>
     </row>
     <row r="72" spans="1:59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="84"/>
-      <c r="B72" s="85"/>
-      <c r="C72" s="87"/>
-      <c r="D72" s="85"/>
-      <c r="E72" s="87"/>
-      <c r="F72" s="85"/>
+      <c r="A72" s="118"/>
+      <c r="B72" s="107"/>
+      <c r="C72" s="106"/>
+      <c r="D72" s="107"/>
+      <c r="E72" s="106"/>
+      <c r="F72" s="107"/>
       <c r="G72" s="25"/>
       <c r="H72" s="26"/>
       <c r="I72" s="26"/>
@@ -5556,18 +5565,18 @@
       <c r="BG72" s="38"/>
     </row>
     <row r="73" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A73" s="82" t="s">
+      <c r="A73" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="B73" s="83"/>
-      <c r="C73" s="86">
+      <c r="B73" s="105"/>
+      <c r="C73" s="104">
         <v>0</v>
       </c>
-      <c r="D73" s="83"/>
-      <c r="E73" s="86">
+      <c r="D73" s="105"/>
+      <c r="E73" s="104">
         <v>0</v>
       </c>
-      <c r="F73" s="83"/>
+      <c r="F73" s="105"/>
       <c r="G73" s="25"/>
       <c r="H73" s="26"/>
       <c r="I73" s="26"/>
@@ -5619,12 +5628,12 @@
       <c r="BG73" s="39"/>
     </row>
     <row r="74" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A74" s="84"/>
-      <c r="B74" s="85"/>
-      <c r="C74" s="87"/>
-      <c r="D74" s="85"/>
-      <c r="E74" s="87"/>
-      <c r="F74" s="85"/>
+      <c r="A74" s="118"/>
+      <c r="B74" s="107"/>
+      <c r="C74" s="106"/>
+      <c r="D74" s="107"/>
+      <c r="E74" s="106"/>
+      <c r="F74" s="107"/>
       <c r="G74" s="25"/>
       <c r="H74" s="26"/>
       <c r="I74" s="26"/>
@@ -5738,20 +5747,20 @@
       <c r="BG75" s="3"/>
     </row>
     <row r="76" spans="1:59" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="105" t="s">
+      <c r="A76" s="138" t="s">
         <v>49</v>
       </c>
-      <c r="B76" s="106"/>
-      <c r="C76" s="107">
+      <c r="B76" s="139"/>
+      <c r="C76" s="140">
         <f>SUM(C14+C17+C29+C40+C45+C62+C65+C26 + C68)</f>
         <v>74</v>
       </c>
-      <c r="D76" s="108"/>
-      <c r="E76" s="109">
+      <c r="D76" s="141"/>
+      <c r="E76" s="142">
         <f>SUM(E14+E17+E29+E40+E45+E62+E65+E26+E68)</f>
         <v>74</v>
       </c>
-      <c r="F76" s="110"/>
+      <c r="F76" s="143"/>
       <c r="G76" s="39"/>
       <c r="H76" s="39"/>
       <c r="I76" s="39"/>
@@ -5869,6 +5878,108 @@
     </row>
   </sheetData>
   <mergeCells count="122">
+    <mergeCell ref="A58:B59"/>
+    <mergeCell ref="C58:D59"/>
+    <mergeCell ref="E58:F59"/>
+    <mergeCell ref="A60:B61"/>
+    <mergeCell ref="C60:D61"/>
+    <mergeCell ref="E60:F61"/>
+    <mergeCell ref="A54:B55"/>
+    <mergeCell ref="C54:D55"/>
+    <mergeCell ref="E54:F55"/>
+    <mergeCell ref="A56:B57"/>
+    <mergeCell ref="C56:D57"/>
+    <mergeCell ref="E56:F57"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="A66:B67"/>
+    <mergeCell ref="C66:D67"/>
+    <mergeCell ref="E66:F67"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="A63:B64"/>
+    <mergeCell ref="C63:D64"/>
+    <mergeCell ref="E63:F64"/>
+    <mergeCell ref="A73:B74"/>
+    <mergeCell ref="C73:D74"/>
+    <mergeCell ref="E73:F74"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="A69:B70"/>
+    <mergeCell ref="C69:D70"/>
+    <mergeCell ref="E69:F70"/>
+    <mergeCell ref="A71:B72"/>
+    <mergeCell ref="C71:D72"/>
+    <mergeCell ref="E71:F72"/>
+    <mergeCell ref="A50:B51"/>
+    <mergeCell ref="C50:D51"/>
+    <mergeCell ref="E50:F51"/>
+    <mergeCell ref="A52:B53"/>
+    <mergeCell ref="C52:D53"/>
+    <mergeCell ref="E52:F53"/>
+    <mergeCell ref="A46:B47"/>
+    <mergeCell ref="C46:D47"/>
+    <mergeCell ref="E46:F47"/>
+    <mergeCell ref="A48:B49"/>
+    <mergeCell ref="C48:D49"/>
+    <mergeCell ref="E48:F49"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="C43:D44"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="A38:B39"/>
+    <mergeCell ref="C38:D39"/>
+    <mergeCell ref="E38:F39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="A41:B42"/>
+    <mergeCell ref="C41:D42"/>
+    <mergeCell ref="E41:F42"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="E36:F37"/>
+    <mergeCell ref="A32:B33"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="E32:F33"/>
+    <mergeCell ref="A34:B35"/>
+    <mergeCell ref="C34:D35"/>
+    <mergeCell ref="E34:F35"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="E30:F31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:F28"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="E22:F23"/>
+    <mergeCell ref="A24:B25"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="E24:F25"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="E20:F21"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="AQ11:AT11"/>
     <mergeCell ref="A14:B14"/>
@@ -5886,111 +5997,9 @@
     <mergeCell ref="AE11:AH11"/>
     <mergeCell ref="AI11:AL11"/>
     <mergeCell ref="AM11:AP11"/>
-    <mergeCell ref="A22:B23"/>
-    <mergeCell ref="C22:D23"/>
-    <mergeCell ref="E22:F23"/>
-    <mergeCell ref="A24:B25"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="E24:F25"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="E30:F31"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:F28"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="E36:F37"/>
-    <mergeCell ref="A32:B33"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="E32:F33"/>
-    <mergeCell ref="A34:B35"/>
-    <mergeCell ref="C34:D35"/>
-    <mergeCell ref="E34:F35"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="C43:D44"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="A38:B39"/>
-    <mergeCell ref="C38:D39"/>
-    <mergeCell ref="E38:F39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="A50:B51"/>
-    <mergeCell ref="C50:D51"/>
-    <mergeCell ref="E50:F51"/>
-    <mergeCell ref="A52:B53"/>
-    <mergeCell ref="C52:D53"/>
-    <mergeCell ref="E52:F53"/>
-    <mergeCell ref="A46:B47"/>
-    <mergeCell ref="C46:D47"/>
-    <mergeCell ref="E46:F47"/>
-    <mergeCell ref="A48:B49"/>
-    <mergeCell ref="C48:D49"/>
-    <mergeCell ref="E48:F49"/>
     <mergeCell ref="E11:F13"/>
     <mergeCell ref="C11:D13"/>
     <mergeCell ref="A11:B13"/>
-    <mergeCell ref="A73:B74"/>
-    <mergeCell ref="C73:D74"/>
-    <mergeCell ref="E73:F74"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="A69:B70"/>
-    <mergeCell ref="C69:D70"/>
-    <mergeCell ref="E69:F70"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="A66:B67"/>
-    <mergeCell ref="C66:D67"/>
-    <mergeCell ref="E66:F67"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="A71:B72"/>
-    <mergeCell ref="C71:D72"/>
-    <mergeCell ref="E71:F72"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="E20:F21"/>
-    <mergeCell ref="A41:B42"/>
-    <mergeCell ref="C41:D42"/>
-    <mergeCell ref="E41:F42"/>
-    <mergeCell ref="A63:B64"/>
-    <mergeCell ref="C63:D64"/>
-    <mergeCell ref="E63:F64"/>
-    <mergeCell ref="A58:B59"/>
-    <mergeCell ref="C58:D59"/>
-    <mergeCell ref="E58:F59"/>
-    <mergeCell ref="A60:B61"/>
-    <mergeCell ref="C60:D61"/>
-    <mergeCell ref="E60:F61"/>
-    <mergeCell ref="A54:B55"/>
-    <mergeCell ref="C54:D55"/>
-    <mergeCell ref="E54:F55"/>
-    <mergeCell ref="A56:B57"/>
-    <mergeCell ref="C56:D57"/>
-    <mergeCell ref="E56:F57"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add laravel model to documentation
</commit_message>
<xml_diff>
--- a/documentation/Zeitplan.xlsx
+++ b/documentation/Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp8\htdocs\IPA\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE28CCFC-13FF-4C1E-A99E-6C515B650574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD03B229-E55D-475A-AE51-B604A2EB4A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1178,6 +1178,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="41" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1202,6 +1205,54 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1212,6 +1263,66 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1238,9 +1349,6 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1253,13 +1361,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1291,108 +1393,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1680,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AR75" sqref="AR75:AT75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,27 +1694,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:59" ht="44.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="139" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
-      <c r="Q1" s="102"/>
-      <c r="R1" s="102"/>
-      <c r="S1" s="102"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="139"/>
+      <c r="L1" s="139"/>
+      <c r="M1" s="139"/>
+      <c r="N1" s="139"/>
+      <c r="O1" s="139"/>
+      <c r="P1" s="139"/>
+      <c r="Q1" s="139"/>
+      <c r="R1" s="139"/>
+      <c r="S1" s="139"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
@@ -2346,86 +2346,86 @@
       <c r="BG10" s="3"/>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A11" s="123" t="s">
+      <c r="A11" s="157" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="124"/>
-      <c r="C11" s="118" t="s">
+      <c r="B11" s="158"/>
+      <c r="C11" s="152" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="119"/>
-      <c r="E11" s="118" t="s">
+      <c r="D11" s="153"/>
+      <c r="E11" s="152" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="119"/>
-      <c r="G11" s="103" t="s">
+      <c r="F11" s="153"/>
+      <c r="G11" s="140" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="104"/>
-      <c r="I11" s="104"/>
-      <c r="J11" s="105"/>
-      <c r="K11" s="103" t="s">
+      <c r="H11" s="141"/>
+      <c r="I11" s="141"/>
+      <c r="J11" s="142"/>
+      <c r="K11" s="140" t="s">
         <v>58</v>
       </c>
-      <c r="L11" s="104"/>
-      <c r="M11" s="104"/>
-      <c r="N11" s="105"/>
-      <c r="O11" s="103" t="s">
+      <c r="L11" s="141"/>
+      <c r="M11" s="141"/>
+      <c r="N11" s="142"/>
+      <c r="O11" s="140" t="s">
         <v>59</v>
       </c>
-      <c r="P11" s="104"/>
-      <c r="Q11" s="104"/>
-      <c r="R11" s="105"/>
-      <c r="S11" s="103" t="s">
+      <c r="P11" s="141"/>
+      <c r="Q11" s="141"/>
+      <c r="R11" s="142"/>
+      <c r="S11" s="140" t="s">
         <v>60</v>
       </c>
-      <c r="T11" s="104"/>
-      <c r="U11" s="104"/>
-      <c r="V11" s="105"/>
-      <c r="W11" s="103" t="s">
+      <c r="T11" s="141"/>
+      <c r="U11" s="141"/>
+      <c r="V11" s="142"/>
+      <c r="W11" s="140" t="s">
         <v>61</v>
       </c>
-      <c r="X11" s="104"/>
-      <c r="Y11" s="104"/>
-      <c r="Z11" s="105"/>
-      <c r="AA11" s="103" t="s">
+      <c r="X11" s="141"/>
+      <c r="Y11" s="141"/>
+      <c r="Z11" s="142"/>
+      <c r="AA11" s="140" t="s">
         <v>62</v>
       </c>
-      <c r="AB11" s="104"/>
-      <c r="AC11" s="104"/>
-      <c r="AD11" s="105"/>
-      <c r="AE11" s="103" t="s">
+      <c r="AB11" s="141"/>
+      <c r="AC11" s="141"/>
+      <c r="AD11" s="142"/>
+      <c r="AE11" s="140" t="s">
         <v>63</v>
       </c>
-      <c r="AF11" s="104"/>
-      <c r="AG11" s="104"/>
-      <c r="AH11" s="105"/>
-      <c r="AI11" s="103" t="s">
+      <c r="AF11" s="141"/>
+      <c r="AG11" s="141"/>
+      <c r="AH11" s="142"/>
+      <c r="AI11" s="140" t="s">
         <v>64</v>
       </c>
-      <c r="AJ11" s="104"/>
-      <c r="AK11" s="104"/>
-      <c r="AL11" s="105"/>
-      <c r="AM11" s="103" t="s">
+      <c r="AJ11" s="141"/>
+      <c r="AK11" s="141"/>
+      <c r="AL11" s="142"/>
+      <c r="AM11" s="140" t="s">
         <v>65</v>
       </c>
-      <c r="AN11" s="104"/>
-      <c r="AO11" s="104"/>
-      <c r="AP11" s="105"/>
-      <c r="AQ11" s="103" t="s">
+      <c r="AN11" s="141"/>
+      <c r="AO11" s="141"/>
+      <c r="AP11" s="142"/>
+      <c r="AQ11" s="140" t="s">
         <v>66</v>
       </c>
-      <c r="AR11" s="104"/>
-      <c r="AS11" s="104"/>
-      <c r="AT11" s="105"/>
+      <c r="AR11" s="141"/>
+      <c r="AS11" s="141"/>
+      <c r="AT11" s="142"/>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A12" s="125"/>
-      <c r="B12" s="124"/>
-      <c r="C12" s="120"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="119"/>
+      <c r="A12" s="159"/>
+      <c r="B12" s="158"/>
+      <c r="C12" s="154"/>
+      <c r="D12" s="153"/>
+      <c r="E12" s="154"/>
+      <c r="F12" s="153"/>
       <c r="G12" s="10">
         <v>1</v>
       </c>
@@ -2548,12 +2548,12 @@
       </c>
     </row>
     <row r="13" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="126"/>
-      <c r="B13" s="127"/>
-      <c r="C13" s="121"/>
-      <c r="D13" s="122"/>
-      <c r="E13" s="121"/>
-      <c r="F13" s="122"/>
+      <c r="A13" s="160"/>
+      <c r="B13" s="161"/>
+      <c r="C13" s="155"/>
+      <c r="D13" s="156"/>
+      <c r="E13" s="155"/>
+      <c r="F13" s="156"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
@@ -2596,20 +2596,20 @@
       <c r="AT13" s="16"/>
     </row>
     <row r="14" spans="1:59" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="106" t="s">
+      <c r="A14" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="107"/>
-      <c r="C14" s="108">
+      <c r="B14" s="144"/>
+      <c r="C14" s="145">
         <f>SUM(C15:D16)</f>
         <v>6</v>
       </c>
-      <c r="D14" s="109"/>
-      <c r="E14" s="108">
+      <c r="D14" s="146"/>
+      <c r="E14" s="145">
         <f>SUM(E15)</f>
         <v>6</v>
       </c>
-      <c r="F14" s="109"/>
+      <c r="F14" s="146"/>
       <c r="G14" s="18"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
@@ -2661,18 +2661,18 @@
       <c r="BC14" s="24"/>
     </row>
     <row r="15" spans="1:59" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="111"/>
-      <c r="C15" s="114">
+      <c r="B15" s="147"/>
+      <c r="C15" s="150">
         <v>6</v>
       </c>
-      <c r="D15" s="115"/>
-      <c r="E15" s="114">
+      <c r="D15" s="123"/>
+      <c r="E15" s="150">
         <v>6</v>
       </c>
-      <c r="F15" s="115"/>
+      <c r="F15" s="123"/>
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
       <c r="I15" s="26"/>
@@ -2720,12 +2720,12 @@
       <c r="BC15" s="29"/>
     </row>
     <row r="16" spans="1:59" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="112"/>
-      <c r="B16" s="113"/>
-      <c r="C16" s="116"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="117"/>
+      <c r="A16" s="148"/>
+      <c r="B16" s="149"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="125"/>
       <c r="G16" s="30"/>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
@@ -2766,20 +2766,20 @@
       <c r="BC16" s="29"/>
     </row>
     <row r="17" spans="1:55" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="132" t="s">
+      <c r="A17" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="133"/>
-      <c r="C17" s="134">
+      <c r="B17" s="100"/>
+      <c r="C17" s="101">
         <f>SUM(C18:D25)</f>
         <v>12</v>
       </c>
-      <c r="D17" s="135"/>
-      <c r="E17" s="136">
+      <c r="D17" s="102"/>
+      <c r="E17" s="133">
         <f>SUM(E18:F25)</f>
         <v>12</v>
       </c>
-      <c r="F17" s="137"/>
+      <c r="F17" s="134"/>
       <c r="G17" s="31"/>
       <c r="H17" s="32"/>
       <c r="I17" s="32"/>
@@ -2829,18 +2829,18 @@
       <c r="BC17" s="29"/>
     </row>
     <row r="18" spans="1:55" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="110" t="s">
+      <c r="A18" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="95"/>
-      <c r="C18" s="94">
+      <c r="B18" s="96"/>
+      <c r="C18" s="95">
         <v>6</v>
       </c>
-      <c r="D18" s="95"/>
-      <c r="E18" s="94">
+      <c r="D18" s="96"/>
+      <c r="E18" s="95">
         <v>6</v>
       </c>
-      <c r="F18" s="95"/>
+      <c r="F18" s="96"/>
       <c r="G18" s="52"/>
       <c r="H18" s="53"/>
       <c r="I18" s="53"/>
@@ -2890,12 +2890,12 @@
       <c r="BC18" s="29"/>
     </row>
     <row r="19" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="138"/>
-      <c r="B19" s="97"/>
-      <c r="C19" s="96"/>
-      <c r="D19" s="97"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="97"/>
+      <c r="A19" s="104"/>
+      <c r="B19" s="98"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="97"/>
+      <c r="F19" s="98"/>
       <c r="G19" s="51"/>
       <c r="H19" s="59"/>
       <c r="I19" s="59"/>
@@ -2940,18 +2940,18 @@
       <c r="BC19" s="29"/>
     </row>
     <row r="20" spans="1:55" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="110" t="s">
+      <c r="A20" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="95"/>
-      <c r="C20" s="94">
+      <c r="B20" s="96"/>
+      <c r="C20" s="95">
         <v>2</v>
       </c>
-      <c r="D20" s="95"/>
-      <c r="E20" s="94">
+      <c r="D20" s="96"/>
+      <c r="E20" s="95">
         <v>2</v>
       </c>
-      <c r="F20" s="95"/>
+      <c r="F20" s="96"/>
       <c r="J20" s="50"/>
       <c r="K20" s="25"/>
       <c r="L20" s="26"/>
@@ -3000,12 +3000,12 @@
       <c r="BC20" s="37"/>
     </row>
     <row r="21" spans="1:55" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="138"/>
-      <c r="B21" s="97"/>
-      <c r="C21" s="96"/>
-      <c r="D21" s="97"/>
-      <c r="E21" s="96"/>
-      <c r="F21" s="97"/>
+      <c r="A21" s="104"/>
+      <c r="B21" s="98"/>
+      <c r="C21" s="97"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="97"/>
+      <c r="F21" s="98"/>
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
       <c r="J21" s="82"/>
@@ -3047,18 +3047,18 @@
       <c r="AT21" s="35"/>
     </row>
     <row r="22" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="90" t="s">
+      <c r="A22" s="91" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="91"/>
-      <c r="C22" s="94">
+      <c r="B22" s="92"/>
+      <c r="C22" s="95">
         <v>2</v>
       </c>
-      <c r="D22" s="95"/>
-      <c r="E22" s="94">
+      <c r="D22" s="96"/>
+      <c r="E22" s="95">
         <v>2</v>
       </c>
-      <c r="F22" s="95"/>
+      <c r="F22" s="96"/>
       <c r="G22" s="25"/>
       <c r="J22" s="56"/>
       <c r="K22" s="61"/>
@@ -3098,12 +3098,12 @@
       <c r="AT22" s="35"/>
     </row>
     <row r="23" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="92"/>
-      <c r="B23" s="93"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="97"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="97"/>
+      <c r="A23" s="93"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="98"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="98"/>
       <c r="G23" s="25"/>
       <c r="J23" s="83"/>
       <c r="K23" s="27"/>
@@ -3144,18 +3144,18 @@
       <c r="AT23" s="35"/>
     </row>
     <row r="24" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="90" t="s">
+      <c r="A24" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="91"/>
-      <c r="C24" s="94">
+      <c r="B24" s="92"/>
+      <c r="C24" s="95">
         <v>2</v>
       </c>
-      <c r="D24" s="95"/>
-      <c r="E24" s="128">
+      <c r="D24" s="96"/>
+      <c r="E24" s="135">
         <v>2</v>
       </c>
-      <c r="F24" s="129"/>
+      <c r="F24" s="136"/>
       <c r="G24" s="25"/>
       <c r="I24" s="26"/>
       <c r="J24" s="67"/>
@@ -3199,12 +3199,12 @@
       <c r="AT24" s="35"/>
     </row>
     <row r="25" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="92"/>
-      <c r="B25" s="93"/>
-      <c r="C25" s="96"/>
-      <c r="D25" s="97"/>
-      <c r="E25" s="130"/>
-      <c r="F25" s="131"/>
+      <c r="A25" s="93"/>
+      <c r="B25" s="94"/>
+      <c r="C25" s="97"/>
+      <c r="D25" s="98"/>
+      <c r="E25" s="137"/>
+      <c r="F25" s="138"/>
       <c r="G25" s="25"/>
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
@@ -3248,20 +3248,20 @@
       <c r="AT25" s="35"/>
     </row>
     <row r="26" spans="1:55" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="132" t="s">
+      <c r="A26" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="133"/>
-      <c r="C26" s="134">
+      <c r="B26" s="100"/>
+      <c r="C26" s="101">
         <f>SUM(C27)</f>
         <v>2</v>
       </c>
-      <c r="D26" s="135"/>
-      <c r="E26" s="136">
+      <c r="D26" s="102"/>
+      <c r="E26" s="133">
         <f>SUM(E27)</f>
         <v>2</v>
       </c>
-      <c r="F26" s="137"/>
+      <c r="F26" s="134"/>
       <c r="G26" s="31"/>
       <c r="H26" s="32"/>
       <c r="I26" s="32"/>
@@ -3304,18 +3304,18 @@
       <c r="AT26" s="33"/>
     </row>
     <row r="27" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="110" t="s">
+      <c r="A27" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="95"/>
-      <c r="C27" s="94">
+      <c r="B27" s="96"/>
+      <c r="C27" s="95">
         <v>2</v>
       </c>
-      <c r="D27" s="95"/>
-      <c r="E27" s="94">
+      <c r="D27" s="96"/>
+      <c r="E27" s="95">
         <v>2</v>
       </c>
-      <c r="F27" s="95"/>
+      <c r="F27" s="96"/>
       <c r="G27" s="25"/>
       <c r="H27" s="26"/>
       <c r="I27" s="26"/>
@@ -3357,12 +3357,12 @@
       <c r="AT27" s="35"/>
     </row>
     <row r="28" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="138"/>
-      <c r="B28" s="97"/>
-      <c r="C28" s="96"/>
-      <c r="D28" s="97"/>
-      <c r="E28" s="96"/>
-      <c r="F28" s="97"/>
+      <c r="A28" s="104"/>
+      <c r="B28" s="98"/>
+      <c r="C28" s="97"/>
+      <c r="D28" s="98"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="98"/>
       <c r="G28" s="25"/>
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
@@ -3406,20 +3406,20 @@
       <c r="AT28" s="35"/>
     </row>
     <row r="29" spans="1:55" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="132" t="s">
+      <c r="A29" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="133"/>
-      <c r="C29" s="134">
+      <c r="B29" s="100"/>
+      <c r="C29" s="101">
         <f>SUM(C30:D41)</f>
         <v>12</v>
       </c>
-      <c r="D29" s="135"/>
-      <c r="E29" s="134">
+      <c r="D29" s="102"/>
+      <c r="E29" s="101">
         <f>SUM(E30:F41)</f>
         <v>12</v>
       </c>
-      <c r="F29" s="135"/>
+      <c r="F29" s="102"/>
       <c r="G29" s="31"/>
       <c r="H29" s="32"/>
       <c r="I29" s="32"/>
@@ -3462,18 +3462,18 @@
       <c r="AT29" s="33"/>
     </row>
     <row r="30" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="90" t="s">
+      <c r="A30" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="91"/>
-      <c r="C30" s="94">
+      <c r="B30" s="92"/>
+      <c r="C30" s="95">
         <v>2</v>
       </c>
-      <c r="D30" s="95"/>
-      <c r="E30" s="98">
+      <c r="D30" s="96"/>
+      <c r="E30" s="115">
         <v>2</v>
       </c>
-      <c r="F30" s="99"/>
+      <c r="F30" s="116"/>
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
@@ -3514,12 +3514,12 @@
       <c r="AT30" s="35"/>
     </row>
     <row r="31" spans="1:55" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="92"/>
-      <c r="B31" s="93"/>
-      <c r="C31" s="96"/>
-      <c r="D31" s="97"/>
-      <c r="E31" s="100"/>
-      <c r="F31" s="101"/>
+      <c r="A31" s="93"/>
+      <c r="B31" s="94"/>
+      <c r="C31" s="97"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="117"/>
+      <c r="F31" s="118"/>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
@@ -3561,18 +3561,18 @@
       <c r="AT31" s="35"/>
     </row>
     <row r="32" spans="1:55" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="90" t="s">
+      <c r="A32" s="91" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="91"/>
-      <c r="C32" s="94">
+      <c r="B32" s="92"/>
+      <c r="C32" s="95">
         <v>2</v>
       </c>
-      <c r="D32" s="95"/>
-      <c r="E32" s="98">
+      <c r="D32" s="96"/>
+      <c r="E32" s="115">
         <v>2</v>
       </c>
-      <c r="F32" s="99"/>
+      <c r="F32" s="116"/>
       <c r="G32" s="25"/>
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
@@ -3613,12 +3613,12 @@
       <c r="AT32" s="35"/>
     </row>
     <row r="33" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="92"/>
-      <c r="B33" s="93"/>
-      <c r="C33" s="96"/>
-      <c r="D33" s="97"/>
-      <c r="E33" s="100"/>
-      <c r="F33" s="101"/>
+      <c r="A33" s="93"/>
+      <c r="B33" s="94"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="98"/>
+      <c r="E33" s="117"/>
+      <c r="F33" s="118"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3659,18 +3659,18 @@
       <c r="AT33" s="35"/>
     </row>
     <row r="34" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="90" t="s">
+      <c r="A34" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="91"/>
-      <c r="C34" s="94">
+      <c r="B34" s="92"/>
+      <c r="C34" s="95">
         <v>2</v>
       </c>
-      <c r="D34" s="95"/>
-      <c r="E34" s="94">
+      <c r="D34" s="96"/>
+      <c r="E34" s="95">
         <v>2</v>
       </c>
-      <c r="F34" s="95"/>
+      <c r="F34" s="96"/>
       <c r="G34" s="25"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3711,12 +3711,12 @@
       <c r="AT34" s="35"/>
     </row>
     <row r="35" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="92"/>
-      <c r="B35" s="93"/>
-      <c r="C35" s="96"/>
-      <c r="D35" s="97"/>
-      <c r="E35" s="96"/>
-      <c r="F35" s="97"/>
+      <c r="A35" s="93"/>
+      <c r="B35" s="94"/>
+      <c r="C35" s="97"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="97"/>
+      <c r="F35" s="98"/>
       <c r="G35" s="25"/>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3724,7 +3724,7 @@
       <c r="K35" s="25"/>
       <c r="L35" s="26"/>
       <c r="N35" s="67"/>
-      <c r="O35" s="161"/>
+      <c r="O35" s="90"/>
       <c r="P35" s="26"/>
       <c r="Q35" s="26"/>
       <c r="R35" s="64"/>
@@ -3758,18 +3758,18 @@
       <c r="AT35" s="35"/>
     </row>
     <row r="36" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="90" t="s">
+      <c r="A36" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="91"/>
-      <c r="C36" s="94">
+      <c r="B36" s="92"/>
+      <c r="C36" s="95">
         <v>2</v>
       </c>
-      <c r="D36" s="95"/>
-      <c r="E36" s="94">
+      <c r="D36" s="96"/>
+      <c r="E36" s="95">
         <v>2</v>
       </c>
-      <c r="F36" s="95"/>
+      <c r="F36" s="96"/>
       <c r="G36" s="25"/>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3811,12 +3811,12 @@
       <c r="AT36" s="35"/>
     </row>
     <row r="37" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A37" s="92"/>
-      <c r="B37" s="93"/>
-      <c r="C37" s="96"/>
-      <c r="D37" s="97"/>
-      <c r="E37" s="96"/>
-      <c r="F37" s="97"/>
+      <c r="A37" s="93"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="97"/>
+      <c r="D37" s="98"/>
+      <c r="E37" s="97"/>
+      <c r="F37" s="98"/>
       <c r="G37" s="25"/>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3858,18 +3858,18 @@
       <c r="AT37" s="35"/>
     </row>
     <row r="38" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="110" t="s">
+      <c r="A38" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="95"/>
-      <c r="C38" s="94">
+      <c r="B38" s="96"/>
+      <c r="C38" s="95">
         <v>2</v>
       </c>
-      <c r="D38" s="95"/>
-      <c r="E38" s="94">
+      <c r="D38" s="96"/>
+      <c r="E38" s="95">
         <v>2</v>
       </c>
-      <c r="F38" s="95"/>
+      <c r="F38" s="96"/>
       <c r="G38" s="25"/>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3909,12 +3909,12 @@
       <c r="AT38" s="35"/>
     </row>
     <row r="39" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="138"/>
-      <c r="B39" s="97"/>
-      <c r="C39" s="96"/>
-      <c r="D39" s="97"/>
-      <c r="E39" s="96"/>
-      <c r="F39" s="97"/>
+      <c r="A39" s="104"/>
+      <c r="B39" s="98"/>
+      <c r="C39" s="97"/>
+      <c r="D39" s="98"/>
+      <c r="E39" s="97"/>
+      <c r="F39" s="98"/>
       <c r="G39" s="25"/>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3955,18 +3955,18 @@
       <c r="AT39" s="35"/>
     </row>
     <row r="40" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A40" s="90" t="s">
+      <c r="A40" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="91"/>
-      <c r="C40" s="94">
+      <c r="B40" s="92"/>
+      <c r="C40" s="95">
         <v>2</v>
       </c>
-      <c r="D40" s="95"/>
-      <c r="E40" s="94">
+      <c r="D40" s="96"/>
+      <c r="E40" s="95">
         <v>2</v>
       </c>
-      <c r="F40" s="95"/>
+      <c r="F40" s="96"/>
       <c r="G40" s="25"/>
       <c r="H40" s="26"/>
       <c r="I40" s="26"/>
@@ -4008,12 +4008,12 @@
       <c r="AT40" s="35"/>
     </row>
     <row r="41" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="92"/>
-      <c r="B41" s="93"/>
-      <c r="C41" s="96"/>
-      <c r="D41" s="97"/>
-      <c r="E41" s="96"/>
-      <c r="F41" s="97"/>
+      <c r="A41" s="93"/>
+      <c r="B41" s="94"/>
+      <c r="C41" s="97"/>
+      <c r="D41" s="98"/>
+      <c r="E41" s="97"/>
+      <c r="F41" s="98"/>
       <c r="G41" s="25"/>
       <c r="H41" s="26"/>
       <c r="I41" s="26"/>
@@ -4055,20 +4055,20 @@
       <c r="AT41" s="35"/>
     </row>
     <row r="42" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="132" t="s">
+      <c r="A42" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="133"/>
-      <c r="C42" s="134">
+      <c r="B42" s="100"/>
+      <c r="C42" s="101">
         <f>SUM(C43:C45)</f>
         <v>3</v>
       </c>
-      <c r="D42" s="135"/>
-      <c r="E42" s="134">
+      <c r="D42" s="102"/>
+      <c r="E42" s="101">
         <f>SUM(E45+E43)</f>
         <v>3</v>
       </c>
-      <c r="F42" s="135"/>
+      <c r="F42" s="102"/>
       <c r="G42" s="31"/>
       <c r="H42" s="32"/>
       <c r="I42" s="32"/>
@@ -4111,18 +4111,18 @@
       <c r="AT42" s="33"/>
     </row>
     <row r="43" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="140" t="s">
+      <c r="A43" s="126" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="141"/>
-      <c r="C43" s="140">
+      <c r="B43" s="127"/>
+      <c r="C43" s="126">
         <v>2</v>
       </c>
-      <c r="D43" s="144"/>
-      <c r="E43" s="140">
+      <c r="D43" s="130"/>
+      <c r="E43" s="126">
         <v>2</v>
       </c>
-      <c r="F43" s="144"/>
+      <c r="F43" s="130"/>
       <c r="J43" s="54"/>
       <c r="N43" s="56"/>
       <c r="R43" s="63"/>
@@ -4137,12 +4137,12 @@
       <c r="AT43" s="56"/>
     </row>
     <row r="44" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="142"/>
-      <c r="B44" s="143"/>
-      <c r="C44" s="145"/>
-      <c r="D44" s="146"/>
-      <c r="E44" s="145"/>
-      <c r="F44" s="146"/>
+      <c r="A44" s="128"/>
+      <c r="B44" s="129"/>
+      <c r="C44" s="131"/>
+      <c r="D44" s="132"/>
+      <c r="E44" s="131"/>
+      <c r="F44" s="132"/>
       <c r="J44" s="55"/>
       <c r="N44" s="57"/>
       <c r="R44" s="63"/>
@@ -4156,18 +4156,18 @@
       <c r="AT44" s="57"/>
     </row>
     <row r="45" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="110" t="s">
+      <c r="A45" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="B45" s="115"/>
-      <c r="C45" s="94">
+      <c r="B45" s="123"/>
+      <c r="C45" s="95">
         <v>1</v>
       </c>
-      <c r="D45" s="95"/>
-      <c r="E45" s="94">
+      <c r="D45" s="96"/>
+      <c r="E45" s="95">
         <v>1</v>
       </c>
-      <c r="F45" s="95"/>
+      <c r="F45" s="96"/>
       <c r="G45" s="25"/>
       <c r="H45" s="26"/>
       <c r="I45" s="26"/>
@@ -4210,12 +4210,12 @@
       <c r="AT45" s="35"/>
     </row>
     <row r="46" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="139"/>
-      <c r="B46" s="117"/>
-      <c r="C46" s="96"/>
-      <c r="D46" s="97"/>
-      <c r="E46" s="96"/>
-      <c r="F46" s="97"/>
+      <c r="A46" s="124"/>
+      <c r="B46" s="125"/>
+      <c r="C46" s="97"/>
+      <c r="D46" s="98"/>
+      <c r="E46" s="97"/>
+      <c r="F46" s="98"/>
       <c r="G46" s="25"/>
       <c r="H46" s="26"/>
       <c r="I46" s="26"/>
@@ -4258,20 +4258,20 @@
       <c r="AT46" s="35"/>
     </row>
     <row r="47" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="132" t="s">
+      <c r="A47" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="133"/>
-      <c r="C47" s="134">
+      <c r="B47" s="100"/>
+      <c r="C47" s="101">
         <f>SUM(C48:D63)</f>
         <v>19</v>
       </c>
-      <c r="D47" s="135"/>
-      <c r="E47" s="134">
+      <c r="D47" s="102"/>
+      <c r="E47" s="101">
         <f>SUM(E48:F63)</f>
         <v>19</v>
       </c>
-      <c r="F47" s="135"/>
+      <c r="F47" s="102"/>
       <c r="G47" s="31"/>
       <c r="H47" s="32"/>
       <c r="I47" s="32"/>
@@ -4314,18 +4314,18 @@
       <c r="AT47" s="33"/>
     </row>
     <row r="48" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="147" t="s">
+      <c r="A48" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="B48" s="148"/>
-      <c r="C48" s="94">
+      <c r="B48" s="120"/>
+      <c r="C48" s="95">
         <v>0.5</v>
       </c>
-      <c r="D48" s="95"/>
-      <c r="E48" s="94">
+      <c r="D48" s="96"/>
+      <c r="E48" s="95">
         <v>0.5</v>
       </c>
-      <c r="F48" s="95"/>
+      <c r="F48" s="96"/>
       <c r="G48" s="25"/>
       <c r="H48" s="26"/>
       <c r="I48" s="26"/>
@@ -4365,12 +4365,12 @@
       <c r="AT48" s="35"/>
     </row>
     <row r="49" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="149"/>
-      <c r="B49" s="150"/>
-      <c r="C49" s="96"/>
-      <c r="D49" s="97"/>
-      <c r="E49" s="96"/>
-      <c r="F49" s="97"/>
+      <c r="A49" s="121"/>
+      <c r="B49" s="122"/>
+      <c r="C49" s="97"/>
+      <c r="D49" s="98"/>
+      <c r="E49" s="97"/>
+      <c r="F49" s="98"/>
       <c r="G49" s="25"/>
       <c r="H49" s="26"/>
       <c r="I49" s="26"/>
@@ -4412,18 +4412,18 @@
       <c r="AT49" s="35"/>
     </row>
     <row r="50" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A50" s="110" t="s">
+      <c r="A50" s="103" t="s">
         <v>75</v>
       </c>
-      <c r="B50" s="95"/>
-      <c r="C50" s="94">
+      <c r="B50" s="96"/>
+      <c r="C50" s="95">
         <v>0.5</v>
       </c>
-      <c r="D50" s="95"/>
-      <c r="E50" s="98">
+      <c r="D50" s="96"/>
+      <c r="E50" s="115">
         <v>0.5</v>
       </c>
-      <c r="F50" s="99"/>
+      <c r="F50" s="116"/>
       <c r="G50" s="25"/>
       <c r="H50" s="26"/>
       <c r="I50" s="26"/>
@@ -4463,12 +4463,12 @@
       <c r="AT50" s="35"/>
     </row>
     <row r="51" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="138"/>
-      <c r="B51" s="97"/>
-      <c r="C51" s="96"/>
-      <c r="D51" s="97"/>
-      <c r="E51" s="100"/>
-      <c r="F51" s="101"/>
+      <c r="A51" s="104"/>
+      <c r="B51" s="98"/>
+      <c r="C51" s="97"/>
+      <c r="D51" s="98"/>
+      <c r="E51" s="117"/>
+      <c r="F51" s="118"/>
       <c r="G51" s="25"/>
       <c r="H51" s="26"/>
       <c r="I51" s="26"/>
@@ -4510,18 +4510,18 @@
       <c r="AT51" s="35"/>
     </row>
     <row r="52" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A52" s="110" t="s">
+      <c r="A52" s="103" t="s">
         <v>76</v>
       </c>
-      <c r="B52" s="95"/>
-      <c r="C52" s="94">
+      <c r="B52" s="96"/>
+      <c r="C52" s="95">
         <v>2</v>
       </c>
-      <c r="D52" s="95"/>
-      <c r="E52" s="98">
+      <c r="D52" s="96"/>
+      <c r="E52" s="115">
         <v>2</v>
       </c>
-      <c r="F52" s="99"/>
+      <c r="F52" s="116"/>
       <c r="G52" s="25"/>
       <c r="H52" s="26"/>
       <c r="I52" s="26"/>
@@ -4560,12 +4560,12 @@
       <c r="AT52" s="35"/>
     </row>
     <row r="53" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="138"/>
-      <c r="B53" s="97"/>
-      <c r="C53" s="96"/>
-      <c r="D53" s="97"/>
-      <c r="E53" s="100"/>
-      <c r="F53" s="101"/>
+      <c r="A53" s="104"/>
+      <c r="B53" s="98"/>
+      <c r="C53" s="97"/>
+      <c r="D53" s="98"/>
+      <c r="E53" s="117"/>
+      <c r="F53" s="118"/>
       <c r="G53" s="25"/>
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
@@ -4607,18 +4607,18 @@
       <c r="AT53" s="35"/>
     </row>
     <row r="54" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="110" t="s">
+      <c r="A54" s="103" t="s">
         <v>78</v>
       </c>
-      <c r="B54" s="95"/>
-      <c r="C54" s="94">
+      <c r="B54" s="96"/>
+      <c r="C54" s="95">
         <v>2</v>
       </c>
-      <c r="D54" s="95"/>
-      <c r="E54" s="98">
+      <c r="D54" s="96"/>
+      <c r="E54" s="115">
         <v>2</v>
       </c>
-      <c r="F54" s="99"/>
+      <c r="F54" s="116"/>
       <c r="G54" s="25"/>
       <c r="H54" s="26"/>
       <c r="I54" s="26"/>
@@ -4657,12 +4657,12 @@
       <c r="AT54" s="35"/>
     </row>
     <row r="55" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="138"/>
-      <c r="B55" s="97"/>
-      <c r="C55" s="96"/>
-      <c r="D55" s="97"/>
-      <c r="E55" s="100"/>
-      <c r="F55" s="101"/>
+      <c r="A55" s="104"/>
+      <c r="B55" s="98"/>
+      <c r="C55" s="97"/>
+      <c r="D55" s="98"/>
+      <c r="E55" s="117"/>
+      <c r="F55" s="118"/>
       <c r="G55" s="25"/>
       <c r="H55" s="26"/>
       <c r="I55" s="26"/>
@@ -4704,18 +4704,18 @@
       <c r="AT55" s="35"/>
     </row>
     <row r="56" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="90" t="s">
+      <c r="A56" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="B56" s="91"/>
-      <c r="C56" s="94">
+      <c r="B56" s="92"/>
+      <c r="C56" s="95">
         <v>2</v>
       </c>
-      <c r="D56" s="95"/>
-      <c r="E56" s="94">
+      <c r="D56" s="96"/>
+      <c r="E56" s="95">
         <v>2</v>
       </c>
-      <c r="F56" s="95"/>
+      <c r="F56" s="96"/>
       <c r="G56" s="25"/>
       <c r="H56" s="26"/>
       <c r="I56" s="26"/>
@@ -4754,12 +4754,12 @@
       <c r="AT56" s="35"/>
     </row>
     <row r="57" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A57" s="92"/>
-      <c r="B57" s="93"/>
-      <c r="C57" s="96"/>
-      <c r="D57" s="97"/>
-      <c r="E57" s="96"/>
-      <c r="F57" s="97"/>
+      <c r="A57" s="93"/>
+      <c r="B57" s="94"/>
+      <c r="C57" s="97"/>
+      <c r="D57" s="98"/>
+      <c r="E57" s="97"/>
+      <c r="F57" s="98"/>
       <c r="G57" s="25"/>
       <c r="H57" s="26"/>
       <c r="I57" s="26"/>
@@ -4800,18 +4800,18 @@
       <c r="AT57" s="35"/>
     </row>
     <row r="58" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A58" s="90" t="s">
+      <c r="A58" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="91"/>
-      <c r="C58" s="94">
+      <c r="B58" s="92"/>
+      <c r="C58" s="95">
         <v>2</v>
       </c>
-      <c r="D58" s="95"/>
-      <c r="E58" s="94">
+      <c r="D58" s="96"/>
+      <c r="E58" s="95">
         <v>2</v>
       </c>
-      <c r="F58" s="95"/>
+      <c r="F58" s="96"/>
       <c r="G58" s="25"/>
       <c r="H58" s="26"/>
       <c r="I58" s="26"/>
@@ -4852,12 +4852,12 @@
       <c r="AT58" s="35"/>
     </row>
     <row r="59" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A59" s="92"/>
-      <c r="B59" s="93"/>
-      <c r="C59" s="96"/>
-      <c r="D59" s="97"/>
-      <c r="E59" s="96"/>
-      <c r="F59" s="97"/>
+      <c r="A59" s="93"/>
+      <c r="B59" s="94"/>
+      <c r="C59" s="97"/>
+      <c r="D59" s="98"/>
+      <c r="E59" s="97"/>
+      <c r="F59" s="98"/>
       <c r="G59" s="25"/>
       <c r="H59" s="26"/>
       <c r="I59" s="26"/>
@@ -4898,18 +4898,18 @@
       <c r="AT59" s="35"/>
     </row>
     <row r="60" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A60" s="90" t="s">
+      <c r="A60" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="B60" s="91"/>
-      <c r="C60" s="94">
+      <c r="B60" s="92"/>
+      <c r="C60" s="95">
         <v>6</v>
       </c>
-      <c r="D60" s="95"/>
-      <c r="E60" s="94">
+      <c r="D60" s="96"/>
+      <c r="E60" s="95">
         <v>6</v>
       </c>
-      <c r="F60" s="95"/>
+      <c r="F60" s="96"/>
       <c r="G60" s="25"/>
       <c r="H60" s="26"/>
       <c r="I60" s="26"/>
@@ -4949,12 +4949,12 @@
       <c r="AT60" s="35"/>
     </row>
     <row r="61" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A61" s="92"/>
-      <c r="B61" s="93"/>
-      <c r="C61" s="96"/>
-      <c r="D61" s="97"/>
-      <c r="E61" s="96"/>
-      <c r="F61" s="97"/>
+      <c r="A61" s="93"/>
+      <c r="B61" s="94"/>
+      <c r="C61" s="97"/>
+      <c r="D61" s="98"/>
+      <c r="E61" s="97"/>
+      <c r="F61" s="98"/>
       <c r="G61" s="25"/>
       <c r="H61" s="26"/>
       <c r="I61" s="26"/>
@@ -4993,18 +4993,18 @@
       <c r="AT61" s="35"/>
     </row>
     <row r="62" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A62" s="90" t="s">
+      <c r="A62" s="91" t="s">
         <v>80</v>
       </c>
-      <c r="B62" s="91"/>
-      <c r="C62" s="94">
+      <c r="B62" s="92"/>
+      <c r="C62" s="95">
         <v>4</v>
       </c>
-      <c r="D62" s="95"/>
-      <c r="E62" s="94">
+      <c r="D62" s="96"/>
+      <c r="E62" s="95">
         <v>4</v>
       </c>
-      <c r="F62" s="95"/>
+      <c r="F62" s="96"/>
       <c r="G62" s="25"/>
       <c r="H62" s="26"/>
       <c r="I62" s="26"/>
@@ -5044,12 +5044,12 @@
       <c r="AT62" s="35"/>
     </row>
     <row r="63" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A63" s="92"/>
-      <c r="B63" s="93"/>
-      <c r="C63" s="96"/>
-      <c r="D63" s="97"/>
-      <c r="E63" s="96"/>
-      <c r="F63" s="97"/>
+      <c r="A63" s="93"/>
+      <c r="B63" s="94"/>
+      <c r="C63" s="97"/>
+      <c r="D63" s="98"/>
+      <c r="E63" s="97"/>
+      <c r="F63" s="98"/>
       <c r="G63" s="25"/>
       <c r="H63" s="26"/>
       <c r="I63" s="26"/>
@@ -5090,20 +5090,20 @@
       <c r="AT63" s="35"/>
     </row>
     <row r="64" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="132" t="s">
+      <c r="A64" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="B64" s="133"/>
-      <c r="C64" s="134">
+      <c r="B64" s="100"/>
+      <c r="C64" s="101">
         <f>SUM(C65:D66)</f>
         <v>4</v>
       </c>
-      <c r="D64" s="135"/>
-      <c r="E64" s="134">
+      <c r="D64" s="102"/>
+      <c r="E64" s="101">
         <f>SUM(E65)</f>
         <v>4</v>
       </c>
-      <c r="F64" s="135"/>
+      <c r="F64" s="102"/>
       <c r="G64" s="31"/>
       <c r="H64" s="32"/>
       <c r="I64" s="32"/>
@@ -5146,18 +5146,18 @@
       <c r="AT64" s="33"/>
     </row>
     <row r="65" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="110" t="s">
+      <c r="A65" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B65" s="95"/>
-      <c r="C65" s="94">
+      <c r="B65" s="96"/>
+      <c r="C65" s="95">
         <v>4</v>
       </c>
-      <c r="D65" s="95"/>
-      <c r="E65" s="94">
+      <c r="D65" s="96"/>
+      <c r="E65" s="95">
         <v>4</v>
       </c>
-      <c r="F65" s="95"/>
+      <c r="F65" s="96"/>
       <c r="G65" s="25"/>
       <c r="H65" s="26"/>
       <c r="I65" s="26"/>
@@ -5199,12 +5199,12 @@
       <c r="AT65" s="35"/>
     </row>
     <row r="66" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="138"/>
-      <c r="B66" s="97"/>
-      <c r="C66" s="96"/>
-      <c r="D66" s="97"/>
-      <c r="E66" s="96"/>
-      <c r="F66" s="97"/>
+      <c r="A66" s="104"/>
+      <c r="B66" s="98"/>
+      <c r="C66" s="97"/>
+      <c r="D66" s="98"/>
+      <c r="E66" s="97"/>
+      <c r="F66" s="98"/>
       <c r="G66" s="25"/>
       <c r="H66" s="26"/>
       <c r="I66" s="26"/>
@@ -5246,20 +5246,20 @@
       <c r="AT66" s="35"/>
     </row>
     <row r="67" spans="1:59" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="132" t="s">
+      <c r="A67" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="B67" s="133"/>
-      <c r="C67" s="134">
+      <c r="B67" s="100"/>
+      <c r="C67" s="101">
         <f>SUM(C68:D69)</f>
         <v>4</v>
       </c>
-      <c r="D67" s="135"/>
-      <c r="E67" s="134">
+      <c r="D67" s="102"/>
+      <c r="E67" s="101">
         <f>SUM(E68)</f>
         <v>4</v>
       </c>
-      <c r="F67" s="135"/>
+      <c r="F67" s="102"/>
       <c r="G67" s="31"/>
       <c r="H67" s="32"/>
       <c r="I67" s="32"/>
@@ -5302,18 +5302,18 @@
       <c r="AT67" s="33"/>
     </row>
     <row r="68" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A68" s="110" t="s">
+      <c r="A68" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="B68" s="95"/>
-      <c r="C68" s="94">
+      <c r="B68" s="96"/>
+      <c r="C68" s="95">
         <v>4</v>
       </c>
-      <c r="D68" s="95"/>
-      <c r="E68" s="94">
+      <c r="D68" s="96"/>
+      <c r="E68" s="95">
         <v>4</v>
       </c>
-      <c r="F68" s="95"/>
+      <c r="F68" s="96"/>
       <c r="G68" s="25"/>
       <c r="H68" s="26"/>
       <c r="I68" s="26"/>
@@ -5356,12 +5356,12 @@
       <c r="AU68" s="38"/>
     </row>
     <row r="69" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A69" s="138"/>
-      <c r="B69" s="97"/>
-      <c r="C69" s="96"/>
-      <c r="D69" s="97"/>
-      <c r="E69" s="96"/>
-      <c r="F69" s="97"/>
+      <c r="A69" s="104"/>
+      <c r="B69" s="98"/>
+      <c r="C69" s="97"/>
+      <c r="D69" s="98"/>
+      <c r="E69" s="97"/>
+      <c r="F69" s="98"/>
       <c r="G69" s="25"/>
       <c r="H69" s="26"/>
       <c r="I69" s="26"/>
@@ -5403,20 +5403,20 @@
       <c r="AU69" s="39"/>
     </row>
     <row r="70" spans="1:59" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="157" t="s">
+      <c r="A70" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="B70" s="158"/>
-      <c r="C70" s="159">
+      <c r="B70" s="112"/>
+      <c r="C70" s="113">
         <f>SUM(C71:D76)</f>
         <v>12</v>
       </c>
-      <c r="D70" s="160"/>
-      <c r="E70" s="134">
+      <c r="D70" s="114"/>
+      <c r="E70" s="101">
         <f>SUM(E71:F76)</f>
         <v>12</v>
       </c>
-      <c r="F70" s="135"/>
+      <c r="F70" s="102"/>
       <c r="G70" s="40"/>
       <c r="H70" s="41"/>
       <c r="I70" s="41"/>
@@ -5460,18 +5460,18 @@
       <c r="AU70" s="3"/>
     </row>
     <row r="71" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A71" s="110" t="s">
+      <c r="A71" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="B71" s="95"/>
-      <c r="C71" s="94">
+      <c r="B71" s="96"/>
+      <c r="C71" s="95">
         <v>6</v>
       </c>
-      <c r="D71" s="95"/>
-      <c r="E71" s="94">
+      <c r="D71" s="96"/>
+      <c r="E71" s="95">
         <v>6</v>
       </c>
-      <c r="F71" s="95"/>
+      <c r="F71" s="96"/>
       <c r="G71" s="25"/>
       <c r="H71" s="26"/>
       <c r="I71" s="26"/>
@@ -5511,12 +5511,12 @@
       <c r="AU71" s="3"/>
     </row>
     <row r="72" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A72" s="138"/>
-      <c r="B72" s="97"/>
-      <c r="C72" s="96"/>
-      <c r="D72" s="97"/>
-      <c r="E72" s="96"/>
-      <c r="F72" s="97"/>
+      <c r="A72" s="104"/>
+      <c r="B72" s="98"/>
+      <c r="C72" s="97"/>
+      <c r="D72" s="98"/>
+      <c r="E72" s="97"/>
+      <c r="F72" s="98"/>
       <c r="G72" s="25"/>
       <c r="H72" s="26"/>
       <c r="I72" s="26"/>
@@ -5569,18 +5569,18 @@
       <c r="BG72" s="38"/>
     </row>
     <row r="73" spans="1:59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="110" t="s">
+      <c r="A73" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="B73" s="95"/>
-      <c r="C73" s="94">
+      <c r="B73" s="96"/>
+      <c r="C73" s="95">
         <v>6</v>
       </c>
-      <c r="D73" s="95"/>
-      <c r="E73" s="94">
+      <c r="D73" s="96"/>
+      <c r="E73" s="95">
         <v>6</v>
       </c>
-      <c r="F73" s="95"/>
+      <c r="F73" s="96"/>
       <c r="G73" s="25"/>
       <c r="H73" s="26"/>
       <c r="I73" s="26"/>
@@ -5636,12 +5636,12 @@
       <c r="BG73" s="38"/>
     </row>
     <row r="74" spans="1:59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="138"/>
-      <c r="B74" s="97"/>
-      <c r="C74" s="96"/>
-      <c r="D74" s="97"/>
-      <c r="E74" s="96"/>
-      <c r="F74" s="97"/>
+      <c r="A74" s="104"/>
+      <c r="B74" s="98"/>
+      <c r="C74" s="97"/>
+      <c r="D74" s="98"/>
+      <c r="E74" s="97"/>
+      <c r="F74" s="98"/>
       <c r="G74" s="25"/>
       <c r="H74" s="26"/>
       <c r="I74" s="26"/>
@@ -5694,18 +5694,18 @@
       <c r="BG74" s="38"/>
     </row>
     <row r="75" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A75" s="110" t="s">
+      <c r="A75" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="B75" s="95"/>
-      <c r="C75" s="94">
+      <c r="B75" s="96"/>
+      <c r="C75" s="95">
         <v>0</v>
       </c>
-      <c r="D75" s="95"/>
-      <c r="E75" s="94">
+      <c r="D75" s="96"/>
+      <c r="E75" s="95">
         <v>0</v>
       </c>
-      <c r="F75" s="95"/>
+      <c r="F75" s="96"/>
       <c r="G75" s="25"/>
       <c r="H75" s="26"/>
       <c r="I75" s="26"/>
@@ -5757,12 +5757,12 @@
       <c r="BG75" s="39"/>
     </row>
     <row r="76" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A76" s="138"/>
-      <c r="B76" s="97"/>
-      <c r="C76" s="96"/>
-      <c r="D76" s="97"/>
-      <c r="E76" s="96"/>
-      <c r="F76" s="97"/>
+      <c r="A76" s="104"/>
+      <c r="B76" s="98"/>
+      <c r="C76" s="97"/>
+      <c r="D76" s="98"/>
+      <c r="E76" s="97"/>
+      <c r="F76" s="98"/>
       <c r="G76" s="25"/>
       <c r="H76" s="26"/>
       <c r="I76" s="26"/>
@@ -5876,20 +5876,20 @@
       <c r="BG77" s="3"/>
     </row>
     <row r="78" spans="1:59" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="151" t="s">
+      <c r="A78" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="B78" s="152"/>
-      <c r="C78" s="153">
+      <c r="B78" s="106"/>
+      <c r="C78" s="107">
         <f>SUM(C14+C17+C29+C42+C47+C64+C67+C26 + C70)</f>
         <v>74</v>
       </c>
-      <c r="D78" s="154"/>
-      <c r="E78" s="155">
+      <c r="D78" s="108"/>
+      <c r="E78" s="109">
         <f>SUM(E14+E17+E29+E42+E47+E64+E67+E26+E70)</f>
         <v>74</v>
       </c>
-      <c r="F78" s="156"/>
+      <c r="F78" s="110"/>
       <c r="G78" s="39"/>
       <c r="H78" s="39"/>
       <c r="I78" s="39"/>
@@ -6007,107 +6007,6 @@
     </row>
   </sheetData>
   <mergeCells count="125">
-    <mergeCell ref="A60:B61"/>
-    <mergeCell ref="C60:D61"/>
-    <mergeCell ref="E60:F61"/>
-    <mergeCell ref="A62:B63"/>
-    <mergeCell ref="C62:D63"/>
-    <mergeCell ref="E62:F63"/>
-    <mergeCell ref="A56:B57"/>
-    <mergeCell ref="C56:D57"/>
-    <mergeCell ref="E56:F57"/>
-    <mergeCell ref="A58:B59"/>
-    <mergeCell ref="C58:D59"/>
-    <mergeCell ref="E58:F59"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="A68:B69"/>
-    <mergeCell ref="C68:D69"/>
-    <mergeCell ref="E68:F69"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="A65:B66"/>
-    <mergeCell ref="C65:D66"/>
-    <mergeCell ref="E65:F66"/>
-    <mergeCell ref="A75:B76"/>
-    <mergeCell ref="C75:D76"/>
-    <mergeCell ref="E75:F76"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="A71:B72"/>
-    <mergeCell ref="C71:D72"/>
-    <mergeCell ref="E71:F72"/>
-    <mergeCell ref="A73:B74"/>
-    <mergeCell ref="C73:D74"/>
-    <mergeCell ref="E73:F74"/>
-    <mergeCell ref="A52:B53"/>
-    <mergeCell ref="C52:D53"/>
-    <mergeCell ref="E52:F53"/>
-    <mergeCell ref="A54:B55"/>
-    <mergeCell ref="C54:D55"/>
-    <mergeCell ref="E54:F55"/>
-    <mergeCell ref="A48:B49"/>
-    <mergeCell ref="C48:D49"/>
-    <mergeCell ref="E48:F49"/>
-    <mergeCell ref="A50:B51"/>
-    <mergeCell ref="C50:D51"/>
-    <mergeCell ref="E50:F51"/>
-    <mergeCell ref="A45:B46"/>
-    <mergeCell ref="C45:D46"/>
-    <mergeCell ref="E45:F46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="A40:B41"/>
-    <mergeCell ref="C40:D41"/>
-    <mergeCell ref="E40:F41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="C43:D44"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="A38:B39"/>
-    <mergeCell ref="C38:D39"/>
-    <mergeCell ref="E38:F39"/>
-    <mergeCell ref="A34:B35"/>
-    <mergeCell ref="C34:D35"/>
-    <mergeCell ref="E34:F35"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="E36:F37"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="E30:F31"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:F28"/>
-    <mergeCell ref="C22:D23"/>
-    <mergeCell ref="E22:F23"/>
-    <mergeCell ref="A24:B25"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="E24:F25"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="E20:F21"/>
     <mergeCell ref="A32:B33"/>
     <mergeCell ref="C32:D33"/>
     <mergeCell ref="E32:F33"/>
@@ -6132,6 +6031,107 @@
     <mergeCell ref="C11:D13"/>
     <mergeCell ref="A11:B13"/>
     <mergeCell ref="A22:B23"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="E22:F23"/>
+    <mergeCell ref="A24:B25"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="E24:F25"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="E20:F21"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="E30:F31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:F28"/>
+    <mergeCell ref="A38:B39"/>
+    <mergeCell ref="C38:D39"/>
+    <mergeCell ref="E38:F39"/>
+    <mergeCell ref="A34:B35"/>
+    <mergeCell ref="C34:D35"/>
+    <mergeCell ref="E34:F35"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="E36:F37"/>
+    <mergeCell ref="A45:B46"/>
+    <mergeCell ref="C45:D46"/>
+    <mergeCell ref="E45:F46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="A40:B41"/>
+    <mergeCell ref="C40:D41"/>
+    <mergeCell ref="E40:F41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="C43:D44"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="A52:B53"/>
+    <mergeCell ref="C52:D53"/>
+    <mergeCell ref="E52:F53"/>
+    <mergeCell ref="A54:B55"/>
+    <mergeCell ref="C54:D55"/>
+    <mergeCell ref="E54:F55"/>
+    <mergeCell ref="A48:B49"/>
+    <mergeCell ref="C48:D49"/>
+    <mergeCell ref="E48:F49"/>
+    <mergeCell ref="A50:B51"/>
+    <mergeCell ref="C50:D51"/>
+    <mergeCell ref="E50:F51"/>
+    <mergeCell ref="A75:B76"/>
+    <mergeCell ref="C75:D76"/>
+    <mergeCell ref="E75:F76"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="A71:B72"/>
+    <mergeCell ref="C71:D72"/>
+    <mergeCell ref="E71:F72"/>
+    <mergeCell ref="A73:B74"/>
+    <mergeCell ref="C73:D74"/>
+    <mergeCell ref="E73:F74"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="A68:B69"/>
+    <mergeCell ref="C68:D69"/>
+    <mergeCell ref="E68:F69"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="A65:B66"/>
+    <mergeCell ref="C65:D66"/>
+    <mergeCell ref="E65:F66"/>
+    <mergeCell ref="A60:B61"/>
+    <mergeCell ref="C60:D61"/>
+    <mergeCell ref="E60:F61"/>
+    <mergeCell ref="A62:B63"/>
+    <mergeCell ref="C62:D63"/>
+    <mergeCell ref="E62:F63"/>
+    <mergeCell ref="A56:B57"/>
+    <mergeCell ref="C56:D57"/>
+    <mergeCell ref="E56:F57"/>
+    <mergeCell ref="A58:B59"/>
+    <mergeCell ref="C58:D59"/>
+    <mergeCell ref="E58:F59"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
controller for shop and product
</commit_message>
<xml_diff>
--- a/documentation/Zeitplan.xlsx
+++ b/documentation/Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp8\htdocs\IPA\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116D1F35-78C8-478D-A826-65F66B9269B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA57A392-4865-4FE5-AF63-02B809952802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
   <si>
     <t>Projekttitel</t>
   </si>
@@ -464,7 +464,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -885,19 +885,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color theme="1"/>
@@ -1024,7 +1011,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1143,7 +1130,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1178,7 +1164,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="37" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="36" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1201,43 +1187,43 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="39" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="43" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="43" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="3" applyBorder="1"/>
@@ -1245,7 +1231,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="43" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1280,6 +1266,108 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1292,11 +1380,50 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1327,147 +1454,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1758,8 +1744,8 @@
   </sheetPr>
   <dimension ref="A1:BG79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="Z44" sqref="Z44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="AB59" sqref="AB59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,27 +1758,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:59" ht="44.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="116" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
-      <c r="E1" s="153"/>
-      <c r="F1" s="153"/>
-      <c r="G1" s="153"/>
-      <c r="H1" s="153"/>
-      <c r="I1" s="153"/>
-      <c r="J1" s="153"/>
-      <c r="K1" s="153"/>
-      <c r="L1" s="153"/>
-      <c r="M1" s="153"/>
-      <c r="N1" s="153"/>
-      <c r="O1" s="153"/>
-      <c r="P1" s="153"/>
-      <c r="Q1" s="153"/>
-      <c r="R1" s="153"/>
-      <c r="S1" s="153"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
+      <c r="M1" s="116"/>
+      <c r="N1" s="116"/>
+      <c r="O1" s="116"/>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="116"/>
+      <c r="R1" s="116"/>
+      <c r="S1" s="116"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
@@ -2175,7 +2161,7 @@
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
       <c r="AL7" s="3"/>
-      <c r="AN7" s="67" t="s">
+      <c r="AN7" s="66" t="s">
         <v>20</v>
       </c>
       <c r="AO7" s="28" t="s">
@@ -2241,7 +2227,7 @@
       <c r="AI8" s="3"/>
       <c r="AJ8" s="3"/>
       <c r="AL8" s="3"/>
-      <c r="AN8" s="68"/>
+      <c r="AN8" s="67"/>
       <c r="AT8" s="29"/>
       <c r="AV8" s="3"/>
       <c r="AW8" s="3"/>
@@ -2294,8 +2280,8 @@
       <c r="AI9" s="3"/>
       <c r="AJ9" s="3"/>
       <c r="AL9" s="3"/>
-      <c r="AN9" s="69"/>
-      <c r="AO9" s="70" t="s">
+      <c r="AN9" s="68"/>
+      <c r="AO9" s="69" t="s">
         <v>81</v>
       </c>
       <c r="AP9" s="36"/>
@@ -2368,86 +2354,86 @@
       <c r="BG10" s="3"/>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A11" s="171" t="s">
+      <c r="A11" s="137" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="172"/>
-      <c r="C11" s="166" t="s">
+      <c r="B11" s="138"/>
+      <c r="C11" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="167"/>
-      <c r="E11" s="166" t="s">
+      <c r="D11" s="133"/>
+      <c r="E11" s="132" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="167"/>
-      <c r="G11" s="154" t="s">
+      <c r="F11" s="133"/>
+      <c r="G11" s="117" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="155"/>
-      <c r="I11" s="155"/>
-      <c r="J11" s="156"/>
-      <c r="K11" s="154" t="s">
+      <c r="H11" s="118"/>
+      <c r="I11" s="118"/>
+      <c r="J11" s="119"/>
+      <c r="K11" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="L11" s="155"/>
-      <c r="M11" s="155"/>
-      <c r="N11" s="156"/>
-      <c r="O11" s="154" t="s">
+      <c r="L11" s="118"/>
+      <c r="M11" s="118"/>
+      <c r="N11" s="119"/>
+      <c r="O11" s="117" t="s">
         <v>59</v>
       </c>
-      <c r="P11" s="155"/>
-      <c r="Q11" s="155"/>
-      <c r="R11" s="156"/>
-      <c r="S11" s="154" t="s">
+      <c r="P11" s="118"/>
+      <c r="Q11" s="118"/>
+      <c r="R11" s="119"/>
+      <c r="S11" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="T11" s="155"/>
-      <c r="U11" s="155"/>
-      <c r="V11" s="156"/>
-      <c r="W11" s="154" t="s">
+      <c r="T11" s="118"/>
+      <c r="U11" s="118"/>
+      <c r="V11" s="119"/>
+      <c r="W11" s="117" t="s">
         <v>61</v>
       </c>
-      <c r="X11" s="155"/>
-      <c r="Y11" s="155"/>
-      <c r="Z11" s="156"/>
-      <c r="AA11" s="154" t="s">
+      <c r="X11" s="118"/>
+      <c r="Y11" s="118"/>
+      <c r="Z11" s="119"/>
+      <c r="AA11" s="117" t="s">
         <v>62</v>
       </c>
-      <c r="AB11" s="155"/>
-      <c r="AC11" s="155"/>
-      <c r="AD11" s="156"/>
-      <c r="AE11" s="154" t="s">
+      <c r="AB11" s="118"/>
+      <c r="AC11" s="118"/>
+      <c r="AD11" s="119"/>
+      <c r="AE11" s="117" t="s">
         <v>63</v>
       </c>
-      <c r="AF11" s="155"/>
-      <c r="AG11" s="155"/>
-      <c r="AH11" s="156"/>
-      <c r="AI11" s="154" t="s">
+      <c r="AF11" s="118"/>
+      <c r="AG11" s="118"/>
+      <c r="AH11" s="119"/>
+      <c r="AI11" s="117" t="s">
         <v>64</v>
       </c>
-      <c r="AJ11" s="155"/>
-      <c r="AK11" s="155"/>
-      <c r="AL11" s="156"/>
-      <c r="AM11" s="154" t="s">
+      <c r="AJ11" s="118"/>
+      <c r="AK11" s="118"/>
+      <c r="AL11" s="119"/>
+      <c r="AM11" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="AN11" s="155"/>
-      <c r="AO11" s="155"/>
-      <c r="AP11" s="156"/>
-      <c r="AQ11" s="154" t="s">
+      <c r="AN11" s="118"/>
+      <c r="AO11" s="118"/>
+      <c r="AP11" s="119"/>
+      <c r="AQ11" s="117" t="s">
         <v>66</v>
       </c>
-      <c r="AR11" s="155"/>
-      <c r="AS11" s="155"/>
-      <c r="AT11" s="156"/>
+      <c r="AR11" s="118"/>
+      <c r="AS11" s="118"/>
+      <c r="AT11" s="119"/>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A12" s="173"/>
-      <c r="B12" s="172"/>
-      <c r="C12" s="168"/>
-      <c r="D12" s="167"/>
-      <c r="E12" s="168"/>
-      <c r="F12" s="167"/>
+      <c r="A12" s="139"/>
+      <c r="B12" s="138"/>
+      <c r="C12" s="134"/>
+      <c r="D12" s="133"/>
+      <c r="E12" s="134"/>
+      <c r="F12" s="133"/>
       <c r="G12" s="10">
         <v>1</v>
       </c>
@@ -2570,12 +2556,12 @@
       </c>
     </row>
     <row r="13" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="174"/>
-      <c r="B13" s="175"/>
-      <c r="C13" s="169"/>
-      <c r="D13" s="170"/>
-      <c r="E13" s="169"/>
-      <c r="F13" s="170"/>
+      <c r="A13" s="140"/>
+      <c r="B13" s="141"/>
+      <c r="C13" s="135"/>
+      <c r="D13" s="136"/>
+      <c r="E13" s="135"/>
+      <c r="F13" s="136"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
@@ -2618,20 +2604,20 @@
       <c r="AT13" s="16"/>
     </row>
     <row r="14" spans="1:59" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="157" t="s">
+      <c r="A14" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="158"/>
-      <c r="C14" s="159">
+      <c r="B14" s="121"/>
+      <c r="C14" s="122">
         <f>SUM(C15:D16)</f>
         <v>6</v>
       </c>
-      <c r="D14" s="160"/>
-      <c r="E14" s="159">
+      <c r="D14" s="123"/>
+      <c r="E14" s="122">
         <f>SUM(E15)</f>
         <v>6</v>
       </c>
-      <c r="F14" s="160"/>
+      <c r="F14" s="123"/>
       <c r="G14" s="18"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
@@ -2674,18 +2660,18 @@
       <c r="AT14" s="20"/>
     </row>
     <row r="15" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="117" t="s">
+      <c r="A15" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="161"/>
-      <c r="C15" s="164">
+      <c r="B15" s="125"/>
+      <c r="C15" s="128">
         <v>6</v>
       </c>
-      <c r="D15" s="137"/>
-      <c r="E15" s="164">
+      <c r="D15" s="129"/>
+      <c r="E15" s="128">
         <v>6</v>
       </c>
-      <c r="F15" s="137"/>
+      <c r="F15" s="129"/>
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
       <c r="I15" s="26"/>
@@ -2697,7 +2683,7 @@
       <c r="O15" s="25"/>
       <c r="P15" s="26"/>
       <c r="Q15" s="52"/>
-      <c r="R15" s="60"/>
+      <c r="R15" s="59"/>
       <c r="S15" s="27"/>
       <c r="T15" s="26"/>
       <c r="U15" s="26"/>
@@ -2712,8 +2698,8 @@
       <c r="AD15" s="50"/>
       <c r="AE15" s="25"/>
       <c r="AF15" s="52"/>
-      <c r="AG15" s="60"/>
-      <c r="AH15" s="60"/>
+      <c r="AG15" s="59"/>
+      <c r="AH15" s="59"/>
       <c r="AI15" s="25"/>
       <c r="AJ15" s="26"/>
       <c r="AK15" s="26"/>
@@ -2728,12 +2714,12 @@
       <c r="AT15" s="50"/>
     </row>
     <row r="16" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="162"/>
-      <c r="B16" s="163"/>
-      <c r="C16" s="165"/>
-      <c r="D16" s="139"/>
-      <c r="E16" s="165"/>
-      <c r="F16" s="139"/>
+      <c r="A16" s="126"/>
+      <c r="B16" s="127"/>
+      <c r="C16" s="130"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="131"/>
       <c r="G16" s="30"/>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
@@ -2743,7 +2729,7 @@
       <c r="O16" s="25"/>
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
-      <c r="R16" s="59"/>
+      <c r="R16" s="58"/>
       <c r="S16" s="27"/>
       <c r="T16" s="26"/>
       <c r="U16" s="26"/>
@@ -2755,8 +2741,8 @@
       <c r="AC16" s="26"/>
       <c r="AE16" s="25"/>
       <c r="AF16" s="26"/>
-      <c r="AG16" s="60"/>
-      <c r="AH16" s="59"/>
+      <c r="AG16" s="59"/>
+      <c r="AH16" s="58"/>
       <c r="AI16" s="25"/>
       <c r="AJ16" s="26"/>
       <c r="AK16" s="26"/>
@@ -2766,23 +2752,23 @@
       <c r="AQ16" s="25"/>
       <c r="AR16" s="26"/>
       <c r="AS16" s="26"/>
-      <c r="AT16" s="55"/>
+      <c r="AT16" s="54"/>
     </row>
     <row r="17" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="113" t="s">
+      <c r="A17" s="146" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="114"/>
-      <c r="C17" s="115">
+      <c r="B17" s="147"/>
+      <c r="C17" s="148">
         <f>SUM(C18:D25)</f>
         <v>12</v>
       </c>
-      <c r="D17" s="116"/>
-      <c r="E17" s="147">
+      <c r="D17" s="149"/>
+      <c r="E17" s="150">
         <f>SUM(E18:F25)</f>
         <v>12</v>
       </c>
-      <c r="F17" s="148"/>
+      <c r="F17" s="151"/>
       <c r="G17" s="31"/>
       <c r="H17" s="32"/>
       <c r="I17" s="32"/>
@@ -2794,7 +2780,7 @@
       <c r="O17" s="31"/>
       <c r="P17" s="32"/>
       <c r="Q17" s="32"/>
-      <c r="R17" s="61"/>
+      <c r="R17" s="60"/>
       <c r="S17" s="34"/>
       <c r="T17" s="32"/>
       <c r="U17" s="32"/>
@@ -2809,8 +2795,8 @@
       <c r="AD17" s="33"/>
       <c r="AE17" s="31"/>
       <c r="AF17" s="32"/>
-      <c r="AG17" s="61"/>
-      <c r="AH17" s="61"/>
+      <c r="AG17" s="60"/>
+      <c r="AH17" s="60"/>
       <c r="AI17" s="31"/>
       <c r="AJ17" s="32"/>
       <c r="AK17" s="32"/>
@@ -2825,21 +2811,21 @@
       <c r="AT17" s="33"/>
     </row>
     <row r="18" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="117" t="s">
+      <c r="A18" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="110"/>
-      <c r="C18" s="109">
+      <c r="B18" s="109"/>
+      <c r="C18" s="108">
         <v>6</v>
       </c>
-      <c r="D18" s="110"/>
-      <c r="E18" s="109">
+      <c r="D18" s="109"/>
+      <c r="E18" s="108">
         <v>6</v>
       </c>
-      <c r="F18" s="110"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="79"/>
-      <c r="I18" s="79"/>
+      <c r="F18" s="109"/>
+      <c r="G18" s="77"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="78"/>
       <c r="J18" s="35"/>
       <c r="K18" s="25"/>
       <c r="L18" s="26"/>
@@ -2848,7 +2834,7 @@
       <c r="O18" s="25"/>
       <c r="P18" s="26"/>
       <c r="Q18" s="26"/>
-      <c r="R18" s="60"/>
+      <c r="R18" s="59"/>
       <c r="S18" s="27"/>
       <c r="T18" s="26"/>
       <c r="U18" s="26"/>
@@ -2863,8 +2849,8 @@
       <c r="AD18" s="35"/>
       <c r="AE18" s="25"/>
       <c r="AF18" s="26"/>
-      <c r="AG18" s="60"/>
-      <c r="AH18" s="60"/>
+      <c r="AG18" s="59"/>
+      <c r="AH18" s="59"/>
       <c r="AI18" s="25"/>
       <c r="AJ18" s="26"/>
       <c r="AK18" s="26"/>
@@ -2879,16 +2865,16 @@
       <c r="AT18" s="35"/>
     </row>
     <row r="19" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="118"/>
-      <c r="B19" s="112"/>
-      <c r="C19" s="111"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="112"/>
-      <c r="G19" s="102"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="75"/>
+      <c r="A19" s="152"/>
+      <c r="B19" s="111"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="111"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="101"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="74"/>
       <c r="K19" s="25"/>
       <c r="L19" s="26"/>
       <c r="M19" s="26"/>
@@ -2896,7 +2882,7 @@
       <c r="O19" s="25"/>
       <c r="P19" s="26"/>
       <c r="Q19" s="26"/>
-      <c r="R19" s="60"/>
+      <c r="R19" s="59"/>
       <c r="S19" s="27"/>
       <c r="T19" s="26"/>
       <c r="U19" s="26"/>
@@ -2911,8 +2897,8 @@
       <c r="AD19" s="35"/>
       <c r="AE19" s="25"/>
       <c r="AF19" s="26"/>
-      <c r="AG19" s="60"/>
-      <c r="AH19" s="60"/>
+      <c r="AG19" s="59"/>
+      <c r="AH19" s="59"/>
       <c r="AI19" s="25"/>
       <c r="AJ19" s="26"/>
       <c r="AK19" s="26"/>
@@ -2927,22 +2913,22 @@
       <c r="AT19" s="35"/>
     </row>
     <row r="20" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="117" t="s">
+      <c r="A20" s="124" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="110"/>
-      <c r="C20" s="109">
+      <c r="B20" s="109"/>
+      <c r="C20" s="108">
         <v>2</v>
       </c>
-      <c r="D20" s="110"/>
-      <c r="E20" s="109">
+      <c r="D20" s="109"/>
+      <c r="E20" s="108">
         <v>2</v>
       </c>
-      <c r="F20" s="110"/>
-      <c r="G20" s="87"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="76"/>
+      <c r="F20" s="109"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="75"/>
       <c r="K20" s="25"/>
       <c r="L20" s="26"/>
       <c r="M20" s="26"/>
@@ -2950,7 +2936,7 @@
       <c r="O20" s="25"/>
       <c r="P20" s="26"/>
       <c r="Q20" s="26"/>
-      <c r="R20" s="60"/>
+      <c r="R20" s="59"/>
       <c r="S20" s="27"/>
       <c r="T20" s="26"/>
       <c r="U20" s="26"/>
@@ -2965,8 +2951,8 @@
       <c r="AD20" s="35"/>
       <c r="AE20" s="25"/>
       <c r="AF20" s="26"/>
-      <c r="AG20" s="60"/>
-      <c r="AH20" s="60"/>
+      <c r="AG20" s="59"/>
+      <c r="AH20" s="59"/>
       <c r="AI20" s="25"/>
       <c r="AJ20" s="26"/>
       <c r="AK20" s="26"/>
@@ -2981,16 +2967,16 @@
       <c r="AT20" s="35"/>
     </row>
     <row r="21" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="118"/>
-      <c r="B21" s="112"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="111"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="87"/>
+      <c r="A21" s="152"/>
+      <c r="B21" s="111"/>
+      <c r="C21" s="110"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="86"/>
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
-      <c r="J21" s="77"/>
+      <c r="J21" s="76"/>
       <c r="K21" s="25"/>
       <c r="L21" s="26"/>
       <c r="M21" s="26"/>
@@ -2998,7 +2984,7 @@
       <c r="O21" s="25"/>
       <c r="P21" s="26"/>
       <c r="Q21" s="26"/>
-      <c r="R21" s="60"/>
+      <c r="R21" s="59"/>
       <c r="S21" s="27"/>
       <c r="T21" s="26"/>
       <c r="U21" s="26"/>
@@ -3013,8 +2999,8 @@
       <c r="AD21" s="35"/>
       <c r="AE21" s="25"/>
       <c r="AF21" s="26"/>
-      <c r="AG21" s="60"/>
-      <c r="AH21" s="60"/>
+      <c r="AG21" s="59"/>
+      <c r="AH21" s="59"/>
       <c r="AI21" s="25"/>
       <c r="AJ21" s="26"/>
       <c r="AK21" s="26"/>
@@ -3029,29 +3015,29 @@
       <c r="AT21" s="35"/>
     </row>
     <row r="22" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="105" t="s">
+      <c r="A22" s="104" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="106"/>
-      <c r="C22" s="109">
+      <c r="B22" s="105"/>
+      <c r="C22" s="108">
         <v>2</v>
       </c>
-      <c r="D22" s="110"/>
-      <c r="E22" s="109">
+      <c r="D22" s="109"/>
+      <c r="E22" s="108">
         <v>2</v>
       </c>
-      <c r="F22" s="110"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="81"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="58"/>
+      <c r="F22" s="109"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="57"/>
       <c r="M22" s="26"/>
       <c r="N22" s="35"/>
       <c r="O22" s="25"/>
       <c r="P22" s="26"/>
       <c r="Q22" s="26"/>
-      <c r="R22" s="60"/>
+      <c r="R22" s="59"/>
       <c r="S22" s="27"/>
       <c r="T22" s="26"/>
       <c r="U22" s="26"/>
@@ -3066,8 +3052,8 @@
       <c r="AD22" s="35"/>
       <c r="AE22" s="25"/>
       <c r="AF22" s="26"/>
-      <c r="AG22" s="60"/>
-      <c r="AH22" s="60"/>
+      <c r="AG22" s="59"/>
+      <c r="AH22" s="59"/>
       <c r="AI22" s="25"/>
       <c r="AJ22" s="26"/>
       <c r="AK22" s="26"/>
@@ -3082,16 +3068,16 @@
       <c r="AT22" s="35"/>
     </row>
     <row r="23" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="107"/>
-      <c r="B23" s="108"/>
-      <c r="C23" s="111"/>
-      <c r="D23" s="112"/>
-      <c r="E23" s="111"/>
-      <c r="F23" s="112"/>
+      <c r="A23" s="106"/>
+      <c r="B23" s="107"/>
+      <c r="C23" s="110"/>
+      <c r="D23" s="111"/>
+      <c r="E23" s="110"/>
+      <c r="F23" s="111"/>
       <c r="G23" s="25"/>
-      <c r="H23" s="82"/>
-      <c r="I23" s="82"/>
-      <c r="J23" s="71"/>
+      <c r="H23" s="81"/>
+      <c r="I23" s="81"/>
+      <c r="J23" s="70"/>
       <c r="K23" s="27"/>
       <c r="L23" s="26"/>
       <c r="M23" s="26"/>
@@ -3099,7 +3085,7 @@
       <c r="O23" s="25"/>
       <c r="P23" s="26"/>
       <c r="Q23" s="26"/>
-      <c r="R23" s="60"/>
+      <c r="R23" s="59"/>
       <c r="S23" s="27"/>
       <c r="T23" s="26"/>
       <c r="U23" s="26"/>
@@ -3114,8 +3100,8 @@
       <c r="AD23" s="35"/>
       <c r="AE23" s="25"/>
       <c r="AF23" s="26"/>
-      <c r="AG23" s="60"/>
-      <c r="AH23" s="60"/>
+      <c r="AG23" s="59"/>
+      <c r="AH23" s="59"/>
       <c r="AI23" s="25"/>
       <c r="AJ23" s="26"/>
       <c r="AK23" s="26"/>
@@ -3130,30 +3116,30 @@
       <c r="AT23" s="35"/>
     </row>
     <row r="24" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="105" t="s">
+      <c r="A24" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="106"/>
-      <c r="C24" s="109">
+      <c r="B24" s="105"/>
+      <c r="C24" s="108">
         <v>2</v>
       </c>
-      <c r="D24" s="110"/>
-      <c r="E24" s="149">
+      <c r="D24" s="109"/>
+      <c r="E24" s="142">
         <v>2</v>
       </c>
-      <c r="F24" s="150"/>
+      <c r="F24" s="143"/>
       <c r="G24" s="25"/>
-      <c r="H24" s="82"/>
+      <c r="H24" s="81"/>
       <c r="I24" s="26"/>
-      <c r="J24" s="55"/>
-      <c r="L24" s="64" t="s">
+      <c r="J24" s="54"/>
+      <c r="L24" s="63" t="s">
         <v>25</v>
       </c>
       <c r="N24" s="35"/>
       <c r="O24" s="25"/>
       <c r="P24" s="26"/>
       <c r="Q24" s="26"/>
-      <c r="R24" s="60"/>
+      <c r="R24" s="59"/>
       <c r="S24" s="27"/>
       <c r="T24" s="26"/>
       <c r="U24" s="26"/>
@@ -3168,8 +3154,8 @@
       <c r="AD24" s="35"/>
       <c r="AE24" s="25"/>
       <c r="AF24" s="26"/>
-      <c r="AG24" s="60"/>
-      <c r="AH24" s="60"/>
+      <c r="AG24" s="59"/>
+      <c r="AH24" s="59"/>
       <c r="AI24" s="25"/>
       <c r="AJ24" s="26" t="s">
         <v>26</v>
@@ -3186,17 +3172,17 @@
       <c r="AT24" s="35"/>
     </row>
     <row r="25" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="107"/>
-      <c r="B25" s="108"/>
-      <c r="C25" s="111"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="151"/>
-      <c r="F25" s="152"/>
+      <c r="A25" s="106"/>
+      <c r="B25" s="107"/>
+      <c r="C25" s="110"/>
+      <c r="D25" s="111"/>
+      <c r="E25" s="144"/>
+      <c r="F25" s="145"/>
       <c r="G25" s="25"/>
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
-      <c r="J25" s="83"/>
-      <c r="K25" s="72" t="s">
+      <c r="J25" s="82"/>
+      <c r="K25" s="71" t="s">
         <v>25</v>
       </c>
       <c r="L25" s="26"/>
@@ -3205,7 +3191,7 @@
       <c r="O25" s="25"/>
       <c r="P25" s="26"/>
       <c r="Q25" s="26"/>
-      <c r="R25" s="60"/>
+      <c r="R25" s="59"/>
       <c r="S25" s="27"/>
       <c r="T25" s="26"/>
       <c r="U25" s="26"/>
@@ -3220,8 +3206,8 @@
       <c r="AD25" s="35"/>
       <c r="AE25" s="25"/>
       <c r="AF25" s="26"/>
-      <c r="AG25" s="60"/>
-      <c r="AH25" s="60"/>
+      <c r="AG25" s="59"/>
+      <c r="AH25" s="59"/>
       <c r="AI25" s="25"/>
       <c r="AJ25" s="26"/>
       <c r="AK25" s="26"/>
@@ -3236,20 +3222,20 @@
       <c r="AT25" s="35"/>
     </row>
     <row r="26" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="113" t="s">
+      <c r="A26" s="146" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="114"/>
-      <c r="C26" s="115">
+      <c r="B26" s="147"/>
+      <c r="C26" s="148">
         <f>SUM(C27)</f>
         <v>2</v>
       </c>
-      <c r="D26" s="116"/>
-      <c r="E26" s="147">
+      <c r="D26" s="149"/>
+      <c r="E26" s="150">
         <f>SUM(E27)</f>
         <v>2</v>
       </c>
-      <c r="F26" s="148"/>
+      <c r="F26" s="151"/>
       <c r="G26" s="31"/>
       <c r="H26" s="32"/>
       <c r="I26" s="32"/>
@@ -3261,7 +3247,7 @@
       <c r="O26" s="31"/>
       <c r="P26" s="32"/>
       <c r="Q26" s="32"/>
-      <c r="R26" s="61"/>
+      <c r="R26" s="60"/>
       <c r="S26" s="34"/>
       <c r="T26" s="32"/>
       <c r="U26" s="32"/>
@@ -3276,8 +3262,8 @@
       <c r="AD26" s="33"/>
       <c r="AE26" s="31"/>
       <c r="AF26" s="32"/>
-      <c r="AG26" s="61"/>
-      <c r="AH26" s="61"/>
+      <c r="AG26" s="60"/>
+      <c r="AH26" s="60"/>
       <c r="AI26" s="31"/>
       <c r="AJ26" s="32"/>
       <c r="AK26" s="32"/>
@@ -3292,31 +3278,31 @@
       <c r="AT26" s="33"/>
     </row>
     <row r="27" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="117" t="s">
+      <c r="A27" s="124" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="110"/>
-      <c r="C27" s="109">
+      <c r="B27" s="109"/>
+      <c r="C27" s="108">
         <v>2</v>
       </c>
-      <c r="D27" s="110"/>
-      <c r="E27" s="109">
+      <c r="D27" s="109"/>
+      <c r="E27" s="108">
         <v>2</v>
       </c>
-      <c r="F27" s="110"/>
+      <c r="F27" s="109"/>
       <c r="G27" s="25"/>
       <c r="H27" s="26"/>
       <c r="I27" s="26"/>
       <c r="J27" s="35"/>
-      <c r="K27" s="85"/>
-      <c r="L27" s="82"/>
-      <c r="M27" s="64" t="s">
+      <c r="K27" s="84"/>
+      <c r="L27" s="81"/>
+      <c r="M27" s="63" t="s">
         <v>29</v>
       </c>
       <c r="N27" s="35"/>
       <c r="P27" s="26"/>
       <c r="Q27" s="26"/>
-      <c r="R27" s="60"/>
+      <c r="R27" s="59"/>
       <c r="S27" s="27"/>
       <c r="T27" s="26"/>
       <c r="U27" s="26"/>
@@ -3331,8 +3317,8 @@
       <c r="AD27" s="35"/>
       <c r="AE27" s="25"/>
       <c r="AF27" s="26"/>
-      <c r="AG27" s="60"/>
-      <c r="AH27" s="60"/>
+      <c r="AG27" s="59"/>
+      <c r="AH27" s="59"/>
       <c r="AI27" s="25"/>
       <c r="AJ27" s="26"/>
       <c r="AK27" s="26"/>
@@ -3347,26 +3333,26 @@
       <c r="AT27" s="35"/>
     </row>
     <row r="28" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="118"/>
-      <c r="B28" s="112"/>
-      <c r="C28" s="111"/>
-      <c r="D28" s="112"/>
-      <c r="E28" s="111"/>
-      <c r="F28" s="112"/>
+      <c r="A28" s="152"/>
+      <c r="B28" s="111"/>
+      <c r="C28" s="110"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="111"/>
       <c r="G28" s="25"/>
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
       <c r="J28" s="35"/>
-      <c r="K28" s="85"/>
-      <c r="L28" s="73"/>
-      <c r="M28" s="73" t="s">
+      <c r="K28" s="84"/>
+      <c r="L28" s="72"/>
+      <c r="M28" s="72" t="s">
         <v>29</v>
       </c>
       <c r="N28" s="35"/>
       <c r="O28" s="25"/>
       <c r="P28" s="26"/>
       <c r="Q28" s="26"/>
-      <c r="R28" s="60"/>
+      <c r="R28" s="59"/>
       <c r="S28" s="27"/>
       <c r="T28" s="26"/>
       <c r="U28" s="26"/>
@@ -3381,8 +3367,8 @@
       <c r="AD28" s="35"/>
       <c r="AE28" s="25"/>
       <c r="AF28" s="26"/>
-      <c r="AG28" s="60"/>
-      <c r="AH28" s="60"/>
+      <c r="AG28" s="59"/>
+      <c r="AH28" s="59"/>
       <c r="AI28" s="25"/>
       <c r="AJ28" s="26"/>
       <c r="AK28" s="26"/>
@@ -3397,20 +3383,20 @@
       <c r="AT28" s="35"/>
     </row>
     <row r="29" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="113" t="s">
+      <c r="A29" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="114"/>
-      <c r="C29" s="115">
+      <c r="B29" s="147"/>
+      <c r="C29" s="148">
         <f>SUM(C30:D41)</f>
         <v>12</v>
       </c>
-      <c r="D29" s="116"/>
-      <c r="E29" s="115">
+      <c r="D29" s="149"/>
+      <c r="E29" s="148">
         <f>SUM(E30:F41)</f>
         <v>12</v>
       </c>
-      <c r="F29" s="116"/>
+      <c r="F29" s="149"/>
       <c r="G29" s="31"/>
       <c r="H29" s="32"/>
       <c r="I29" s="32"/>
@@ -3422,7 +3408,7 @@
       <c r="O29" s="31"/>
       <c r="P29" s="32"/>
       <c r="Q29" s="32"/>
-      <c r="R29" s="61"/>
+      <c r="R29" s="60"/>
       <c r="S29" s="34"/>
       <c r="T29" s="32"/>
       <c r="U29" s="32"/>
@@ -3437,8 +3423,8 @@
       <c r="AD29" s="33"/>
       <c r="AE29" s="31"/>
       <c r="AF29" s="32"/>
-      <c r="AG29" s="61"/>
-      <c r="AH29" s="61"/>
+      <c r="AG29" s="60"/>
+      <c r="AH29" s="60"/>
       <c r="AI29" s="31"/>
       <c r="AJ29" s="32"/>
       <c r="AK29" s="32"/>
@@ -3453,30 +3439,30 @@
       <c r="AT29" s="33"/>
     </row>
     <row r="30" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="105" t="s">
+      <c r="A30" s="104" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="106"/>
-      <c r="C30" s="109">
+      <c r="B30" s="105"/>
+      <c r="C30" s="108">
         <v>2</v>
       </c>
-      <c r="D30" s="110"/>
-      <c r="E30" s="129">
+      <c r="D30" s="109"/>
+      <c r="E30" s="112">
         <v>2</v>
       </c>
-      <c r="F30" s="130"/>
+      <c r="F30" s="113"/>
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
       <c r="J30" s="35"/>
       <c r="K30" s="25"/>
-      <c r="L30" s="82"/>
-      <c r="M30" s="82"/>
-      <c r="N30" s="66"/>
+      <c r="L30" s="81"/>
+      <c r="M30" s="81"/>
+      <c r="N30" s="65"/>
       <c r="O30" s="25"/>
       <c r="P30" s="26"/>
       <c r="Q30" s="26"/>
-      <c r="R30" s="60"/>
+      <c r="R30" s="59"/>
       <c r="S30" s="27"/>
       <c r="T30" s="26"/>
       <c r="U30" s="26"/>
@@ -3491,8 +3477,8 @@
       <c r="AD30" s="35"/>
       <c r="AE30" s="25"/>
       <c r="AF30" s="26"/>
-      <c r="AG30" s="60"/>
-      <c r="AH30" s="60"/>
+      <c r="AG30" s="59"/>
+      <c r="AH30" s="59"/>
       <c r="AI30" s="25"/>
       <c r="AJ30" s="26"/>
       <c r="AK30" s="26"/>
@@ -3507,24 +3493,24 @@
       <c r="AT30" s="35"/>
     </row>
     <row r="31" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="107"/>
-      <c r="B31" s="108"/>
-      <c r="C31" s="111"/>
-      <c r="D31" s="112"/>
-      <c r="E31" s="131"/>
-      <c r="F31" s="132"/>
+      <c r="A31" s="106"/>
+      <c r="B31" s="107"/>
+      <c r="C31" s="110"/>
+      <c r="D31" s="111"/>
+      <c r="E31" s="114"/>
+      <c r="F31" s="115"/>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
       <c r="J31" s="35"/>
       <c r="K31" s="25"/>
-      <c r="L31" s="82"/>
-      <c r="M31" s="84"/>
-      <c r="N31" s="57"/>
+      <c r="L31" s="81"/>
+      <c r="M31" s="83"/>
+      <c r="N31" s="56"/>
       <c r="O31" s="27"/>
       <c r="P31" s="26"/>
-      <c r="Q31" s="86"/>
-      <c r="R31" s="60"/>
+      <c r="Q31" s="85"/>
+      <c r="R31" s="59"/>
       <c r="S31" s="27"/>
       <c r="T31" s="26"/>
       <c r="U31" s="26"/>
@@ -3539,8 +3525,8 @@
       <c r="AD31" s="35"/>
       <c r="AE31" s="25"/>
       <c r="AF31" s="26"/>
-      <c r="AG31" s="60"/>
-      <c r="AH31" s="60"/>
+      <c r="AG31" s="59"/>
+      <c r="AH31" s="59"/>
       <c r="AI31" s="25"/>
       <c r="AJ31" s="26"/>
       <c r="AK31" s="26"/>
@@ -3555,30 +3541,30 @@
       <c r="AT31" s="35"/>
     </row>
     <row r="32" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="105" t="s">
+      <c r="A32" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="106"/>
-      <c r="C32" s="109">
+      <c r="B32" s="105"/>
+      <c r="C32" s="108">
         <v>2</v>
       </c>
-      <c r="D32" s="110"/>
-      <c r="E32" s="129">
+      <c r="D32" s="109"/>
+      <c r="E32" s="112">
         <v>2</v>
       </c>
-      <c r="F32" s="130"/>
+      <c r="F32" s="113"/>
       <c r="G32" s="25"/>
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
       <c r="J32" s="35"/>
       <c r="K32" s="25"/>
-      <c r="L32" s="82"/>
-      <c r="M32" s="82"/>
-      <c r="N32" s="57"/>
+      <c r="L32" s="81"/>
+      <c r="M32" s="81"/>
+      <c r="N32" s="56"/>
       <c r="O32" s="51"/>
       <c r="P32" s="26"/>
-      <c r="Q32" s="86"/>
-      <c r="R32" s="60"/>
+      <c r="Q32" s="85"/>
+      <c r="R32" s="59"/>
       <c r="S32" s="27"/>
       <c r="T32" s="26"/>
       <c r="U32" s="26"/>
@@ -3593,8 +3579,8 @@
       <c r="AD32" s="35"/>
       <c r="AE32" s="25"/>
       <c r="AF32" s="26"/>
-      <c r="AG32" s="60"/>
-      <c r="AH32" s="60"/>
+      <c r="AG32" s="59"/>
+      <c r="AH32" s="59"/>
       <c r="AI32" s="25"/>
       <c r="AJ32" s="26"/>
       <c r="AK32" s="26"/>
@@ -3609,24 +3595,24 @@
       <c r="AT32" s="35"/>
     </row>
     <row r="33" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="107"/>
-      <c r="B33" s="108"/>
-      <c r="C33" s="111"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="131"/>
-      <c r="F33" s="132"/>
+      <c r="A33" s="106"/>
+      <c r="B33" s="107"/>
+      <c r="C33" s="110"/>
+      <c r="D33" s="111"/>
+      <c r="E33" s="114"/>
+      <c r="F33" s="115"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
       <c r="J33" s="35"/>
       <c r="K33" s="25"/>
-      <c r="L33" s="82"/>
-      <c r="M33" s="82"/>
-      <c r="N33" s="71"/>
+      <c r="L33" s="81"/>
+      <c r="M33" s="81"/>
+      <c r="N33" s="70"/>
       <c r="O33" s="27"/>
       <c r="P33" s="26"/>
-      <c r="Q33" s="86"/>
-      <c r="R33" s="60"/>
+      <c r="Q33" s="85"/>
+      <c r="R33" s="59"/>
       <c r="S33" s="27"/>
       <c r="T33" s="26"/>
       <c r="U33" s="26"/>
@@ -3641,8 +3627,8 @@
       <c r="AD33" s="35"/>
       <c r="AE33" s="25"/>
       <c r="AF33" s="26"/>
-      <c r="AG33" s="60"/>
-      <c r="AH33" s="60"/>
+      <c r="AG33" s="59"/>
+      <c r="AH33" s="59"/>
       <c r="AI33" s="25"/>
       <c r="AJ33" s="26"/>
       <c r="AK33" s="26"/>
@@ -3657,30 +3643,30 @@
       <c r="AT33" s="35"/>
     </row>
     <row r="34" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="105" t="s">
+      <c r="A34" s="104" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="106"/>
-      <c r="C34" s="109">
+      <c r="B34" s="105"/>
+      <c r="C34" s="108">
         <v>2</v>
       </c>
-      <c r="D34" s="110"/>
-      <c r="E34" s="109">
+      <c r="D34" s="109"/>
+      <c r="E34" s="108">
         <v>2</v>
       </c>
-      <c r="F34" s="110"/>
+      <c r="F34" s="109"/>
       <c r="G34" s="25"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
       <c r="J34" s="35"/>
       <c r="K34" s="25"/>
       <c r="L34" s="26"/>
-      <c r="M34" s="82"/>
-      <c r="N34" s="55"/>
-      <c r="O34" s="87"/>
-      <c r="P34" s="88"/>
-      <c r="Q34" s="86"/>
-      <c r="R34" s="60"/>
+      <c r="M34" s="81"/>
+      <c r="N34" s="54"/>
+      <c r="O34" s="86"/>
+      <c r="P34" s="87"/>
+      <c r="Q34" s="85"/>
+      <c r="R34" s="59"/>
       <c r="S34" s="27"/>
       <c r="T34" s="26"/>
       <c r="U34" s="26"/>
@@ -3695,8 +3681,8 @@
       <c r="AD34" s="35"/>
       <c r="AE34" s="25"/>
       <c r="AF34" s="26"/>
-      <c r="AG34" s="60"/>
-      <c r="AH34" s="60"/>
+      <c r="AG34" s="59"/>
+      <c r="AH34" s="59"/>
       <c r="AI34" s="25"/>
       <c r="AJ34" s="26"/>
       <c r="AK34" s="26"/>
@@ -3711,24 +3697,24 @@
       <c r="AT34" s="35"/>
     </row>
     <row r="35" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="107"/>
-      <c r="B35" s="108"/>
-      <c r="C35" s="111"/>
-      <c r="D35" s="112"/>
-      <c r="E35" s="111"/>
-      <c r="F35" s="112"/>
+      <c r="A35" s="106"/>
+      <c r="B35" s="107"/>
+      <c r="C35" s="110"/>
+      <c r="D35" s="111"/>
+      <c r="E35" s="110"/>
+      <c r="F35" s="111"/>
       <c r="G35" s="25"/>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
       <c r="J35" s="35"/>
       <c r="K35" s="25"/>
       <c r="L35" s="26"/>
-      <c r="M35" s="82"/>
-      <c r="N35" s="55"/>
-      <c r="O35" s="74"/>
+      <c r="M35" s="81"/>
+      <c r="N35" s="54"/>
+      <c r="O35" s="73"/>
       <c r="P35" s="26"/>
-      <c r="Q35" s="86"/>
-      <c r="R35" s="60"/>
+      <c r="Q35" s="85"/>
+      <c r="R35" s="59"/>
       <c r="S35" s="27"/>
       <c r="T35" s="26"/>
       <c r="U35" s="26"/>
@@ -3743,8 +3729,8 @@
       <c r="AD35" s="35"/>
       <c r="AE35" s="25"/>
       <c r="AF35" s="26"/>
-      <c r="AG35" s="60"/>
-      <c r="AH35" s="60"/>
+      <c r="AG35" s="59"/>
+      <c r="AH35" s="59"/>
       <c r="AI35" s="25"/>
       <c r="AJ35" s="26"/>
       <c r="AK35" s="26"/>
@@ -3759,18 +3745,18 @@
       <c r="AT35" s="35"/>
     </row>
     <row r="36" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="105" t="s">
+      <c r="A36" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="106"/>
-      <c r="C36" s="109">
+      <c r="B36" s="105"/>
+      <c r="C36" s="108">
         <v>2</v>
       </c>
-      <c r="D36" s="110"/>
-      <c r="E36" s="109">
+      <c r="D36" s="109"/>
+      <c r="E36" s="108">
         <v>2</v>
       </c>
-      <c r="F36" s="110"/>
+      <c r="F36" s="109"/>
       <c r="G36" s="25"/>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3778,11 +3764,11 @@
       <c r="K36" s="25"/>
       <c r="L36" s="26"/>
       <c r="M36" s="26"/>
-      <c r="N36" s="55"/>
+      <c r="N36" s="54"/>
       <c r="O36" s="27"/>
-      <c r="P36" s="82"/>
-      <c r="Q36" s="89"/>
-      <c r="R36" s="60"/>
+      <c r="P36" s="81"/>
+      <c r="Q36" s="88"/>
+      <c r="R36" s="59"/>
       <c r="S36" s="27"/>
       <c r="T36" s="26"/>
       <c r="U36" s="26"/>
@@ -3797,8 +3783,8 @@
       <c r="AD36" s="35"/>
       <c r="AE36" s="25"/>
       <c r="AF36" s="26"/>
-      <c r="AG36" s="60"/>
-      <c r="AH36" s="60"/>
+      <c r="AG36" s="59"/>
+      <c r="AH36" s="59"/>
       <c r="AI36" s="25"/>
       <c r="AJ36" s="26"/>
       <c r="AK36" s="26"/>
@@ -3813,12 +3799,12 @@
       <c r="AT36" s="35"/>
     </row>
     <row r="37" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A37" s="107"/>
-      <c r="B37" s="108"/>
-      <c r="C37" s="111"/>
-      <c r="D37" s="112"/>
-      <c r="E37" s="111"/>
-      <c r="F37" s="112"/>
+      <c r="A37" s="106"/>
+      <c r="B37" s="107"/>
+      <c r="C37" s="110"/>
+      <c r="D37" s="111"/>
+      <c r="E37" s="110"/>
+      <c r="F37" s="111"/>
       <c r="G37" s="25"/>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3826,11 +3812,11 @@
       <c r="K37" s="25"/>
       <c r="L37" s="26"/>
       <c r="M37" s="26"/>
-      <c r="N37" s="55"/>
-      <c r="O37" s="87"/>
-      <c r="P37" s="56"/>
-      <c r="Q37" s="90"/>
-      <c r="R37" s="60"/>
+      <c r="N37" s="54"/>
+      <c r="O37" s="86"/>
+      <c r="P37" s="55"/>
+      <c r="Q37" s="89"/>
+      <c r="R37" s="59"/>
       <c r="S37" s="27"/>
       <c r="T37" s="26"/>
       <c r="U37" s="26"/>
@@ -3845,8 +3831,8 @@
       <c r="AD37" s="35"/>
       <c r="AE37" s="25"/>
       <c r="AF37" s="26"/>
-      <c r="AG37" s="60"/>
-      <c r="AH37" s="60"/>
+      <c r="AG37" s="59"/>
+      <c r="AH37" s="59"/>
       <c r="AI37" s="25"/>
       <c r="AJ37" s="26"/>
       <c r="AK37" s="26"/>
@@ -3861,18 +3847,18 @@
       <c r="AT37" s="35"/>
     </row>
     <row r="38" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="117" t="s">
+      <c r="A38" s="124" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="110"/>
-      <c r="C38" s="109">
+      <c r="B38" s="109"/>
+      <c r="C38" s="108">
         <v>2</v>
       </c>
-      <c r="D38" s="110"/>
-      <c r="E38" s="109">
+      <c r="D38" s="109"/>
+      <c r="E38" s="108">
         <v>2</v>
       </c>
-      <c r="F38" s="110"/>
+      <c r="F38" s="109"/>
       <c r="G38" s="25"/>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3880,11 +3866,11 @@
       <c r="K38" s="25"/>
       <c r="L38" s="26"/>
       <c r="M38" s="26"/>
-      <c r="N38" s="54"/>
-      <c r="O38" s="87"/>
-      <c r="P38" s="82"/>
-      <c r="Q38" s="91"/>
-      <c r="R38" s="60"/>
+      <c r="N38" s="53"/>
+      <c r="O38" s="86"/>
+      <c r="P38" s="81"/>
+      <c r="Q38" s="90"/>
+      <c r="R38" s="59"/>
       <c r="S38" s="51"/>
       <c r="T38" s="26"/>
       <c r="U38" s="26"/>
@@ -3899,8 +3885,8 @@
       <c r="AD38" s="35"/>
       <c r="AE38" s="25"/>
       <c r="AF38" s="26"/>
-      <c r="AG38" s="60"/>
-      <c r="AH38" s="60"/>
+      <c r="AG38" s="59"/>
+      <c r="AH38" s="59"/>
       <c r="AI38" s="25"/>
       <c r="AJ38" s="26"/>
       <c r="AK38" s="26"/>
@@ -3915,12 +3901,12 @@
       <c r="AT38" s="35"/>
     </row>
     <row r="39" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="118"/>
-      <c r="B39" s="112"/>
-      <c r="C39" s="111"/>
-      <c r="D39" s="112"/>
-      <c r="E39" s="111"/>
-      <c r="F39" s="112"/>
+      <c r="A39" s="152"/>
+      <c r="B39" s="111"/>
+      <c r="C39" s="110"/>
+      <c r="D39" s="111"/>
+      <c r="E39" s="110"/>
+      <c r="F39" s="111"/>
       <c r="G39" s="25"/>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3928,14 +3914,14 @@
       <c r="K39" s="25"/>
       <c r="L39" s="26"/>
       <c r="M39" s="26"/>
-      <c r="N39" s="57"/>
-      <c r="O39" s="87"/>
-      <c r="P39" s="82"/>
-      <c r="Q39" s="86"/>
-      <c r="R39" s="60"/>
-      <c r="S39" s="74"/>
-      <c r="T39" s="56"/>
-      <c r="U39" s="56"/>
+      <c r="N39" s="56"/>
+      <c r="O39" s="86"/>
+      <c r="P39" s="81"/>
+      <c r="Q39" s="85"/>
+      <c r="R39" s="59"/>
+      <c r="S39" s="73"/>
+      <c r="T39" s="55"/>
+      <c r="U39" s="55"/>
       <c r="V39" s="35"/>
       <c r="W39" s="25"/>
       <c r="X39" s="26"/>
@@ -3947,8 +3933,8 @@
       <c r="AD39" s="35"/>
       <c r="AE39" s="25"/>
       <c r="AF39" s="26"/>
-      <c r="AG39" s="60"/>
-      <c r="AH39" s="60"/>
+      <c r="AG39" s="59"/>
+      <c r="AH39" s="59"/>
       <c r="AI39" s="25"/>
       <c r="AJ39" s="26"/>
       <c r="AK39" s="26"/>
@@ -3963,18 +3949,18 @@
       <c r="AT39" s="35"/>
     </row>
     <row r="40" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A40" s="105" t="s">
+      <c r="A40" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="106"/>
-      <c r="C40" s="109">
+      <c r="B40" s="105"/>
+      <c r="C40" s="108">
         <v>2</v>
       </c>
-      <c r="D40" s="110"/>
-      <c r="E40" s="109">
+      <c r="D40" s="109"/>
+      <c r="E40" s="108">
         <v>2</v>
       </c>
-      <c r="F40" s="110"/>
+      <c r="F40" s="109"/>
       <c r="G40" s="25"/>
       <c r="H40" s="26"/>
       <c r="I40" s="26"/>
@@ -3984,11 +3970,11 @@
       <c r="M40" s="26"/>
       <c r="N40" s="26"/>
       <c r="O40" s="25"/>
-      <c r="P40" s="82"/>
-      <c r="Q40" s="91"/>
-      <c r="R40" s="60"/>
-      <c r="S40" s="93"/>
-      <c r="T40" s="64" t="s">
+      <c r="P40" s="81"/>
+      <c r="Q40" s="90"/>
+      <c r="R40" s="59"/>
+      <c r="S40" s="92"/>
+      <c r="T40" s="63" t="s">
         <v>33</v>
       </c>
       <c r="U40" s="26"/>
@@ -4003,8 +3989,8 @@
       <c r="AD40" s="35"/>
       <c r="AE40" s="25"/>
       <c r="AF40" s="26"/>
-      <c r="AG40" s="60"/>
-      <c r="AH40" s="60"/>
+      <c r="AG40" s="59"/>
+      <c r="AH40" s="59"/>
       <c r="AI40" s="25"/>
       <c r="AJ40" s="26"/>
       <c r="AK40" s="26"/>
@@ -4019,12 +4005,12 @@
       <c r="AT40" s="35"/>
     </row>
     <row r="41" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="107"/>
-      <c r="B41" s="108"/>
-      <c r="C41" s="111"/>
-      <c r="D41" s="112"/>
-      <c r="E41" s="111"/>
-      <c r="F41" s="112"/>
+      <c r="A41" s="106"/>
+      <c r="B41" s="107"/>
+      <c r="C41" s="110"/>
+      <c r="D41" s="111"/>
+      <c r="E41" s="110"/>
+      <c r="F41" s="111"/>
       <c r="G41" s="25"/>
       <c r="H41" s="26"/>
       <c r="I41" s="26"/>
@@ -4035,24 +4021,26 @@
       <c r="N41" s="35"/>
       <c r="O41" s="25"/>
       <c r="P41" s="26"/>
-      <c r="Q41" s="91"/>
-      <c r="R41" s="60"/>
-      <c r="S41" s="94"/>
+      <c r="Q41" s="90"/>
+      <c r="R41" s="59"/>
+      <c r="S41" s="93"/>
       <c r="T41" s="26"/>
-      <c r="U41" s="56"/>
-      <c r="V41" s="103"/>
-      <c r="W41" s="104"/>
-      <c r="X41" s="56"/>
-      <c r="Y41" s="56"/>
-      <c r="Z41" s="103"/>
+      <c r="U41" s="55"/>
+      <c r="V41" s="102"/>
+      <c r="W41" s="103"/>
+      <c r="X41" s="55"/>
+      <c r="Y41" s="55"/>
+      <c r="Z41" s="102" t="s">
+        <v>33</v>
+      </c>
       <c r="AA41" s="25"/>
       <c r="AB41" s="26"/>
       <c r="AC41" s="26"/>
       <c r="AD41" s="35"/>
       <c r="AE41" s="25"/>
-      <c r="AF41" s="86"/>
-      <c r="AG41" s="60"/>
-      <c r="AH41" s="60"/>
+      <c r="AF41" s="85"/>
+      <c r="AG41" s="59"/>
+      <c r="AH41" s="59"/>
       <c r="AI41" s="25"/>
       <c r="AJ41" s="26"/>
       <c r="AK41" s="26"/>
@@ -4067,20 +4055,20 @@
       <c r="AT41" s="35"/>
     </row>
     <row r="42" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="113" t="s">
+      <c r="A42" s="146" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="114"/>
-      <c r="C42" s="115">
+      <c r="B42" s="147"/>
+      <c r="C42" s="148">
         <f>SUM(C43:C45)</f>
         <v>3</v>
       </c>
-      <c r="D42" s="116"/>
-      <c r="E42" s="115">
+      <c r="D42" s="149"/>
+      <c r="E42" s="148">
         <f>SUM(E45+E43)</f>
         <v>3</v>
       </c>
-      <c r="F42" s="116"/>
+      <c r="F42" s="149"/>
       <c r="G42" s="31"/>
       <c r="H42" s="32"/>
       <c r="I42" s="32"/>
@@ -4091,9 +4079,9 @@
       <c r="N42" s="33"/>
       <c r="O42" s="31"/>
       <c r="P42" s="32"/>
-      <c r="Q42" s="92"/>
-      <c r="R42" s="61"/>
-      <c r="S42" s="95"/>
+      <c r="Q42" s="91"/>
+      <c r="R42" s="60"/>
+      <c r="S42" s="94"/>
       <c r="T42" s="32"/>
       <c r="U42" s="32"/>
       <c r="V42" s="33"/>
@@ -4106,9 +4094,9 @@
       <c r="AC42" s="32"/>
       <c r="AD42" s="33"/>
       <c r="AE42" s="31"/>
-      <c r="AF42" s="92"/>
-      <c r="AG42" s="61"/>
-      <c r="AH42" s="61"/>
+      <c r="AF42" s="91"/>
+      <c r="AG42" s="60"/>
+      <c r="AH42" s="60"/>
       <c r="AI42" s="31"/>
       <c r="AJ42" s="32"/>
       <c r="AK42" s="32"/>
@@ -4123,120 +4111,120 @@
       <c r="AT42" s="33"/>
     </row>
     <row r="43" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="140" t="s">
+      <c r="A43" s="154" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="141"/>
-      <c r="C43" s="140">
+      <c r="B43" s="155"/>
+      <c r="C43" s="154">
         <v>2</v>
       </c>
-      <c r="D43" s="144"/>
-      <c r="E43" s="140">
+      <c r="D43" s="158"/>
+      <c r="E43" s="154">
         <v>2</v>
       </c>
-      <c r="F43" s="144"/>
-      <c r="G43" s="85"/>
-      <c r="H43" s="82"/>
-      <c r="I43" s="82"/>
-      <c r="J43" s="55"/>
-      <c r="K43" s="87"/>
-      <c r="L43" s="82"/>
-      <c r="M43" s="82"/>
-      <c r="N43" s="55"/>
-      <c r="O43" s="87"/>
-      <c r="P43" s="82"/>
-      <c r="Q43" s="91"/>
-      <c r="R43" s="59"/>
-      <c r="S43" s="93"/>
-      <c r="T43" s="82"/>
-      <c r="U43" s="88"/>
-      <c r="V43" s="55"/>
-      <c r="W43" s="87"/>
-      <c r="X43" s="82"/>
-      <c r="Y43" s="82"/>
-      <c r="Z43" s="55"/>
-      <c r="AA43" s="87"/>
-      <c r="AB43" s="82"/>
-      <c r="AC43" s="82"/>
-      <c r="AD43" s="55"/>
-      <c r="AE43" s="87"/>
-      <c r="AF43" s="91"/>
-      <c r="AG43" s="59"/>
-      <c r="AH43" s="59"/>
-      <c r="AI43" s="87"/>
-      <c r="AJ43" s="82"/>
-      <c r="AK43" s="82"/>
-      <c r="AL43" s="55"/>
-      <c r="AM43" s="87"/>
-      <c r="AN43" s="82"/>
-      <c r="AO43" s="82"/>
-      <c r="AP43" s="55"/>
-      <c r="AQ43" s="87"/>
-      <c r="AR43" s="82"/>
-      <c r="AS43" s="82"/>
-      <c r="AT43" s="55"/>
+      <c r="F43" s="158"/>
+      <c r="G43" s="84"/>
+      <c r="H43" s="81"/>
+      <c r="I43" s="81"/>
+      <c r="J43" s="54"/>
+      <c r="K43" s="86"/>
+      <c r="L43" s="81"/>
+      <c r="M43" s="81"/>
+      <c r="N43" s="54"/>
+      <c r="O43" s="86"/>
+      <c r="P43" s="81"/>
+      <c r="Q43" s="90"/>
+      <c r="R43" s="58"/>
+      <c r="S43" s="92"/>
+      <c r="T43" s="81"/>
+      <c r="U43" s="87"/>
+      <c r="V43" s="54"/>
+      <c r="W43" s="86"/>
+      <c r="X43" s="81"/>
+      <c r="Y43" s="81"/>
+      <c r="Z43" s="54"/>
+      <c r="AA43" s="86"/>
+      <c r="AB43" s="81"/>
+      <c r="AC43" s="81"/>
+      <c r="AD43" s="54"/>
+      <c r="AE43" s="86"/>
+      <c r="AF43" s="90"/>
+      <c r="AG43" s="58"/>
+      <c r="AH43" s="58"/>
+      <c r="AI43" s="86"/>
+      <c r="AJ43" s="81"/>
+      <c r="AK43" s="81"/>
+      <c r="AL43" s="54"/>
+      <c r="AM43" s="86"/>
+      <c r="AN43" s="81"/>
+      <c r="AO43" s="81"/>
+      <c r="AP43" s="54"/>
+      <c r="AQ43" s="86"/>
+      <c r="AR43" s="81"/>
+      <c r="AS43" s="81"/>
+      <c r="AT43" s="54"/>
     </row>
     <row r="44" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="142"/>
-      <c r="B44" s="143"/>
-      <c r="C44" s="145"/>
-      <c r="D44" s="146"/>
-      <c r="E44" s="145"/>
-      <c r="F44" s="146"/>
-      <c r="G44" s="85"/>
-      <c r="H44" s="82"/>
-      <c r="I44" s="82"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="87"/>
-      <c r="L44" s="82"/>
-      <c r="M44" s="82"/>
-      <c r="N44" s="55"/>
-      <c r="O44" s="87"/>
-      <c r="P44" s="82"/>
-      <c r="Q44" s="91"/>
-      <c r="R44" s="59"/>
-      <c r="S44" s="93"/>
-      <c r="T44" s="82"/>
-      <c r="U44" s="82"/>
-      <c r="V44" s="55"/>
-      <c r="W44" s="87"/>
-      <c r="X44" s="82"/>
-      <c r="Y44" s="82"/>
-      <c r="Z44" s="55"/>
-      <c r="AA44" s="87"/>
-      <c r="AB44" s="82"/>
-      <c r="AC44" s="82"/>
-      <c r="AD44" s="55"/>
-      <c r="AE44" s="87"/>
-      <c r="AF44" s="91"/>
-      <c r="AG44" s="59"/>
-      <c r="AH44" s="59"/>
-      <c r="AI44" s="87"/>
-      <c r="AJ44" s="82"/>
-      <c r="AK44" s="82"/>
-      <c r="AL44" s="55"/>
-      <c r="AM44" s="87"/>
-      <c r="AN44" s="82"/>
-      <c r="AO44" s="82"/>
-      <c r="AP44" s="55"/>
-      <c r="AQ44" s="87"/>
-      <c r="AR44" s="82"/>
-      <c r="AS44" s="82"/>
-      <c r="AT44" s="55"/>
+      <c r="A44" s="156"/>
+      <c r="B44" s="157"/>
+      <c r="C44" s="159"/>
+      <c r="D44" s="160"/>
+      <c r="E44" s="159"/>
+      <c r="F44" s="160"/>
+      <c r="G44" s="84"/>
+      <c r="H44" s="81"/>
+      <c r="I44" s="81"/>
+      <c r="J44" s="54"/>
+      <c r="K44" s="86"/>
+      <c r="L44" s="81"/>
+      <c r="M44" s="81"/>
+      <c r="N44" s="54"/>
+      <c r="O44" s="86"/>
+      <c r="P44" s="81"/>
+      <c r="Q44" s="90"/>
+      <c r="R44" s="58"/>
+      <c r="S44" s="92"/>
+      <c r="T44" s="81"/>
+      <c r="U44" s="81"/>
+      <c r="V44" s="54"/>
+      <c r="W44" s="86"/>
+      <c r="X44" s="81"/>
+      <c r="Y44" s="81"/>
+      <c r="Z44" s="54"/>
+      <c r="AA44" s="101"/>
+      <c r="AB44" s="81"/>
+      <c r="AC44" s="81"/>
+      <c r="AD44" s="54"/>
+      <c r="AE44" s="86"/>
+      <c r="AF44" s="90"/>
+      <c r="AG44" s="58"/>
+      <c r="AH44" s="58"/>
+      <c r="AI44" s="86"/>
+      <c r="AJ44" s="81"/>
+      <c r="AK44" s="81"/>
+      <c r="AL44" s="54"/>
+      <c r="AM44" s="86"/>
+      <c r="AN44" s="81"/>
+      <c r="AO44" s="81"/>
+      <c r="AP44" s="54"/>
+      <c r="AQ44" s="86"/>
+      <c r="AR44" s="81"/>
+      <c r="AS44" s="81"/>
+      <c r="AT44" s="54"/>
     </row>
     <row r="45" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="117" t="s">
+      <c r="A45" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="B45" s="137"/>
-      <c r="C45" s="109">
+      <c r="B45" s="129"/>
+      <c r="C45" s="108">
         <v>1</v>
       </c>
-      <c r="D45" s="110"/>
-      <c r="E45" s="109">
+      <c r="D45" s="109"/>
+      <c r="E45" s="108">
         <v>1</v>
       </c>
-      <c r="F45" s="110"/>
+      <c r="F45" s="109"/>
       <c r="G45" s="25"/>
       <c r="H45" s="26"/>
       <c r="I45" s="26"/>
@@ -4247,12 +4235,12 @@
       <c r="N45" s="35"/>
       <c r="O45" s="25"/>
       <c r="P45" s="26"/>
-      <c r="Q45" s="86"/>
-      <c r="R45" s="59"/>
-      <c r="S45" s="93"/>
+      <c r="Q45" s="85"/>
+      <c r="R45" s="58"/>
+      <c r="S45" s="92"/>
       <c r="T45" s="26"/>
-      <c r="U45" s="82"/>
-      <c r="V45" s="96" t="s">
+      <c r="U45" s="81"/>
+      <c r="V45" s="95" t="s">
         <v>35</v>
       </c>
       <c r="W45" s="25"/>
@@ -4264,9 +4252,9 @@
       <c r="AC45" s="26"/>
       <c r="AD45" s="35"/>
       <c r="AE45" s="25"/>
-      <c r="AF45" s="86"/>
-      <c r="AG45" s="60"/>
-      <c r="AH45" s="60"/>
+      <c r="AF45" s="85"/>
+      <c r="AG45" s="59"/>
+      <c r="AH45" s="59"/>
       <c r="AI45" s="25"/>
       <c r="AJ45" s="26"/>
       <c r="AK45" s="26"/>
@@ -4281,12 +4269,12 @@
       <c r="AT45" s="35"/>
     </row>
     <row r="46" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="138"/>
-      <c r="B46" s="139"/>
-      <c r="C46" s="111"/>
-      <c r="D46" s="112"/>
-      <c r="E46" s="111"/>
-      <c r="F46" s="112"/>
+      <c r="A46" s="153"/>
+      <c r="B46" s="131"/>
+      <c r="C46" s="110"/>
+      <c r="D46" s="111"/>
+      <c r="E46" s="110"/>
+      <c r="F46" s="111"/>
       <c r="G46" s="25"/>
       <c r="H46" s="26"/>
       <c r="I46" s="26"/>
@@ -4297,9 +4285,9 @@
       <c r="N46" s="35"/>
       <c r="O46" s="25"/>
       <c r="P46" s="26"/>
-      <c r="Q46" s="86"/>
-      <c r="R46" s="59"/>
-      <c r="S46" s="94"/>
+      <c r="Q46" s="85"/>
+      <c r="R46" s="58"/>
+      <c r="S46" s="93"/>
       <c r="T46" s="26"/>
       <c r="U46" s="26"/>
       <c r="V46" s="35"/>
@@ -4307,14 +4295,16 @@
       <c r="X46" s="26"/>
       <c r="Y46" s="26"/>
       <c r="Z46" s="35"/>
-      <c r="AA46" s="25"/>
+      <c r="AA46" s="103" t="s">
+        <v>35</v>
+      </c>
       <c r="AB46" s="26"/>
       <c r="AC46" s="26"/>
       <c r="AD46" s="35"/>
       <c r="AE46" s="25"/>
-      <c r="AF46" s="86"/>
-      <c r="AG46" s="60"/>
-      <c r="AH46" s="60"/>
+      <c r="AF46" s="85"/>
+      <c r="AG46" s="59"/>
+      <c r="AH46" s="59"/>
       <c r="AI46" s="25"/>
       <c r="AJ46" s="26"/>
       <c r="AK46" s="26"/>
@@ -4329,20 +4319,20 @@
       <c r="AT46" s="35"/>
     </row>
     <row r="47" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="113" t="s">
+      <c r="A47" s="146" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="114"/>
-      <c r="C47" s="115">
+      <c r="B47" s="147"/>
+      <c r="C47" s="148">
         <f>SUM(C48:D63)</f>
         <v>19</v>
       </c>
-      <c r="D47" s="116"/>
-      <c r="E47" s="115">
+      <c r="D47" s="149"/>
+      <c r="E47" s="148">
         <f>SUM(E48:F63)</f>
         <v>19</v>
       </c>
-      <c r="F47" s="116"/>
+      <c r="F47" s="149"/>
       <c r="G47" s="31"/>
       <c r="H47" s="32"/>
       <c r="I47" s="32"/>
@@ -4354,8 +4344,8 @@
       <c r="O47" s="31"/>
       <c r="P47" s="32"/>
       <c r="Q47" s="32"/>
-      <c r="R47" s="61"/>
-      <c r="S47" s="95"/>
+      <c r="R47" s="60"/>
+      <c r="S47" s="94"/>
       <c r="T47" s="32"/>
       <c r="U47" s="32"/>
       <c r="V47" s="33"/>
@@ -4368,9 +4358,9 @@
       <c r="AC47" s="32"/>
       <c r="AD47" s="33"/>
       <c r="AE47" s="31"/>
-      <c r="AF47" s="92"/>
-      <c r="AG47" s="61"/>
-      <c r="AH47" s="61"/>
+      <c r="AF47" s="91"/>
+      <c r="AG47" s="60"/>
+      <c r="AH47" s="60"/>
       <c r="AI47" s="31"/>
       <c r="AJ47" s="32"/>
       <c r="AK47" s="32"/>
@@ -4385,18 +4375,18 @@
       <c r="AT47" s="33"/>
     </row>
     <row r="48" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="133" t="s">
+      <c r="A48" s="161" t="s">
         <v>74</v>
       </c>
-      <c r="B48" s="134"/>
-      <c r="C48" s="109">
+      <c r="B48" s="162"/>
+      <c r="C48" s="108">
         <v>0.5</v>
       </c>
-      <c r="D48" s="110"/>
-      <c r="E48" s="109">
+      <c r="D48" s="109"/>
+      <c r="E48" s="108">
         <v>0.5</v>
       </c>
-      <c r="F48" s="110"/>
+      <c r="F48" s="109"/>
       <c r="G48" s="25"/>
       <c r="H48" s="26"/>
       <c r="I48" s="26"/>
@@ -4408,12 +4398,12 @@
       <c r="O48" s="25"/>
       <c r="P48" s="26"/>
       <c r="Q48" s="26"/>
-      <c r="R48" s="59"/>
-      <c r="S48" s="93"/>
+      <c r="R48" s="58"/>
+      <c r="S48" s="92"/>
       <c r="T48" s="26"/>
-      <c r="U48" s="82"/>
-      <c r="V48" s="97"/>
-      <c r="W48" s="87"/>
+      <c r="U48" s="81"/>
+      <c r="V48" s="96"/>
+      <c r="W48" s="86"/>
       <c r="X48" s="26"/>
       <c r="Y48" s="26"/>
       <c r="Z48" s="35"/>
@@ -4422,9 +4412,9 @@
       <c r="AC48" s="26"/>
       <c r="AD48" s="35"/>
       <c r="AE48" s="25"/>
-      <c r="AF48" s="86"/>
-      <c r="AG48" s="60"/>
-      <c r="AH48" s="60"/>
+      <c r="AF48" s="85"/>
+      <c r="AG48" s="59"/>
+      <c r="AH48" s="59"/>
       <c r="AI48" s="25"/>
       <c r="AJ48" s="26"/>
       <c r="AK48" s="26"/>
@@ -4439,12 +4429,12 @@
       <c r="AT48" s="35"/>
     </row>
     <row r="49" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="135"/>
-      <c r="B49" s="136"/>
-      <c r="C49" s="111"/>
-      <c r="D49" s="112"/>
-      <c r="E49" s="111"/>
-      <c r="F49" s="112"/>
+      <c r="A49" s="163"/>
+      <c r="B49" s="164"/>
+      <c r="C49" s="110"/>
+      <c r="D49" s="111"/>
+      <c r="E49" s="110"/>
+      <c r="F49" s="111"/>
       <c r="G49" s="25"/>
       <c r="H49" s="26"/>
       <c r="I49" s="26"/>
@@ -4456,23 +4446,23 @@
       <c r="O49" s="25"/>
       <c r="P49" s="26"/>
       <c r="Q49" s="26"/>
-      <c r="R49" s="60"/>
-      <c r="S49" s="93"/>
+      <c r="R49" s="59"/>
+      <c r="S49" s="92"/>
       <c r="T49" s="26"/>
       <c r="U49" s="26"/>
-      <c r="V49" s="57"/>
+      <c r="V49" s="56"/>
       <c r="W49" s="27"/>
       <c r="X49" s="26"/>
       <c r="Y49" s="26"/>
       <c r="Z49" s="35"/>
-      <c r="AA49" s="25"/>
+      <c r="AA49" s="103"/>
       <c r="AB49" s="26"/>
       <c r="AC49" s="26"/>
       <c r="AD49" s="35"/>
       <c r="AE49" s="25"/>
-      <c r="AF49" s="86"/>
-      <c r="AG49" s="60"/>
-      <c r="AH49" s="60"/>
+      <c r="AF49" s="85"/>
+      <c r="AG49" s="59"/>
+      <c r="AH49" s="59"/>
       <c r="AI49" s="25"/>
       <c r="AJ49" s="26"/>
       <c r="AK49" s="26"/>
@@ -4487,18 +4477,18 @@
       <c r="AT49" s="35"/>
     </row>
     <row r="50" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A50" s="117" t="s">
+      <c r="A50" s="124" t="s">
         <v>75</v>
       </c>
-      <c r="B50" s="110"/>
-      <c r="C50" s="109">
+      <c r="B50" s="109"/>
+      <c r="C50" s="108">
         <v>0.5</v>
       </c>
-      <c r="D50" s="110"/>
-      <c r="E50" s="129">
+      <c r="D50" s="109"/>
+      <c r="E50" s="112">
         <v>0.5</v>
       </c>
-      <c r="F50" s="130"/>
+      <c r="F50" s="113"/>
       <c r="G50" s="25"/>
       <c r="H50" s="26"/>
       <c r="I50" s="26"/>
@@ -4510,12 +4500,12 @@
       <c r="O50" s="25"/>
       <c r="P50" s="26"/>
       <c r="Q50" s="26"/>
-      <c r="R50" s="60"/>
-      <c r="S50" s="93"/>
-      <c r="T50" s="82"/>
+      <c r="R50" s="59"/>
+      <c r="S50" s="92"/>
+      <c r="T50" s="81"/>
       <c r="U50" s="26"/>
-      <c r="V50" s="97"/>
-      <c r="W50" s="87"/>
+      <c r="V50" s="96"/>
+      <c r="W50" s="86"/>
       <c r="X50" s="26"/>
       <c r="Y50" s="26"/>
       <c r="Z50" s="35"/>
@@ -4524,9 +4514,9 @@
       <c r="AC50" s="26"/>
       <c r="AD50" s="35"/>
       <c r="AE50" s="25"/>
-      <c r="AF50" s="86"/>
-      <c r="AG50" s="60"/>
-      <c r="AH50" s="60"/>
+      <c r="AF50" s="85"/>
+      <c r="AG50" s="59"/>
+      <c r="AH50" s="59"/>
       <c r="AI50" s="25"/>
       <c r="AJ50" s="26"/>
       <c r="AK50" s="26"/>
@@ -4541,12 +4531,12 @@
       <c r="AT50" s="35"/>
     </row>
     <row r="51" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="118"/>
-      <c r="B51" s="112"/>
-      <c r="C51" s="111"/>
-      <c r="D51" s="112"/>
-      <c r="E51" s="131"/>
-      <c r="F51" s="132"/>
+      <c r="A51" s="152"/>
+      <c r="B51" s="111"/>
+      <c r="C51" s="110"/>
+      <c r="D51" s="111"/>
+      <c r="E51" s="114"/>
+      <c r="F51" s="115"/>
       <c r="G51" s="25"/>
       <c r="H51" s="26"/>
       <c r="I51" s="26"/>
@@ -4558,23 +4548,23 @@
       <c r="O51" s="25"/>
       <c r="P51" s="26"/>
       <c r="Q51" s="26"/>
-      <c r="R51" s="60"/>
-      <c r="S51" s="94"/>
-      <c r="T51" s="82"/>
+      <c r="R51" s="59"/>
+      <c r="S51" s="93"/>
+      <c r="T51" s="81"/>
       <c r="U51" s="26"/>
-      <c r="V51" s="57"/>
+      <c r="V51" s="56"/>
       <c r="W51" s="27"/>
       <c r="X51" s="26"/>
       <c r="Y51" s="26"/>
       <c r="Z51" s="35"/>
       <c r="AA51" s="25"/>
-      <c r="AB51" s="26"/>
+      <c r="AB51" s="55"/>
       <c r="AC51" s="26"/>
       <c r="AD51" s="35"/>
       <c r="AE51" s="25"/>
-      <c r="AF51" s="86"/>
-      <c r="AG51" s="60"/>
-      <c r="AH51" s="60"/>
+      <c r="AF51" s="85"/>
+      <c r="AG51" s="59"/>
+      <c r="AH51" s="59"/>
       <c r="AI51" s="25"/>
       <c r="AJ51" s="26"/>
       <c r="AK51" s="26"/>
@@ -4589,18 +4579,18 @@
       <c r="AT51" s="35"/>
     </row>
     <row r="52" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A52" s="117" t="s">
+      <c r="A52" s="124" t="s">
         <v>76</v>
       </c>
-      <c r="B52" s="110"/>
-      <c r="C52" s="109">
+      <c r="B52" s="109"/>
+      <c r="C52" s="108">
         <v>2</v>
       </c>
-      <c r="D52" s="110"/>
-      <c r="E52" s="129">
+      <c r="D52" s="109"/>
+      <c r="E52" s="112">
         <v>2</v>
       </c>
-      <c r="F52" s="130"/>
+      <c r="F52" s="113"/>
       <c r="G52" s="25"/>
       <c r="H52" s="26"/>
       <c r="I52" s="26"/>
@@ -4612,23 +4602,23 @@
       <c r="O52" s="25"/>
       <c r="P52" s="26"/>
       <c r="Q52" s="26"/>
-      <c r="R52" s="60"/>
-      <c r="S52" s="94"/>
-      <c r="T52" s="82"/>
-      <c r="U52" s="82"/>
-      <c r="V52" s="55"/>
+      <c r="R52" s="59"/>
+      <c r="S52" s="93"/>
+      <c r="T52" s="81"/>
+      <c r="U52" s="81"/>
+      <c r="V52" s="54"/>
       <c r="W52" s="51"/>
-      <c r="X52" s="82"/>
-      <c r="Y52" s="82"/>
+      <c r="X52" s="81"/>
+      <c r="Y52" s="81"/>
       <c r="Z52" s="35"/>
       <c r="AA52" s="25"/>
       <c r="AB52" s="26"/>
       <c r="AC52" s="26"/>
       <c r="AD52" s="35"/>
       <c r="AE52" s="25"/>
-      <c r="AF52" s="86"/>
-      <c r="AG52" s="60"/>
-      <c r="AH52" s="60"/>
+      <c r="AF52" s="85"/>
+      <c r="AG52" s="59"/>
+      <c r="AH52" s="59"/>
       <c r="AI52" s="25"/>
       <c r="AJ52" s="26"/>
       <c r="AK52" s="26"/>
@@ -4643,12 +4633,12 @@
       <c r="AT52" s="35"/>
     </row>
     <row r="53" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="118"/>
-      <c r="B53" s="112"/>
-      <c r="C53" s="111"/>
-      <c r="D53" s="112"/>
-      <c r="E53" s="131"/>
-      <c r="F53" s="132"/>
+      <c r="A53" s="152"/>
+      <c r="B53" s="111"/>
+      <c r="C53" s="110"/>
+      <c r="D53" s="111"/>
+      <c r="E53" s="114"/>
+      <c r="F53" s="115"/>
       <c r="G53" s="25"/>
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
@@ -4660,23 +4650,23 @@
       <c r="O53" s="25"/>
       <c r="P53" s="26"/>
       <c r="Q53" s="26"/>
-      <c r="R53" s="60"/>
-      <c r="S53" s="94"/>
+      <c r="R53" s="59"/>
+      <c r="S53" s="93"/>
       <c r="T53" s="26"/>
-      <c r="U53" s="82"/>
-      <c r="V53" s="57"/>
+      <c r="U53" s="81"/>
+      <c r="V53" s="56"/>
       <c r="W53" s="27"/>
       <c r="X53" s="26"/>
       <c r="Y53" s="26"/>
       <c r="Z53" s="35"/>
       <c r="AA53" s="25"/>
-      <c r="AB53" s="26"/>
+      <c r="AB53" s="55"/>
       <c r="AC53" s="26"/>
       <c r="AD53" s="35"/>
       <c r="AE53" s="25"/>
-      <c r="AF53" s="86"/>
-      <c r="AG53" s="60"/>
-      <c r="AH53" s="60"/>
+      <c r="AF53" s="85"/>
+      <c r="AG53" s="59"/>
+      <c r="AH53" s="59"/>
       <c r="AI53" s="25"/>
       <c r="AJ53" s="26"/>
       <c r="AK53" s="26"/>
@@ -4691,18 +4681,18 @@
       <c r="AT53" s="35"/>
     </row>
     <row r="54" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="117" t="s">
+      <c r="A54" s="124" t="s">
         <v>78</v>
       </c>
-      <c r="B54" s="110"/>
-      <c r="C54" s="109">
+      <c r="B54" s="109"/>
+      <c r="C54" s="108">
         <v>2</v>
       </c>
-      <c r="D54" s="110"/>
-      <c r="E54" s="129">
+      <c r="D54" s="109"/>
+      <c r="E54" s="112">
         <v>2</v>
       </c>
-      <c r="F54" s="130"/>
+      <c r="F54" s="113"/>
       <c r="G54" s="25"/>
       <c r="H54" s="26"/>
       <c r="I54" s="26"/>
@@ -4714,23 +4704,23 @@
       <c r="O54" s="25"/>
       <c r="P54" s="26"/>
       <c r="Q54" s="26"/>
-      <c r="R54" s="60"/>
-      <c r="S54" s="94"/>
+      <c r="R54" s="59"/>
+      <c r="S54" s="93"/>
       <c r="T54" s="26"/>
       <c r="U54" s="26"/>
-      <c r="V54" s="53"/>
-      <c r="W54" s="87"/>
-      <c r="X54" s="88"/>
-      <c r="Y54" s="82"/>
-      <c r="Z54" s="55"/>
-      <c r="AA54" s="87"/>
-      <c r="AB54" s="82"/>
+      <c r="V54" s="54"/>
+      <c r="W54" s="86"/>
+      <c r="X54" s="87"/>
+      <c r="Y54" s="81"/>
+      <c r="Z54" s="54"/>
+      <c r="AA54" s="86"/>
+      <c r="AB54" s="81"/>
       <c r="AC54" s="26"/>
       <c r="AD54" s="35"/>
       <c r="AE54" s="25"/>
-      <c r="AF54" s="86"/>
-      <c r="AG54" s="60"/>
-      <c r="AH54" s="60"/>
+      <c r="AF54" s="85"/>
+      <c r="AG54" s="59"/>
+      <c r="AH54" s="59"/>
       <c r="AI54" s="25"/>
       <c r="AJ54" s="26"/>
       <c r="AK54" s="26"/>
@@ -4745,12 +4735,12 @@
       <c r="AT54" s="35"/>
     </row>
     <row r="55" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="118"/>
-      <c r="B55" s="112"/>
-      <c r="C55" s="111"/>
-      <c r="D55" s="112"/>
-      <c r="E55" s="131"/>
-      <c r="F55" s="132"/>
+      <c r="A55" s="152"/>
+      <c r="B55" s="111"/>
+      <c r="C55" s="110"/>
+      <c r="D55" s="111"/>
+      <c r="E55" s="114"/>
+      <c r="F55" s="115"/>
       <c r="G55" s="25"/>
       <c r="H55" s="26"/>
       <c r="I55" s="26"/>
@@ -4762,22 +4752,22 @@
       <c r="O55" s="25"/>
       <c r="P55" s="26"/>
       <c r="Q55" s="26"/>
-      <c r="R55" s="60"/>
+      <c r="R55" s="59"/>
       <c r="S55" s="27"/>
       <c r="T55" s="26"/>
       <c r="U55" s="26"/>
       <c r="W55" s="25"/>
       <c r="X55" s="26"/>
       <c r="Y55" s="26"/>
-      <c r="Z55" s="57"/>
+      <c r="Z55" s="56"/>
       <c r="AA55" s="27"/>
-      <c r="AB55" s="26"/>
+      <c r="AB55" s="55"/>
       <c r="AC55" s="26"/>
       <c r="AD55" s="35"/>
       <c r="AE55" s="25"/>
-      <c r="AF55" s="86"/>
-      <c r="AG55" s="60"/>
-      <c r="AH55" s="60"/>
+      <c r="AF55" s="85"/>
+      <c r="AG55" s="59"/>
+      <c r="AH55" s="59"/>
       <c r="AI55" s="25"/>
       <c r="AJ55" s="26"/>
       <c r="AK55" s="26"/>
@@ -4792,18 +4782,18 @@
       <c r="AT55" s="35"/>
     </row>
     <row r="56" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="105" t="s">
+      <c r="A56" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="B56" s="106"/>
-      <c r="C56" s="109">
+      <c r="B56" s="105"/>
+      <c r="C56" s="108">
         <v>2</v>
       </c>
-      <c r="D56" s="110"/>
-      <c r="E56" s="109">
+      <c r="D56" s="109"/>
+      <c r="E56" s="108">
         <v>2</v>
       </c>
-      <c r="F56" s="110"/>
+      <c r="F56" s="109"/>
       <c r="G56" s="25"/>
       <c r="H56" s="26"/>
       <c r="I56" s="26"/>
@@ -4815,23 +4805,23 @@
       <c r="O56" s="25"/>
       <c r="P56" s="26"/>
       <c r="Q56" s="26"/>
-      <c r="R56" s="60"/>
+      <c r="R56" s="59"/>
       <c r="S56" s="27"/>
       <c r="T56" s="26"/>
       <c r="U56" s="26"/>
       <c r="V56" s="35"/>
       <c r="W56" s="25"/>
-      <c r="X56" s="82"/>
-      <c r="Y56" s="88"/>
-      <c r="Z56" s="57"/>
-      <c r="AA56" s="87"/>
-      <c r="AB56" s="82"/>
-      <c r="AC56" s="82"/>
+      <c r="X56" s="81"/>
+      <c r="Y56" s="87"/>
+      <c r="Z56" s="56"/>
+      <c r="AA56" s="86"/>
+      <c r="AB56" s="81"/>
+      <c r="AC56" s="81"/>
       <c r="AD56" s="35"/>
       <c r="AE56" s="25"/>
-      <c r="AF56" s="86"/>
-      <c r="AG56" s="60"/>
-      <c r="AH56" s="60"/>
+      <c r="AF56" s="85"/>
+      <c r="AG56" s="59"/>
+      <c r="AH56" s="59"/>
       <c r="AI56" s="25"/>
       <c r="AJ56" s="26"/>
       <c r="AK56" s="26"/>
@@ -4846,12 +4836,12 @@
       <c r="AT56" s="35"/>
     </row>
     <row r="57" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A57" s="107"/>
-      <c r="B57" s="108"/>
-      <c r="C57" s="111"/>
-      <c r="D57" s="112"/>
-      <c r="E57" s="111"/>
-      <c r="F57" s="112"/>
+      <c r="A57" s="106"/>
+      <c r="B57" s="107"/>
+      <c r="C57" s="110"/>
+      <c r="D57" s="111"/>
+      <c r="E57" s="110"/>
+      <c r="F57" s="111"/>
       <c r="G57" s="25"/>
       <c r="H57" s="26"/>
       <c r="I57" s="26"/>
@@ -4863,23 +4853,23 @@
       <c r="O57" s="25"/>
       <c r="P57" s="26"/>
       <c r="Q57" s="26"/>
-      <c r="R57" s="60"/>
+      <c r="R57" s="59"/>
       <c r="S57" s="27"/>
       <c r="T57" s="26"/>
       <c r="U57" s="26"/>
       <c r="V57" s="35"/>
-      <c r="W57" s="87"/>
-      <c r="X57" s="82"/>
+      <c r="W57" s="86"/>
+      <c r="X57" s="81"/>
       <c r="Y57" s="26"/>
-      <c r="Z57" s="57"/>
+      <c r="Z57" s="56"/>
       <c r="AA57" s="27"/>
-      <c r="AB57" s="26"/>
+      <c r="AB57" s="55"/>
       <c r="AC57" s="26"/>
       <c r="AD57" s="35"/>
       <c r="AE57" s="25"/>
-      <c r="AF57" s="86"/>
-      <c r="AG57" s="60"/>
-      <c r="AH57" s="60"/>
+      <c r="AF57" s="85"/>
+      <c r="AG57" s="59"/>
+      <c r="AH57" s="59"/>
       <c r="AI57" s="25"/>
       <c r="AJ57" s="26"/>
       <c r="AK57" s="26"/>
@@ -4894,18 +4884,18 @@
       <c r="AT57" s="35"/>
     </row>
     <row r="58" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A58" s="105" t="s">
+      <c r="A58" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="106"/>
-      <c r="C58" s="109">
+      <c r="B58" s="105"/>
+      <c r="C58" s="108">
         <v>2</v>
       </c>
-      <c r="D58" s="110"/>
-      <c r="E58" s="109">
+      <c r="D58" s="109"/>
+      <c r="E58" s="108">
         <v>2</v>
       </c>
-      <c r="F58" s="110"/>
+      <c r="F58" s="109"/>
       <c r="G58" s="25"/>
       <c r="H58" s="26"/>
       <c r="I58" s="26"/>
@@ -4917,23 +4907,23 @@
       <c r="O58" s="25"/>
       <c r="P58" s="26"/>
       <c r="Q58" s="26"/>
-      <c r="R58" s="60"/>
+      <c r="R58" s="59"/>
       <c r="S58" s="27"/>
       <c r="T58" s="26"/>
       <c r="U58" s="26"/>
       <c r="V58" s="35"/>
       <c r="W58" s="25"/>
       <c r="X58" s="26"/>
-      <c r="Y58" s="82"/>
-      <c r="Z58" s="97"/>
+      <c r="Y58" s="81"/>
+      <c r="Z58" s="96"/>
       <c r="AA58" s="27"/>
       <c r="AB58" s="26"/>
       <c r="AC58" s="26"/>
-      <c r="AD58" s="83"/>
+      <c r="AD58" s="82"/>
       <c r="AE58" s="25"/>
-      <c r="AF58" s="86"/>
-      <c r="AG58" s="60"/>
-      <c r="AH58" s="60"/>
+      <c r="AF58" s="85"/>
+      <c r="AG58" s="59"/>
+      <c r="AH58" s="59"/>
       <c r="AI58" s="25"/>
       <c r="AJ58" s="26"/>
       <c r="AK58" s="26"/>
@@ -4948,12 +4938,12 @@
       <c r="AT58" s="35"/>
     </row>
     <row r="59" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A59" s="107"/>
-      <c r="B59" s="108"/>
-      <c r="C59" s="111"/>
-      <c r="D59" s="112"/>
-      <c r="E59" s="111"/>
-      <c r="F59" s="112"/>
+      <c r="A59" s="106"/>
+      <c r="B59" s="107"/>
+      <c r="C59" s="110"/>
+      <c r="D59" s="111"/>
+      <c r="E59" s="110"/>
+      <c r="F59" s="111"/>
       <c r="G59" s="25"/>
       <c r="H59" s="26"/>
       <c r="I59" s="26"/>
@@ -4965,23 +4955,23 @@
       <c r="O59" s="25"/>
       <c r="P59" s="26"/>
       <c r="Q59" s="26"/>
-      <c r="R59" s="60"/>
+      <c r="R59" s="59"/>
       <c r="S59" s="27"/>
       <c r="T59" s="26"/>
       <c r="U59" s="26"/>
       <c r="V59" s="35"/>
       <c r="W59" s="25"/>
-      <c r="X59" s="82"/>
-      <c r="Y59" s="82"/>
-      <c r="Z59" s="55"/>
+      <c r="X59" s="81"/>
+      <c r="Y59" s="81"/>
+      <c r="Z59" s="54"/>
       <c r="AA59" s="27"/>
-      <c r="AB59" s="26"/>
+      <c r="AB59" s="55"/>
       <c r="AC59" s="26"/>
       <c r="AD59" s="35"/>
       <c r="AE59" s="25"/>
-      <c r="AF59" s="86"/>
-      <c r="AG59" s="60"/>
-      <c r="AH59" s="60"/>
+      <c r="AF59" s="85"/>
+      <c r="AG59" s="59"/>
+      <c r="AH59" s="59"/>
       <c r="AI59" s="25"/>
       <c r="AJ59" s="26"/>
       <c r="AK59" s="26"/>
@@ -4996,18 +4986,18 @@
       <c r="AT59" s="35"/>
     </row>
     <row r="60" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A60" s="105" t="s">
+      <c r="A60" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="B60" s="106"/>
-      <c r="C60" s="109">
+      <c r="B60" s="105"/>
+      <c r="C60" s="108">
         <v>6</v>
       </c>
-      <c r="D60" s="110"/>
-      <c r="E60" s="109">
+      <c r="D60" s="109"/>
+      <c r="E60" s="108">
         <v>6</v>
       </c>
-      <c r="F60" s="110"/>
+      <c r="F60" s="109"/>
       <c r="G60" s="25"/>
       <c r="H60" s="26"/>
       <c r="I60" s="26"/>
@@ -5019,7 +5009,7 @@
       <c r="O60" s="25"/>
       <c r="P60" s="26"/>
       <c r="Q60" s="26"/>
-      <c r="R60" s="60"/>
+      <c r="R60" s="59"/>
       <c r="S60" s="27"/>
       <c r="T60" s="26"/>
       <c r="U60" s="26"/>
@@ -5027,16 +5017,16 @@
       <c r="W60" s="25"/>
       <c r="X60" s="26"/>
       <c r="Y60" s="26"/>
-      <c r="Z60" s="55"/>
-      <c r="AA60" s="98"/>
-      <c r="AB60" s="88"/>
-      <c r="AC60" s="88"/>
-      <c r="AD60" s="55"/>
-      <c r="AE60" s="87"/>
-      <c r="AF60" s="91"/>
-      <c r="AG60" s="60"/>
-      <c r="AH60" s="60"/>
-      <c r="AI60" s="87"/>
+      <c r="Z60" s="54"/>
+      <c r="AA60" s="97"/>
+      <c r="AB60" s="87"/>
+      <c r="AC60" s="87"/>
+      <c r="AD60" s="54"/>
+      <c r="AE60" s="86"/>
+      <c r="AF60" s="90"/>
+      <c r="AG60" s="59"/>
+      <c r="AH60" s="59"/>
+      <c r="AI60" s="86"/>
       <c r="AJ60" s="26"/>
       <c r="AK60" s="26"/>
       <c r="AL60" s="35"/>
@@ -5050,12 +5040,12 @@
       <c r="AT60" s="35"/>
     </row>
     <row r="61" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A61" s="107"/>
-      <c r="B61" s="108"/>
-      <c r="C61" s="111"/>
-      <c r="D61" s="112"/>
-      <c r="E61" s="111"/>
-      <c r="F61" s="112"/>
+      <c r="A61" s="106"/>
+      <c r="B61" s="107"/>
+      <c r="C61" s="110"/>
+      <c r="D61" s="111"/>
+      <c r="E61" s="110"/>
+      <c r="F61" s="111"/>
       <c r="G61" s="25"/>
       <c r="H61" s="26"/>
       <c r="I61" s="26"/>
@@ -5067,7 +5057,7 @@
       <c r="O61" s="25"/>
       <c r="P61" s="26"/>
       <c r="Q61" s="26"/>
-      <c r="R61" s="60"/>
+      <c r="R61" s="59"/>
       <c r="S61" s="27"/>
       <c r="T61" s="26"/>
       <c r="U61" s="26"/>
@@ -5076,14 +5066,14 @@
       <c r="X61" s="26"/>
       <c r="Y61" s="26"/>
       <c r="Z61" s="35"/>
-      <c r="AA61" s="87"/>
-      <c r="AB61" s="82"/>
-      <c r="AC61" s="82"/>
-      <c r="AD61" s="55"/>
-      <c r="AE61" s="87"/>
-      <c r="AF61" s="86"/>
-      <c r="AG61" s="60"/>
-      <c r="AH61" s="60"/>
+      <c r="AA61" s="86"/>
+      <c r="AB61" s="81"/>
+      <c r="AC61" s="81"/>
+      <c r="AD61" s="54"/>
+      <c r="AE61" s="86"/>
+      <c r="AF61" s="85"/>
+      <c r="AG61" s="59"/>
+      <c r="AH61" s="59"/>
       <c r="AI61" s="25"/>
       <c r="AJ61" s="26"/>
       <c r="AK61" s="26"/>
@@ -5098,18 +5088,18 @@
       <c r="AT61" s="35"/>
     </row>
     <row r="62" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A62" s="105" t="s">
+      <c r="A62" s="104" t="s">
         <v>80</v>
       </c>
-      <c r="B62" s="106"/>
-      <c r="C62" s="109">
+      <c r="B62" s="105"/>
+      <c r="C62" s="108">
         <v>4</v>
       </c>
-      <c r="D62" s="110"/>
-      <c r="E62" s="109">
+      <c r="D62" s="109"/>
+      <c r="E62" s="108">
         <v>4</v>
       </c>
-      <c r="F62" s="110"/>
+      <c r="F62" s="109"/>
       <c r="G62" s="25"/>
       <c r="H62" s="26"/>
       <c r="I62" s="26"/>
@@ -5121,7 +5111,7 @@
       <c r="O62" s="25"/>
       <c r="P62" s="26"/>
       <c r="Q62" s="26"/>
-      <c r="R62" s="60"/>
+      <c r="R62" s="59"/>
       <c r="S62" s="27"/>
       <c r="T62" s="26"/>
       <c r="U62" s="26"/>
@@ -5132,18 +5122,18 @@
       <c r="Z62" s="35"/>
       <c r="AA62" s="25"/>
       <c r="AB62" s="26"/>
-      <c r="AC62" s="82"/>
-      <c r="AD62" s="97"/>
-      <c r="AE62" s="99" t="s">
+      <c r="AC62" s="81"/>
+      <c r="AD62" s="96"/>
+      <c r="AE62" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="AF62" s="91"/>
-      <c r="AG62" s="60"/>
-      <c r="AH62" s="60"/>
+      <c r="AF62" s="90"/>
+      <c r="AG62" s="59"/>
+      <c r="AH62" s="59"/>
       <c r="AI62" s="25"/>
-      <c r="AJ62" s="82"/>
-      <c r="AK62" s="82"/>
-      <c r="AL62" s="83"/>
+      <c r="AJ62" s="81"/>
+      <c r="AK62" s="81"/>
+      <c r="AL62" s="82"/>
       <c r="AM62" s="25"/>
       <c r="AN62" s="26"/>
       <c r="AO62" s="26"/>
@@ -5154,12 +5144,12 @@
       <c r="AT62" s="35"/>
     </row>
     <row r="63" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A63" s="107"/>
-      <c r="B63" s="108"/>
-      <c r="C63" s="111"/>
-      <c r="D63" s="112"/>
-      <c r="E63" s="111"/>
-      <c r="F63" s="112"/>
+      <c r="A63" s="106"/>
+      <c r="B63" s="107"/>
+      <c r="C63" s="110"/>
+      <c r="D63" s="111"/>
+      <c r="E63" s="110"/>
+      <c r="F63" s="111"/>
       <c r="G63" s="25"/>
       <c r="H63" s="26"/>
       <c r="I63" s="26"/>
@@ -5171,7 +5161,7 @@
       <c r="O63" s="25"/>
       <c r="P63" s="26"/>
       <c r="Q63" s="26"/>
-      <c r="R63" s="60"/>
+      <c r="R63" s="59"/>
       <c r="S63" s="27"/>
       <c r="T63" s="26"/>
       <c r="U63" s="26"/>
@@ -5183,11 +5173,11 @@
       <c r="AA63" s="25"/>
       <c r="AB63" s="26"/>
       <c r="AC63" s="26"/>
-      <c r="AD63" s="57"/>
-      <c r="AE63" s="87"/>
-      <c r="AF63" s="91"/>
-      <c r="AG63" s="60"/>
-      <c r="AH63" s="60"/>
+      <c r="AD63" s="56"/>
+      <c r="AE63" s="86"/>
+      <c r="AF63" s="90"/>
+      <c r="AG63" s="59"/>
+      <c r="AH63" s="59"/>
       <c r="AI63" s="25"/>
       <c r="AJ63" s="26"/>
       <c r="AK63" s="26"/>
@@ -5202,20 +5192,20 @@
       <c r="AT63" s="35"/>
     </row>
     <row r="64" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="113" t="s">
+      <c r="A64" s="146" t="s">
         <v>39</v>
       </c>
-      <c r="B64" s="114"/>
-      <c r="C64" s="115">
+      <c r="B64" s="147"/>
+      <c r="C64" s="148">
         <f>SUM(C65:D66)</f>
         <v>4</v>
       </c>
-      <c r="D64" s="116"/>
-      <c r="E64" s="115">
+      <c r="D64" s="149"/>
+      <c r="E64" s="148">
         <f>SUM(E65)</f>
         <v>4</v>
       </c>
-      <c r="F64" s="116"/>
+      <c r="F64" s="149"/>
       <c r="G64" s="31"/>
       <c r="H64" s="32"/>
       <c r="I64" s="32"/>
@@ -5227,7 +5217,7 @@
       <c r="O64" s="31"/>
       <c r="P64" s="32"/>
       <c r="Q64" s="32"/>
-      <c r="R64" s="61"/>
+      <c r="R64" s="60"/>
       <c r="S64" s="34"/>
       <c r="T64" s="32"/>
       <c r="U64" s="32"/>
@@ -5241,9 +5231,9 @@
       <c r="AC64" s="32"/>
       <c r="AD64" s="33"/>
       <c r="AE64" s="31"/>
-      <c r="AF64" s="92"/>
-      <c r="AG64" s="61"/>
-      <c r="AH64" s="61"/>
+      <c r="AF64" s="91"/>
+      <c r="AG64" s="60"/>
+      <c r="AH64" s="60"/>
       <c r="AI64" s="31"/>
       <c r="AJ64" s="32"/>
       <c r="AK64" s="32"/>
@@ -5258,18 +5248,18 @@
       <c r="AT64" s="33"/>
     </row>
     <row r="65" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="117" t="s">
+      <c r="A65" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="B65" s="110"/>
-      <c r="C65" s="109">
+      <c r="B65" s="109"/>
+      <c r="C65" s="108">
         <v>4</v>
       </c>
-      <c r="D65" s="110"/>
-      <c r="E65" s="109">
+      <c r="D65" s="109"/>
+      <c r="E65" s="108">
         <v>4</v>
       </c>
-      <c r="F65" s="110"/>
+      <c r="F65" s="109"/>
       <c r="G65" s="25"/>
       <c r="H65" s="26"/>
       <c r="I65" s="26"/>
@@ -5281,7 +5271,7 @@
       <c r="O65" s="25"/>
       <c r="P65" s="26"/>
       <c r="Q65" s="26"/>
-      <c r="R65" s="60"/>
+      <c r="R65" s="59"/>
       <c r="S65" s="27"/>
       <c r="T65" s="26"/>
       <c r="U65" s="26"/>
@@ -5295,17 +5285,17 @@
       <c r="AC65" s="26"/>
       <c r="AD65" s="35"/>
       <c r="AE65" s="25"/>
-      <c r="AF65" s="100"/>
-      <c r="AG65" s="60"/>
-      <c r="AH65" s="59"/>
-      <c r="AI65" s="65" t="s">
+      <c r="AF65" s="99"/>
+      <c r="AG65" s="59"/>
+      <c r="AH65" s="58"/>
+      <c r="AI65" s="64" t="s">
         <v>41</v>
       </c>
       <c r="AJ65" s="26"/>
-      <c r="AK65" s="82"/>
-      <c r="AL65" s="55"/>
-      <c r="AM65" s="87"/>
-      <c r="AN65" s="82"/>
+      <c r="AK65" s="81"/>
+      <c r="AL65" s="54"/>
+      <c r="AM65" s="86"/>
+      <c r="AN65" s="81"/>
       <c r="AO65" s="26"/>
       <c r="AP65" s="35"/>
       <c r="AQ65" s="25"/>
@@ -5314,12 +5304,12 @@
       <c r="AT65" s="35"/>
     </row>
     <row r="66" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="118"/>
-      <c r="B66" s="112"/>
-      <c r="C66" s="111"/>
-      <c r="D66" s="112"/>
-      <c r="E66" s="111"/>
-      <c r="F66" s="112"/>
+      <c r="A66" s="152"/>
+      <c r="B66" s="111"/>
+      <c r="C66" s="110"/>
+      <c r="D66" s="111"/>
+      <c r="E66" s="110"/>
+      <c r="F66" s="111"/>
       <c r="G66" s="25"/>
       <c r="H66" s="26"/>
       <c r="I66" s="26"/>
@@ -5331,7 +5321,7 @@
       <c r="O66" s="25"/>
       <c r="P66" s="26"/>
       <c r="Q66" s="26"/>
-      <c r="R66" s="60"/>
+      <c r="R66" s="59"/>
       <c r="S66" s="27"/>
       <c r="T66" s="26"/>
       <c r="U66" s="26"/>
@@ -5345,13 +5335,13 @@
       <c r="AC66" s="26"/>
       <c r="AD66" s="35"/>
       <c r="AE66" s="25"/>
-      <c r="AF66" s="86"/>
-      <c r="AG66" s="59"/>
-      <c r="AH66" s="59"/>
-      <c r="AI66" s="87"/>
+      <c r="AF66" s="85"/>
+      <c r="AG66" s="58"/>
+      <c r="AH66" s="58"/>
+      <c r="AI66" s="86"/>
       <c r="AJ66" s="26"/>
       <c r="AK66" s="26"/>
-      <c r="AL66" s="57"/>
+      <c r="AL66" s="56"/>
       <c r="AM66" s="27"/>
       <c r="AN66" s="26"/>
       <c r="AO66" s="26"/>
@@ -5362,20 +5352,20 @@
       <c r="AT66" s="35"/>
     </row>
     <row r="67" spans="1:59" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="113" t="s">
+      <c r="A67" s="146" t="s">
         <v>42</v>
       </c>
-      <c r="B67" s="114"/>
-      <c r="C67" s="115">
+      <c r="B67" s="147"/>
+      <c r="C67" s="148">
         <f>SUM(C68:D69)</f>
         <v>4</v>
       </c>
-      <c r="D67" s="116"/>
-      <c r="E67" s="115">
+      <c r="D67" s="149"/>
+      <c r="E67" s="148">
         <f>SUM(E68)</f>
         <v>4</v>
       </c>
-      <c r="F67" s="116"/>
+      <c r="F67" s="149"/>
       <c r="G67" s="31"/>
       <c r="H67" s="32"/>
       <c r="I67" s="32"/>
@@ -5387,7 +5377,7 @@
       <c r="O67" s="31"/>
       <c r="P67" s="32"/>
       <c r="Q67" s="32"/>
-      <c r="R67" s="61"/>
+      <c r="R67" s="60"/>
       <c r="S67" s="34"/>
       <c r="T67" s="32"/>
       <c r="U67" s="32"/>
@@ -5402,12 +5392,12 @@
       <c r="AD67" s="33"/>
       <c r="AE67" s="31"/>
       <c r="AF67" s="32"/>
-      <c r="AG67" s="61"/>
-      <c r="AH67" s="61"/>
+      <c r="AG67" s="60"/>
+      <c r="AH67" s="60"/>
       <c r="AI67" s="31"/>
       <c r="AJ67" s="32"/>
       <c r="AK67" s="32"/>
-      <c r="AL67" s="62"/>
+      <c r="AL67" s="61"/>
       <c r="AM67" s="34"/>
       <c r="AN67" s="32"/>
       <c r="AO67" s="32"/>
@@ -5418,18 +5408,18 @@
       <c r="AT67" s="33"/>
     </row>
     <row r="68" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A68" s="117" t="s">
+      <c r="A68" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="B68" s="110"/>
-      <c r="C68" s="109">
+      <c r="B68" s="109"/>
+      <c r="C68" s="108">
         <v>4</v>
       </c>
-      <c r="D68" s="110"/>
-      <c r="E68" s="109">
+      <c r="D68" s="109"/>
+      <c r="E68" s="108">
         <v>4</v>
       </c>
-      <c r="F68" s="110"/>
+      <c r="F68" s="109"/>
       <c r="G68" s="25"/>
       <c r="H68" s="26"/>
       <c r="I68" s="26"/>
@@ -5441,7 +5431,7 @@
       <c r="O68" s="25"/>
       <c r="P68" s="26"/>
       <c r="Q68" s="26"/>
-      <c r="R68" s="60"/>
+      <c r="R68" s="59"/>
       <c r="S68" s="27"/>
       <c r="T68" s="26"/>
       <c r="U68" s="26"/>
@@ -5456,16 +5446,16 @@
       <c r="AD68" s="35"/>
       <c r="AE68" s="25"/>
       <c r="AF68" s="26"/>
-      <c r="AG68" s="60"/>
-      <c r="AH68" s="60"/>
-      <c r="AI68" s="87"/>
-      <c r="AJ68" s="88"/>
-      <c r="AK68" s="64" t="s">
+      <c r="AG68" s="59"/>
+      <c r="AH68" s="59"/>
+      <c r="AI68" s="86"/>
+      <c r="AJ68" s="87"/>
+      <c r="AK68" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="AL68" s="57"/>
-      <c r="AM68" s="87"/>
-      <c r="AN68" s="82"/>
+      <c r="AL68" s="56"/>
+      <c r="AM68" s="86"/>
+      <c r="AN68" s="81"/>
       <c r="AO68" s="26"/>
       <c r="AP68" s="35"/>
       <c r="AQ68" s="25"/>
@@ -5475,12 +5465,12 @@
       <c r="AU68" s="38"/>
     </row>
     <row r="69" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A69" s="118"/>
-      <c r="B69" s="112"/>
-      <c r="C69" s="111"/>
-      <c r="D69" s="112"/>
-      <c r="E69" s="111"/>
-      <c r="F69" s="112"/>
+      <c r="A69" s="152"/>
+      <c r="B69" s="111"/>
+      <c r="C69" s="110"/>
+      <c r="D69" s="111"/>
+      <c r="E69" s="110"/>
+      <c r="F69" s="111"/>
       <c r="G69" s="25"/>
       <c r="H69" s="26"/>
       <c r="I69" s="26"/>
@@ -5492,7 +5482,7 @@
       <c r="O69" s="25"/>
       <c r="P69" s="26"/>
       <c r="Q69" s="26"/>
-      <c r="R69" s="60"/>
+      <c r="R69" s="59"/>
       <c r="S69" s="27"/>
       <c r="T69" s="26"/>
       <c r="U69" s="26"/>
@@ -5507,12 +5497,12 @@
       <c r="AD69" s="35"/>
       <c r="AE69" s="25"/>
       <c r="AF69" s="26"/>
-      <c r="AG69" s="60"/>
-      <c r="AH69" s="60"/>
+      <c r="AG69" s="59"/>
+      <c r="AH69" s="59"/>
       <c r="AI69" s="25"/>
-      <c r="AJ69" s="82"/>
-      <c r="AK69" s="82"/>
-      <c r="AL69" s="57"/>
+      <c r="AJ69" s="81"/>
+      <c r="AK69" s="81"/>
+      <c r="AL69" s="56"/>
       <c r="AM69" s="27"/>
       <c r="AN69" s="26"/>
       <c r="AO69" s="26"/>
@@ -5524,20 +5514,20 @@
       <c r="AU69" s="39"/>
     </row>
     <row r="70" spans="1:59" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="125" t="s">
+      <c r="A70" s="171" t="s">
         <v>45</v>
       </c>
-      <c r="B70" s="126"/>
-      <c r="C70" s="127">
+      <c r="B70" s="172"/>
+      <c r="C70" s="173">
         <f>SUM(C71:D76)</f>
         <v>18</v>
       </c>
-      <c r="D70" s="128"/>
-      <c r="E70" s="115">
+      <c r="D70" s="174"/>
+      <c r="E70" s="148">
         <f>SUM(E71:F76)</f>
         <v>18</v>
       </c>
-      <c r="F70" s="116"/>
+      <c r="F70" s="149"/>
       <c r="G70" s="40"/>
       <c r="H70" s="41"/>
       <c r="I70" s="41"/>
@@ -5549,7 +5539,7 @@
       <c r="O70" s="40"/>
       <c r="P70" s="41"/>
       <c r="Q70" s="41"/>
-      <c r="R70" s="60"/>
+      <c r="R70" s="59"/>
       <c r="S70" s="43"/>
       <c r="T70" s="41"/>
       <c r="U70" s="41"/>
@@ -5564,12 +5554,12 @@
       <c r="AD70" s="42"/>
       <c r="AE70" s="40"/>
       <c r="AF70" s="41"/>
-      <c r="AG70" s="60"/>
-      <c r="AH70" s="60"/>
+      <c r="AG70" s="59"/>
+      <c r="AH70" s="59"/>
       <c r="AI70" s="40"/>
       <c r="AJ70" s="41"/>
       <c r="AK70" s="41"/>
-      <c r="AL70" s="63"/>
+      <c r="AL70" s="62"/>
       <c r="AM70" s="43"/>
       <c r="AN70" s="41"/>
       <c r="AO70" s="41"/>
@@ -5581,18 +5571,18 @@
       <c r="AU70" s="3"/>
     </row>
     <row r="71" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A71" s="117" t="s">
+      <c r="A71" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="B71" s="110"/>
-      <c r="C71" s="109">
+      <c r="B71" s="109"/>
+      <c r="C71" s="108">
         <v>6</v>
       </c>
-      <c r="D71" s="110"/>
-      <c r="E71" s="109">
+      <c r="D71" s="109"/>
+      <c r="E71" s="108">
         <v>6</v>
       </c>
-      <c r="F71" s="110"/>
+      <c r="F71" s="109"/>
       <c r="G71" s="25"/>
       <c r="H71" s="26"/>
       <c r="I71" s="26"/>
@@ -5604,7 +5594,7 @@
       <c r="O71" s="25"/>
       <c r="P71" s="26"/>
       <c r="Q71" s="26"/>
-      <c r="R71" s="60"/>
+      <c r="R71" s="59"/>
       <c r="S71" s="27"/>
       <c r="T71" s="26"/>
       <c r="U71" s="26"/>
@@ -5619,29 +5609,29 @@
       <c r="AD71" s="35"/>
       <c r="AE71" s="25"/>
       <c r="AF71" s="26"/>
-      <c r="AG71" s="60"/>
-      <c r="AH71" s="60"/>
+      <c r="AG71" s="59"/>
+      <c r="AH71" s="59"/>
       <c r="AI71" s="25"/>
-      <c r="AJ71" s="82"/>
-      <c r="AK71" s="82"/>
-      <c r="AL71" s="97"/>
-      <c r="AM71" s="98"/>
-      <c r="AN71" s="88"/>
-      <c r="AO71" s="82"/>
-      <c r="AP71" s="55"/>
-      <c r="AQ71" s="87"/>
+      <c r="AJ71" s="81"/>
+      <c r="AK71" s="81"/>
+      <c r="AL71" s="96"/>
+      <c r="AM71" s="97"/>
+      <c r="AN71" s="87"/>
+      <c r="AO71" s="81"/>
+      <c r="AP71" s="54"/>
+      <c r="AQ71" s="86"/>
       <c r="AR71" s="26"/>
       <c r="AS71" s="26"/>
       <c r="AT71" s="35"/>
       <c r="AU71" s="3"/>
     </row>
     <row r="72" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A72" s="118"/>
-      <c r="B72" s="112"/>
-      <c r="C72" s="111"/>
-      <c r="D72" s="112"/>
-      <c r="E72" s="111"/>
-      <c r="F72" s="112"/>
+      <c r="A72" s="152"/>
+      <c r="B72" s="111"/>
+      <c r="C72" s="110"/>
+      <c r="D72" s="111"/>
+      <c r="E72" s="110"/>
+      <c r="F72" s="111"/>
       <c r="G72" s="25"/>
       <c r="H72" s="26"/>
       <c r="I72" s="26"/>
@@ -5653,7 +5643,7 @@
       <c r="O72" s="25"/>
       <c r="P72" s="26"/>
       <c r="Q72" s="26"/>
-      <c r="R72" s="60"/>
+      <c r="R72" s="59"/>
       <c r="S72" s="27"/>
       <c r="T72" s="26"/>
       <c r="U72" s="26"/>
@@ -5668,20 +5658,20 @@
       <c r="AD72" s="35"/>
       <c r="AE72" s="25"/>
       <c r="AF72" s="26"/>
-      <c r="AG72" s="60"/>
-      <c r="AH72" s="60"/>
+      <c r="AG72" s="59"/>
+      <c r="AH72" s="59"/>
       <c r="AI72" s="25"/>
       <c r="AJ72" s="26"/>
       <c r="AK72" s="26"/>
-      <c r="AL72" s="55"/>
-      <c r="AM72" s="87"/>
-      <c r="AN72" s="82"/>
-      <c r="AO72" s="82"/>
-      <c r="AP72" s="57"/>
+      <c r="AL72" s="54"/>
+      <c r="AM72" s="86"/>
+      <c r="AN72" s="81"/>
+      <c r="AO72" s="81"/>
+      <c r="AP72" s="56"/>
       <c r="AQ72" s="27"/>
       <c r="AR72" s="26"/>
       <c r="AS72" s="26"/>
-      <c r="AT72" s="57"/>
+      <c r="AT72" s="56"/>
       <c r="AU72" s="3"/>
       <c r="AV72" s="38"/>
       <c r="AW72" s="38"/>
@@ -5697,18 +5687,18 @@
       <c r="BG72" s="38"/>
     </row>
     <row r="73" spans="1:59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="117" t="s">
+      <c r="A73" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="B73" s="110"/>
-      <c r="C73" s="109">
+      <c r="B73" s="109"/>
+      <c r="C73" s="108">
         <v>6</v>
       </c>
-      <c r="D73" s="110"/>
-      <c r="E73" s="109">
+      <c r="D73" s="109"/>
+      <c r="E73" s="108">
         <v>6</v>
       </c>
-      <c r="F73" s="110"/>
+      <c r="F73" s="109"/>
       <c r="G73" s="25"/>
       <c r="H73" s="26"/>
       <c r="I73" s="26"/>
@@ -5720,7 +5710,7 @@
       <c r="O73" s="25"/>
       <c r="P73" s="26"/>
       <c r="Q73" s="26"/>
-      <c r="R73" s="60"/>
+      <c r="R73" s="59"/>
       <c r="S73" s="27"/>
       <c r="T73" s="26"/>
       <c r="U73" s="26"/>
@@ -5735,22 +5725,22 @@
       <c r="AD73" s="35"/>
       <c r="AE73" s="25"/>
       <c r="AF73" s="26"/>
-      <c r="AG73" s="60"/>
-      <c r="AH73" s="60"/>
+      <c r="AG73" s="59"/>
+      <c r="AH73" s="59"/>
       <c r="AI73" s="25"/>
       <c r="AJ73" s="26"/>
       <c r="AK73" s="26"/>
-      <c r="AL73" s="55"/>
-      <c r="AM73" s="87"/>
-      <c r="AN73" s="82"/>
-      <c r="AO73" s="88"/>
-      <c r="AP73" s="101"/>
-      <c r="AQ73" s="99" t="s">
+      <c r="AL73" s="54"/>
+      <c r="AM73" s="86"/>
+      <c r="AN73" s="81"/>
+      <c r="AO73" s="87"/>
+      <c r="AP73" s="100"/>
+      <c r="AQ73" s="98" t="s">
         <v>48</v>
       </c>
       <c r="AR73" s="26"/>
       <c r="AS73" s="26"/>
-      <c r="AT73" s="57"/>
+      <c r="AT73" s="56"/>
       <c r="AU73" s="3"/>
       <c r="AV73" s="38"/>
       <c r="AW73" s="38"/>
@@ -5766,12 +5756,12 @@
       <c r="BG73" s="38"/>
     </row>
     <row r="74" spans="1:59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="118"/>
-      <c r="B74" s="112"/>
-      <c r="C74" s="111"/>
-      <c r="D74" s="112"/>
-      <c r="E74" s="111"/>
-      <c r="F74" s="112"/>
+      <c r="A74" s="152"/>
+      <c r="B74" s="111"/>
+      <c r="C74" s="110"/>
+      <c r="D74" s="111"/>
+      <c r="E74" s="110"/>
+      <c r="F74" s="111"/>
       <c r="G74" s="25"/>
       <c r="H74" s="26"/>
       <c r="I74" s="26"/>
@@ -5783,7 +5773,7 @@
       <c r="O74" s="25"/>
       <c r="P74" s="26"/>
       <c r="Q74" s="26"/>
-      <c r="R74" s="60"/>
+      <c r="R74" s="59"/>
       <c r="S74" s="27"/>
       <c r="T74" s="26"/>
       <c r="U74" s="26"/>
@@ -5798,20 +5788,20 @@
       <c r="AD74" s="35"/>
       <c r="AE74" s="25"/>
       <c r="AF74" s="26"/>
-      <c r="AG74" s="60"/>
-      <c r="AH74" s="60"/>
+      <c r="AG74" s="59"/>
+      <c r="AH74" s="59"/>
       <c r="AI74" s="25"/>
       <c r="AJ74" s="26"/>
       <c r="AK74" s="26"/>
-      <c r="AL74" s="55"/>
-      <c r="AM74" s="87"/>
-      <c r="AN74" s="82"/>
-      <c r="AO74" s="82"/>
-      <c r="AP74" s="57"/>
+      <c r="AL74" s="54"/>
+      <c r="AM74" s="86"/>
+      <c r="AN74" s="81"/>
+      <c r="AO74" s="81"/>
+      <c r="AP74" s="56"/>
       <c r="AQ74" s="27"/>
       <c r="AR74" s="26"/>
       <c r="AS74" s="26"/>
-      <c r="AT74" s="57"/>
+      <c r="AT74" s="56"/>
       <c r="AU74" s="3"/>
       <c r="AV74" s="38"/>
       <c r="AW74" s="38"/>
@@ -5827,18 +5817,18 @@
       <c r="BG74" s="38"/>
     </row>
     <row r="75" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A75" s="117" t="s">
+      <c r="A75" s="124" t="s">
         <v>82</v>
       </c>
-      <c r="B75" s="110"/>
-      <c r="C75" s="109">
+      <c r="B75" s="109"/>
+      <c r="C75" s="108">
         <v>6</v>
       </c>
-      <c r="D75" s="110"/>
-      <c r="E75" s="109">
+      <c r="D75" s="109"/>
+      <c r="E75" s="108">
         <v>6</v>
       </c>
-      <c r="F75" s="110"/>
+      <c r="F75" s="109"/>
       <c r="G75" s="25"/>
       <c r="H75" s="26"/>
       <c r="I75" s="26"/>
@@ -5850,7 +5840,7 @@
       <c r="O75" s="25"/>
       <c r="P75" s="26"/>
       <c r="Q75" s="26"/>
-      <c r="R75" s="60"/>
+      <c r="R75" s="59"/>
       <c r="S75" s="27"/>
       <c r="T75" s="26"/>
       <c r="U75" s="26"/>
@@ -5865,20 +5855,20 @@
       <c r="AD75" s="35"/>
       <c r="AE75" s="25"/>
       <c r="AF75" s="26"/>
-      <c r="AG75" s="60"/>
-      <c r="AH75" s="60"/>
+      <c r="AG75" s="59"/>
+      <c r="AH75" s="59"/>
       <c r="AI75" s="25"/>
       <c r="AJ75" s="26"/>
       <c r="AK75" s="26"/>
-      <c r="AL75" s="57"/>
+      <c r="AL75" s="56"/>
       <c r="AM75" s="27"/>
       <c r="AN75" s="26"/>
-      <c r="AO75" s="82"/>
-      <c r="AP75" s="55"/>
-      <c r="AQ75" s="87"/>
-      <c r="AR75" s="88"/>
-      <c r="AS75" s="88"/>
-      <c r="AT75" s="97"/>
+      <c r="AO75" s="81"/>
+      <c r="AP75" s="54"/>
+      <c r="AQ75" s="86"/>
+      <c r="AR75" s="87"/>
+      <c r="AS75" s="87"/>
+      <c r="AT75" s="96"/>
       <c r="AU75" s="3"/>
       <c r="AV75" s="39"/>
       <c r="AW75" s="39"/>
@@ -5894,12 +5884,12 @@
       <c r="BG75" s="39"/>
     </row>
     <row r="76" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A76" s="118"/>
-      <c r="B76" s="112"/>
-      <c r="C76" s="111"/>
-      <c r="D76" s="112"/>
-      <c r="E76" s="111"/>
-      <c r="F76" s="112"/>
+      <c r="A76" s="152"/>
+      <c r="B76" s="111"/>
+      <c r="C76" s="110"/>
+      <c r="D76" s="111"/>
+      <c r="E76" s="110"/>
+      <c r="F76" s="111"/>
       <c r="G76" s="25"/>
       <c r="H76" s="26"/>
       <c r="I76" s="26"/>
@@ -5911,7 +5901,7 @@
       <c r="O76" s="25"/>
       <c r="P76" s="26"/>
       <c r="Q76" s="26"/>
-      <c r="R76" s="60"/>
+      <c r="R76" s="59"/>
       <c r="S76" s="27"/>
       <c r="T76" s="26"/>
       <c r="U76" s="26"/>
@@ -5926,8 +5916,8 @@
       <c r="AD76" s="35"/>
       <c r="AE76" s="25"/>
       <c r="AF76" s="26"/>
-      <c r="AG76" s="60"/>
-      <c r="AH76" s="60"/>
+      <c r="AG76" s="59"/>
+      <c r="AH76" s="59"/>
       <c r="AI76" s="25"/>
       <c r="AJ76" s="26"/>
       <c r="AK76" s="26"/>
@@ -5935,11 +5925,11 @@
       <c r="AM76" s="25"/>
       <c r="AN76" s="26"/>
       <c r="AO76" s="26"/>
-      <c r="AP76" s="55"/>
-      <c r="AQ76" s="87"/>
-      <c r="AR76" s="82"/>
-      <c r="AS76" s="82"/>
-      <c r="AT76" s="55"/>
+      <c r="AP76" s="54"/>
+      <c r="AQ76" s="86"/>
+      <c r="AR76" s="81"/>
+      <c r="AS76" s="81"/>
+      <c r="AT76" s="54"/>
       <c r="AU76" s="3"/>
       <c r="AV76" s="3"/>
       <c r="AW76" s="3"/>
@@ -6016,20 +6006,20 @@
       <c r="BG77" s="3"/>
     </row>
     <row r="78" spans="1:59" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="119" t="s">
+      <c r="A78" s="165" t="s">
         <v>49</v>
       </c>
-      <c r="B78" s="120"/>
-      <c r="C78" s="121">
+      <c r="B78" s="166"/>
+      <c r="C78" s="167">
         <f>SUM(C14+C17+C29+C42+C47+C64+C67+C26 + C70)</f>
         <v>80</v>
       </c>
-      <c r="D78" s="122"/>
-      <c r="E78" s="123">
+      <c r="D78" s="168"/>
+      <c r="E78" s="169">
         <f>SUM(E14+E17+E29+E42+E47+E64+E67+E26+E70)</f>
         <v>80</v>
       </c>
-      <c r="F78" s="124"/>
+      <c r="F78" s="170"/>
       <c r="G78" s="39"/>
       <c r="H78" s="39"/>
       <c r="I78" s="39"/>
@@ -6147,6 +6137,107 @@
     </row>
   </sheetData>
   <mergeCells count="125">
+    <mergeCell ref="A60:B61"/>
+    <mergeCell ref="C60:D61"/>
+    <mergeCell ref="E60:F61"/>
+    <mergeCell ref="A62:B63"/>
+    <mergeCell ref="C62:D63"/>
+    <mergeCell ref="E62:F63"/>
+    <mergeCell ref="A56:B57"/>
+    <mergeCell ref="C56:D57"/>
+    <mergeCell ref="E56:F57"/>
+    <mergeCell ref="A58:B59"/>
+    <mergeCell ref="C58:D59"/>
+    <mergeCell ref="E58:F59"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="A68:B69"/>
+    <mergeCell ref="C68:D69"/>
+    <mergeCell ref="E68:F69"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="A65:B66"/>
+    <mergeCell ref="C65:D66"/>
+    <mergeCell ref="E65:F66"/>
+    <mergeCell ref="A75:B76"/>
+    <mergeCell ref="C75:D76"/>
+    <mergeCell ref="E75:F76"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="A71:B72"/>
+    <mergeCell ref="C71:D72"/>
+    <mergeCell ref="E71:F72"/>
+    <mergeCell ref="A73:B74"/>
+    <mergeCell ref="C73:D74"/>
+    <mergeCell ref="E73:F74"/>
+    <mergeCell ref="A52:B53"/>
+    <mergeCell ref="C52:D53"/>
+    <mergeCell ref="E52:F53"/>
+    <mergeCell ref="A54:B55"/>
+    <mergeCell ref="C54:D55"/>
+    <mergeCell ref="E54:F55"/>
+    <mergeCell ref="A48:B49"/>
+    <mergeCell ref="C48:D49"/>
+    <mergeCell ref="E48:F49"/>
+    <mergeCell ref="A50:B51"/>
+    <mergeCell ref="C50:D51"/>
+    <mergeCell ref="E50:F51"/>
+    <mergeCell ref="A45:B46"/>
+    <mergeCell ref="C45:D46"/>
+    <mergeCell ref="E45:F46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="A40:B41"/>
+    <mergeCell ref="C40:D41"/>
+    <mergeCell ref="E40:F41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="C43:D44"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="A38:B39"/>
+    <mergeCell ref="C38:D39"/>
+    <mergeCell ref="E38:F39"/>
+    <mergeCell ref="A34:B35"/>
+    <mergeCell ref="C34:D35"/>
+    <mergeCell ref="E34:F35"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="E36:F37"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="E30:F31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:F28"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="E22:F23"/>
+    <mergeCell ref="A24:B25"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="E24:F25"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="E20:F21"/>
     <mergeCell ref="A32:B33"/>
     <mergeCell ref="C32:D33"/>
     <mergeCell ref="E32:F33"/>
@@ -6171,107 +6262,6 @@
     <mergeCell ref="C11:D13"/>
     <mergeCell ref="A11:B13"/>
     <mergeCell ref="A22:B23"/>
-    <mergeCell ref="C22:D23"/>
-    <mergeCell ref="E22:F23"/>
-    <mergeCell ref="A24:B25"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="E24:F25"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="E20:F21"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="E30:F31"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:F28"/>
-    <mergeCell ref="A38:B39"/>
-    <mergeCell ref="C38:D39"/>
-    <mergeCell ref="E38:F39"/>
-    <mergeCell ref="A34:B35"/>
-    <mergeCell ref="C34:D35"/>
-    <mergeCell ref="E34:F35"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="E36:F37"/>
-    <mergeCell ref="A45:B46"/>
-    <mergeCell ref="C45:D46"/>
-    <mergeCell ref="E45:F46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="A40:B41"/>
-    <mergeCell ref="C40:D41"/>
-    <mergeCell ref="E40:F41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="C43:D44"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="A52:B53"/>
-    <mergeCell ref="C52:D53"/>
-    <mergeCell ref="E52:F53"/>
-    <mergeCell ref="A54:B55"/>
-    <mergeCell ref="C54:D55"/>
-    <mergeCell ref="E54:F55"/>
-    <mergeCell ref="A48:B49"/>
-    <mergeCell ref="C48:D49"/>
-    <mergeCell ref="E48:F49"/>
-    <mergeCell ref="A50:B51"/>
-    <mergeCell ref="C50:D51"/>
-    <mergeCell ref="E50:F51"/>
-    <mergeCell ref="A75:B76"/>
-    <mergeCell ref="C75:D76"/>
-    <mergeCell ref="E75:F76"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="A71:B72"/>
-    <mergeCell ref="C71:D72"/>
-    <mergeCell ref="E71:F72"/>
-    <mergeCell ref="A73:B74"/>
-    <mergeCell ref="C73:D74"/>
-    <mergeCell ref="E73:F74"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="A68:B69"/>
-    <mergeCell ref="C68:D69"/>
-    <mergeCell ref="E68:F69"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="A65:B66"/>
-    <mergeCell ref="C65:D66"/>
-    <mergeCell ref="E65:F66"/>
-    <mergeCell ref="A60:B61"/>
-    <mergeCell ref="C60:D61"/>
-    <mergeCell ref="E60:F61"/>
-    <mergeCell ref="A62:B63"/>
-    <mergeCell ref="C62:D63"/>
-    <mergeCell ref="E62:F63"/>
-    <mergeCell ref="A56:B57"/>
-    <mergeCell ref="C56:D57"/>
-    <mergeCell ref="E56:F57"/>
-    <mergeCell ref="A58:B59"/>
-    <mergeCell ref="C58:D59"/>
-    <mergeCell ref="E58:F59"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
create controller, request and resource
</commit_message>
<xml_diff>
--- a/documentation/Zeitplan.xlsx
+++ b/documentation/Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp8\htdocs\IPA\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA57A392-4865-4FE5-AF63-02B809952802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5B8D7A-D9EF-4563-B810-5BA53BFACD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1266,6 +1266,54 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1276,6 +1324,66 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1302,9 +1410,6 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1317,13 +1422,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1355,105 +1454,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1744,8 +1744,8 @@
   </sheetPr>
   <dimension ref="A1:BG79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="AB59" sqref="AB59"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="AD63" sqref="AD63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1758,27 +1758,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:59" ht="44.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="152" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116"/>
-      <c r="N1" s="116"/>
-      <c r="O1" s="116"/>
-      <c r="P1" s="116"/>
-      <c r="Q1" s="116"/>
-      <c r="R1" s="116"/>
-      <c r="S1" s="116"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="152"/>
+      <c r="H1" s="152"/>
+      <c r="I1" s="152"/>
+      <c r="J1" s="152"/>
+      <c r="K1" s="152"/>
+      <c r="L1" s="152"/>
+      <c r="M1" s="152"/>
+      <c r="N1" s="152"/>
+      <c r="O1" s="152"/>
+      <c r="P1" s="152"/>
+      <c r="Q1" s="152"/>
+      <c r="R1" s="152"/>
+      <c r="S1" s="152"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
@@ -2354,86 +2354,86 @@
       <c r="BG10" s="3"/>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A11" s="137" t="s">
+      <c r="A11" s="170" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="138"/>
-      <c r="C11" s="132" t="s">
+      <c r="B11" s="171"/>
+      <c r="C11" s="165" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="133"/>
-      <c r="E11" s="132" t="s">
+      <c r="D11" s="166"/>
+      <c r="E11" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="133"/>
-      <c r="G11" s="117" t="s">
+      <c r="F11" s="166"/>
+      <c r="G11" s="153" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="118"/>
-      <c r="I11" s="118"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="117" t="s">
+      <c r="H11" s="154"/>
+      <c r="I11" s="154"/>
+      <c r="J11" s="155"/>
+      <c r="K11" s="153" t="s">
         <v>58</v>
       </c>
-      <c r="L11" s="118"/>
-      <c r="M11" s="118"/>
-      <c r="N11" s="119"/>
-      <c r="O11" s="117" t="s">
+      <c r="L11" s="154"/>
+      <c r="M11" s="154"/>
+      <c r="N11" s="155"/>
+      <c r="O11" s="153" t="s">
         <v>59</v>
       </c>
-      <c r="P11" s="118"/>
-      <c r="Q11" s="118"/>
-      <c r="R11" s="119"/>
-      <c r="S11" s="117" t="s">
+      <c r="P11" s="154"/>
+      <c r="Q11" s="154"/>
+      <c r="R11" s="155"/>
+      <c r="S11" s="153" t="s">
         <v>60</v>
       </c>
-      <c r="T11" s="118"/>
-      <c r="U11" s="118"/>
-      <c r="V11" s="119"/>
-      <c r="W11" s="117" t="s">
+      <c r="T11" s="154"/>
+      <c r="U11" s="154"/>
+      <c r="V11" s="155"/>
+      <c r="W11" s="153" t="s">
         <v>61</v>
       </c>
-      <c r="X11" s="118"/>
-      <c r="Y11" s="118"/>
-      <c r="Z11" s="119"/>
-      <c r="AA11" s="117" t="s">
+      <c r="X11" s="154"/>
+      <c r="Y11" s="154"/>
+      <c r="Z11" s="155"/>
+      <c r="AA11" s="153" t="s">
         <v>62</v>
       </c>
-      <c r="AB11" s="118"/>
-      <c r="AC11" s="118"/>
-      <c r="AD11" s="119"/>
-      <c r="AE11" s="117" t="s">
+      <c r="AB11" s="154"/>
+      <c r="AC11" s="154"/>
+      <c r="AD11" s="155"/>
+      <c r="AE11" s="153" t="s">
         <v>63</v>
       </c>
-      <c r="AF11" s="118"/>
-      <c r="AG11" s="118"/>
-      <c r="AH11" s="119"/>
-      <c r="AI11" s="117" t="s">
+      <c r="AF11" s="154"/>
+      <c r="AG11" s="154"/>
+      <c r="AH11" s="155"/>
+      <c r="AI11" s="153" t="s">
         <v>64</v>
       </c>
-      <c r="AJ11" s="118"/>
-      <c r="AK11" s="118"/>
-      <c r="AL11" s="119"/>
-      <c r="AM11" s="117" t="s">
+      <c r="AJ11" s="154"/>
+      <c r="AK11" s="154"/>
+      <c r="AL11" s="155"/>
+      <c r="AM11" s="153" t="s">
         <v>65</v>
       </c>
-      <c r="AN11" s="118"/>
-      <c r="AO11" s="118"/>
-      <c r="AP11" s="119"/>
-      <c r="AQ11" s="117" t="s">
+      <c r="AN11" s="154"/>
+      <c r="AO11" s="154"/>
+      <c r="AP11" s="155"/>
+      <c r="AQ11" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="AR11" s="118"/>
-      <c r="AS11" s="118"/>
-      <c r="AT11" s="119"/>
+      <c r="AR11" s="154"/>
+      <c r="AS11" s="154"/>
+      <c r="AT11" s="155"/>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A12" s="139"/>
-      <c r="B12" s="138"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="133"/>
+      <c r="A12" s="172"/>
+      <c r="B12" s="171"/>
+      <c r="C12" s="167"/>
+      <c r="D12" s="166"/>
+      <c r="E12" s="167"/>
+      <c r="F12" s="166"/>
       <c r="G12" s="10">
         <v>1</v>
       </c>
@@ -2556,12 +2556,12 @@
       </c>
     </row>
     <row r="13" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="140"/>
-      <c r="B13" s="141"/>
-      <c r="C13" s="135"/>
-      <c r="D13" s="136"/>
-      <c r="E13" s="135"/>
-      <c r="F13" s="136"/>
+      <c r="A13" s="173"/>
+      <c r="B13" s="174"/>
+      <c r="C13" s="168"/>
+      <c r="D13" s="169"/>
+      <c r="E13" s="168"/>
+      <c r="F13" s="169"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
@@ -2604,20 +2604,20 @@
       <c r="AT13" s="16"/>
     </row>
     <row r="14" spans="1:59" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="120" t="s">
+      <c r="A14" s="156" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="121"/>
-      <c r="C14" s="122">
+      <c r="B14" s="157"/>
+      <c r="C14" s="158">
         <f>SUM(C15:D16)</f>
         <v>6</v>
       </c>
-      <c r="D14" s="123"/>
-      <c r="E14" s="122">
+      <c r="D14" s="159"/>
+      <c r="E14" s="158">
         <f>SUM(E15)</f>
         <v>6</v>
       </c>
-      <c r="F14" s="123"/>
+      <c r="F14" s="159"/>
       <c r="G14" s="18"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
@@ -2660,18 +2660,18 @@
       <c r="AT14" s="20"/>
     </row>
     <row r="15" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="124" t="s">
+      <c r="A15" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="125"/>
-      <c r="C15" s="128">
+      <c r="B15" s="160"/>
+      <c r="C15" s="163">
         <v>6</v>
       </c>
-      <c r="D15" s="129"/>
-      <c r="E15" s="128">
+      <c r="D15" s="136"/>
+      <c r="E15" s="163">
         <v>6</v>
       </c>
-      <c r="F15" s="129"/>
+      <c r="F15" s="136"/>
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
       <c r="I15" s="26"/>
@@ -2714,12 +2714,12 @@
       <c r="AT15" s="50"/>
     </row>
     <row r="16" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="126"/>
-      <c r="B16" s="127"/>
-      <c r="C16" s="130"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="130"/>
-      <c r="F16" s="131"/>
+      <c r="A16" s="161"/>
+      <c r="B16" s="162"/>
+      <c r="C16" s="164"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="164"/>
+      <c r="F16" s="138"/>
       <c r="G16" s="30"/>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
@@ -2755,20 +2755,20 @@
       <c r="AT16" s="54"/>
     </row>
     <row r="17" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="146" t="s">
+      <c r="A17" s="112" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="147"/>
-      <c r="C17" s="148">
+      <c r="B17" s="113"/>
+      <c r="C17" s="114">
         <f>SUM(C18:D25)</f>
         <v>12</v>
       </c>
-      <c r="D17" s="149"/>
-      <c r="E17" s="150">
+      <c r="D17" s="115"/>
+      <c r="E17" s="146">
         <f>SUM(E18:F25)</f>
-        <v>12</v>
-      </c>
-      <c r="F17" s="151"/>
+        <v>10</v>
+      </c>
+      <c r="F17" s="147"/>
       <c r="G17" s="31"/>
       <c r="H17" s="32"/>
       <c r="I17" s="32"/>
@@ -2811,7 +2811,7 @@
       <c r="AT17" s="33"/>
     </row>
     <row r="18" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="124" t="s">
+      <c r="A18" s="116" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="109"/>
@@ -2865,7 +2865,7 @@
       <c r="AT18" s="35"/>
     </row>
     <row r="19" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="152"/>
+      <c r="A19" s="117"/>
       <c r="B19" s="111"/>
       <c r="C19" s="110"/>
       <c r="D19" s="111"/>
@@ -2913,7 +2913,7 @@
       <c r="AT19" s="35"/>
     </row>
     <row r="20" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="124" t="s">
+      <c r="A20" s="116" t="s">
         <v>67</v>
       </c>
       <c r="B20" s="109"/>
@@ -2922,7 +2922,7 @@
       </c>
       <c r="D20" s="109"/>
       <c r="E20" s="108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="109"/>
       <c r="G20" s="86"/>
@@ -2967,7 +2967,7 @@
       <c r="AT20" s="35"/>
     </row>
     <row r="21" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="152"/>
+      <c r="A21" s="117"/>
       <c r="B21" s="111"/>
       <c r="C21" s="110"/>
       <c r="D21" s="111"/>
@@ -3024,7 +3024,7 @@
       </c>
       <c r="D22" s="109"/>
       <c r="E22" s="108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" s="109"/>
       <c r="G22" s="79"/>
@@ -3124,10 +3124,10 @@
         <v>2</v>
       </c>
       <c r="D24" s="109"/>
-      <c r="E24" s="142">
+      <c r="E24" s="148">
         <v>2</v>
       </c>
-      <c r="F24" s="143"/>
+      <c r="F24" s="149"/>
       <c r="G24" s="25"/>
       <c r="H24" s="81"/>
       <c r="I24" s="26"/>
@@ -3176,8 +3176,8 @@
       <c r="B25" s="107"/>
       <c r="C25" s="110"/>
       <c r="D25" s="111"/>
-      <c r="E25" s="144"/>
-      <c r="F25" s="145"/>
+      <c r="E25" s="150"/>
+      <c r="F25" s="151"/>
       <c r="G25" s="25"/>
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
@@ -3222,20 +3222,20 @@
       <c r="AT25" s="35"/>
     </row>
     <row r="26" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="146" t="s">
+      <c r="A26" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="147"/>
-      <c r="C26" s="148">
+      <c r="B26" s="113"/>
+      <c r="C26" s="114">
         <f>SUM(C27)</f>
         <v>2</v>
       </c>
-      <c r="D26" s="149"/>
-      <c r="E26" s="150">
+      <c r="D26" s="115"/>
+      <c r="E26" s="146">
         <f>SUM(E27)</f>
-        <v>2</v>
-      </c>
-      <c r="F26" s="151"/>
+        <v>3</v>
+      </c>
+      <c r="F26" s="147"/>
       <c r="G26" s="31"/>
       <c r="H26" s="32"/>
       <c r="I26" s="32"/>
@@ -3278,7 +3278,7 @@
       <c r="AT26" s="33"/>
     </row>
     <row r="27" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="124" t="s">
+      <c r="A27" s="116" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="109"/>
@@ -3287,7 +3287,7 @@
       </c>
       <c r="D27" s="109"/>
       <c r="E27" s="108">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27" s="109"/>
       <c r="G27" s="25"/>
@@ -3333,7 +3333,7 @@
       <c r="AT27" s="35"/>
     </row>
     <row r="28" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="152"/>
+      <c r="A28" s="117"/>
       <c r="B28" s="111"/>
       <c r="C28" s="110"/>
       <c r="D28" s="111"/>
@@ -3383,20 +3383,20 @@
       <c r="AT28" s="35"/>
     </row>
     <row r="29" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="146" t="s">
+      <c r="A29" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="147"/>
-      <c r="C29" s="148">
+      <c r="B29" s="113"/>
+      <c r="C29" s="114">
         <f>SUM(C30:D41)</f>
         <v>12</v>
       </c>
-      <c r="D29" s="149"/>
-      <c r="E29" s="148">
+      <c r="D29" s="115"/>
+      <c r="E29" s="114">
         <f>SUM(E30:F41)</f>
-        <v>12</v>
-      </c>
-      <c r="F29" s="149"/>
+        <v>25</v>
+      </c>
+      <c r="F29" s="115"/>
       <c r="G29" s="31"/>
       <c r="H29" s="32"/>
       <c r="I29" s="32"/>
@@ -3447,10 +3447,10 @@
         <v>2</v>
       </c>
       <c r="D30" s="109"/>
-      <c r="E30" s="112">
-        <v>2</v>
-      </c>
-      <c r="F30" s="113"/>
+      <c r="E30" s="128">
+        <v>1</v>
+      </c>
+      <c r="F30" s="129"/>
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
@@ -3497,8 +3497,8 @@
       <c r="B31" s="107"/>
       <c r="C31" s="110"/>
       <c r="D31" s="111"/>
-      <c r="E31" s="114"/>
-      <c r="F31" s="115"/>
+      <c r="E31" s="130"/>
+      <c r="F31" s="131"/>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
@@ -3549,10 +3549,10 @@
         <v>2</v>
       </c>
       <c r="D32" s="109"/>
-      <c r="E32" s="112">
+      <c r="E32" s="128">
         <v>2</v>
       </c>
-      <c r="F32" s="113"/>
+      <c r="F32" s="129"/>
       <c r="G32" s="25"/>
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
@@ -3599,8 +3599,8 @@
       <c r="B33" s="107"/>
       <c r="C33" s="110"/>
       <c r="D33" s="111"/>
-      <c r="E33" s="114"/>
-      <c r="F33" s="115"/>
+      <c r="E33" s="130"/>
+      <c r="F33" s="131"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3754,7 +3754,7 @@
       </c>
       <c r="D36" s="109"/>
       <c r="E36" s="108">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F36" s="109"/>
       <c r="G36" s="25"/>
@@ -3847,7 +3847,7 @@
       <c r="AT37" s="35"/>
     </row>
     <row r="38" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="124" t="s">
+      <c r="A38" s="116" t="s">
         <v>31</v>
       </c>
       <c r="B38" s="109"/>
@@ -3856,7 +3856,7 @@
       </c>
       <c r="D38" s="109"/>
       <c r="E38" s="108">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F38" s="109"/>
       <c r="G38" s="25"/>
@@ -3901,7 +3901,7 @@
       <c r="AT38" s="35"/>
     </row>
     <row r="39" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="152"/>
+      <c r="A39" s="117"/>
       <c r="B39" s="111"/>
       <c r="C39" s="110"/>
       <c r="D39" s="111"/>
@@ -3958,7 +3958,7 @@
       </c>
       <c r="D40" s="109"/>
       <c r="E40" s="108">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F40" s="109"/>
       <c r="G40" s="25"/>
@@ -4055,20 +4055,20 @@
       <c r="AT41" s="35"/>
     </row>
     <row r="42" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="146" t="s">
+      <c r="A42" s="112" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="147"/>
-      <c r="C42" s="148">
+      <c r="B42" s="113"/>
+      <c r="C42" s="114">
         <f>SUM(C43:C45)</f>
         <v>3</v>
       </c>
-      <c r="D42" s="149"/>
-      <c r="E42" s="148">
+      <c r="D42" s="115"/>
+      <c r="E42" s="114">
         <f>SUM(E45+E43)</f>
-        <v>3</v>
-      </c>
-      <c r="F42" s="149"/>
+        <v>2</v>
+      </c>
+      <c r="F42" s="115"/>
       <c r="G42" s="31"/>
       <c r="H42" s="32"/>
       <c r="I42" s="32"/>
@@ -4111,18 +4111,18 @@
       <c r="AT42" s="33"/>
     </row>
     <row r="43" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="154" t="s">
+      <c r="A43" s="139" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="155"/>
-      <c r="C43" s="154">
+      <c r="B43" s="140"/>
+      <c r="C43" s="139">
         <v>2</v>
       </c>
-      <c r="D43" s="158"/>
-      <c r="E43" s="154">
-        <v>2</v>
-      </c>
-      <c r="F43" s="158"/>
+      <c r="D43" s="143"/>
+      <c r="E43" s="139">
+        <v>1</v>
+      </c>
+      <c r="F43" s="143"/>
       <c r="G43" s="84"/>
       <c r="H43" s="81"/>
       <c r="I43" s="81"/>
@@ -4165,12 +4165,12 @@
       <c r="AT43" s="54"/>
     </row>
     <row r="44" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="156"/>
-      <c r="B44" s="157"/>
-      <c r="C44" s="159"/>
-      <c r="D44" s="160"/>
-      <c r="E44" s="159"/>
-      <c r="F44" s="160"/>
+      <c r="A44" s="141"/>
+      <c r="B44" s="142"/>
+      <c r="C44" s="144"/>
+      <c r="D44" s="145"/>
+      <c r="E44" s="144"/>
+      <c r="F44" s="145"/>
       <c r="G44" s="84"/>
       <c r="H44" s="81"/>
       <c r="I44" s="81"/>
@@ -4213,10 +4213,10 @@
       <c r="AT44" s="54"/>
     </row>
     <row r="45" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="124" t="s">
+      <c r="A45" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B45" s="129"/>
+      <c r="B45" s="136"/>
       <c r="C45" s="108">
         <v>1</v>
       </c>
@@ -4269,8 +4269,8 @@
       <c r="AT45" s="35"/>
     </row>
     <row r="46" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="153"/>
-      <c r="B46" s="131"/>
+      <c r="A46" s="137"/>
+      <c r="B46" s="138"/>
       <c r="C46" s="110"/>
       <c r="D46" s="111"/>
       <c r="E46" s="110"/>
@@ -4319,20 +4319,20 @@
       <c r="AT46" s="35"/>
     </row>
     <row r="47" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="146" t="s">
+      <c r="A47" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="147"/>
-      <c r="C47" s="148">
+      <c r="B47" s="113"/>
+      <c r="C47" s="114">
         <f>SUM(C48:D63)</f>
         <v>19</v>
       </c>
-      <c r="D47" s="149"/>
-      <c r="E47" s="148">
+      <c r="D47" s="115"/>
+      <c r="E47" s="114">
         <f>SUM(E48:F63)</f>
-        <v>19</v>
-      </c>
-      <c r="F47" s="149"/>
+        <v>17</v>
+      </c>
+      <c r="F47" s="115"/>
       <c r="G47" s="31"/>
       <c r="H47" s="32"/>
       <c r="I47" s="32"/>
@@ -4375,10 +4375,10 @@
       <c r="AT47" s="33"/>
     </row>
     <row r="48" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="161" t="s">
+      <c r="A48" s="132" t="s">
         <v>74</v>
       </c>
-      <c r="B48" s="162"/>
+      <c r="B48" s="133"/>
       <c r="C48" s="108">
         <v>0.5</v>
       </c>
@@ -4429,8 +4429,8 @@
       <c r="AT48" s="35"/>
     </row>
     <row r="49" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="163"/>
-      <c r="B49" s="164"/>
+      <c r="A49" s="134"/>
+      <c r="B49" s="135"/>
       <c r="C49" s="110"/>
       <c r="D49" s="111"/>
       <c r="E49" s="110"/>
@@ -4477,7 +4477,7 @@
       <c r="AT49" s="35"/>
     </row>
     <row r="50" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A50" s="124" t="s">
+      <c r="A50" s="116" t="s">
         <v>75</v>
       </c>
       <c r="B50" s="109"/>
@@ -4485,10 +4485,10 @@
         <v>0.5</v>
       </c>
       <c r="D50" s="109"/>
-      <c r="E50" s="112">
+      <c r="E50" s="128">
         <v>0.5</v>
       </c>
-      <c r="F50" s="113"/>
+      <c r="F50" s="129"/>
       <c r="G50" s="25"/>
       <c r="H50" s="26"/>
       <c r="I50" s="26"/>
@@ -4531,12 +4531,12 @@
       <c r="AT50" s="35"/>
     </row>
     <row r="51" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="152"/>
+      <c r="A51" s="117"/>
       <c r="B51" s="111"/>
       <c r="C51" s="110"/>
       <c r="D51" s="111"/>
-      <c r="E51" s="114"/>
-      <c r="F51" s="115"/>
+      <c r="E51" s="130"/>
+      <c r="F51" s="131"/>
       <c r="G51" s="25"/>
       <c r="H51" s="26"/>
       <c r="I51" s="26"/>
@@ -4579,7 +4579,7 @@
       <c r="AT51" s="35"/>
     </row>
     <row r="52" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A52" s="124" t="s">
+      <c r="A52" s="116" t="s">
         <v>76</v>
       </c>
       <c r="B52" s="109"/>
@@ -4587,10 +4587,10 @@
         <v>2</v>
       </c>
       <c r="D52" s="109"/>
-      <c r="E52" s="112">
-        <v>2</v>
-      </c>
-      <c r="F52" s="113"/>
+      <c r="E52" s="128">
+        <v>1.5</v>
+      </c>
+      <c r="F52" s="129"/>
       <c r="G52" s="25"/>
       <c r="H52" s="26"/>
       <c r="I52" s="26"/>
@@ -4633,12 +4633,12 @@
       <c r="AT52" s="35"/>
     </row>
     <row r="53" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="152"/>
+      <c r="A53" s="117"/>
       <c r="B53" s="111"/>
       <c r="C53" s="110"/>
       <c r="D53" s="111"/>
-      <c r="E53" s="114"/>
-      <c r="F53" s="115"/>
+      <c r="E53" s="130"/>
+      <c r="F53" s="131"/>
       <c r="G53" s="25"/>
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
@@ -4661,8 +4661,8 @@
       <c r="Z53" s="35"/>
       <c r="AA53" s="25"/>
       <c r="AB53" s="55"/>
-      <c r="AC53" s="26"/>
-      <c r="AD53" s="35"/>
+      <c r="AC53" s="55"/>
+      <c r="AD53" s="102"/>
       <c r="AE53" s="25"/>
       <c r="AF53" s="85"/>
       <c r="AG53" s="59"/>
@@ -4681,7 +4681,7 @@
       <c r="AT53" s="35"/>
     </row>
     <row r="54" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="124" t="s">
+      <c r="A54" s="116" t="s">
         <v>78</v>
       </c>
       <c r="B54" s="109"/>
@@ -4689,10 +4689,10 @@
         <v>2</v>
       </c>
       <c r="D54" s="109"/>
-      <c r="E54" s="112">
-        <v>2</v>
-      </c>
-      <c r="F54" s="113"/>
+      <c r="E54" s="128">
+        <v>1.5</v>
+      </c>
+      <c r="F54" s="129"/>
       <c r="G54" s="25"/>
       <c r="H54" s="26"/>
       <c r="I54" s="26"/>
@@ -4735,12 +4735,12 @@
       <c r="AT54" s="35"/>
     </row>
     <row r="55" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="152"/>
+      <c r="A55" s="117"/>
       <c r="B55" s="111"/>
       <c r="C55" s="110"/>
       <c r="D55" s="111"/>
-      <c r="E55" s="114"/>
-      <c r="F55" s="115"/>
+      <c r="E55" s="130"/>
+      <c r="F55" s="131"/>
       <c r="G55" s="25"/>
       <c r="H55" s="26"/>
       <c r="I55" s="26"/>
@@ -4762,8 +4762,8 @@
       <c r="Z55" s="56"/>
       <c r="AA55" s="27"/>
       <c r="AB55" s="55"/>
-      <c r="AC55" s="26"/>
-      <c r="AD55" s="35"/>
+      <c r="AC55" s="55"/>
+      <c r="AD55" s="102"/>
       <c r="AE55" s="25"/>
       <c r="AF55" s="85"/>
       <c r="AG55" s="59"/>
@@ -4791,7 +4791,7 @@
       </c>
       <c r="D56" s="109"/>
       <c r="E56" s="108">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F56" s="109"/>
       <c r="G56" s="25"/>
@@ -4864,8 +4864,8 @@
       <c r="Z57" s="56"/>
       <c r="AA57" s="27"/>
       <c r="AB57" s="55"/>
-      <c r="AC57" s="26"/>
-      <c r="AD57" s="35"/>
+      <c r="AC57" s="55"/>
+      <c r="AD57" s="102"/>
       <c r="AE57" s="25"/>
       <c r="AF57" s="85"/>
       <c r="AG57" s="59"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="D58" s="109"/>
       <c r="E58" s="108">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F58" s="109"/>
       <c r="G58" s="25"/>
@@ -4966,8 +4966,8 @@
       <c r="Z59" s="54"/>
       <c r="AA59" s="27"/>
       <c r="AB59" s="55"/>
-      <c r="AC59" s="26"/>
-      <c r="AD59" s="35"/>
+      <c r="AC59" s="55"/>
+      <c r="AD59" s="102"/>
       <c r="AE59" s="25"/>
       <c r="AF59" s="85"/>
       <c r="AG59" s="59"/>
@@ -5192,20 +5192,20 @@
       <c r="AT63" s="35"/>
     </row>
     <row r="64" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="146" t="s">
+      <c r="A64" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="B64" s="147"/>
-      <c r="C64" s="148">
+      <c r="B64" s="113"/>
+      <c r="C64" s="114">
         <f>SUM(C65:D66)</f>
         <v>4</v>
       </c>
-      <c r="D64" s="149"/>
-      <c r="E64" s="148">
+      <c r="D64" s="115"/>
+      <c r="E64" s="114">
         <f>SUM(E65)</f>
         <v>4</v>
       </c>
-      <c r="F64" s="149"/>
+      <c r="F64" s="115"/>
       <c r="G64" s="31"/>
       <c r="H64" s="32"/>
       <c r="I64" s="32"/>
@@ -5248,7 +5248,7 @@
       <c r="AT64" s="33"/>
     </row>
     <row r="65" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="124" t="s">
+      <c r="A65" s="116" t="s">
         <v>40</v>
       </c>
       <c r="B65" s="109"/>
@@ -5304,7 +5304,7 @@
       <c r="AT65" s="35"/>
     </row>
     <row r="66" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="152"/>
+      <c r="A66" s="117"/>
       <c r="B66" s="111"/>
       <c r="C66" s="110"/>
       <c r="D66" s="111"/>
@@ -5352,20 +5352,20 @@
       <c r="AT66" s="35"/>
     </row>
     <row r="67" spans="1:59" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="146" t="s">
+      <c r="A67" s="112" t="s">
         <v>42</v>
       </c>
-      <c r="B67" s="147"/>
-      <c r="C67" s="148">
+      <c r="B67" s="113"/>
+      <c r="C67" s="114">
         <f>SUM(C68:D69)</f>
         <v>4</v>
       </c>
-      <c r="D67" s="149"/>
-      <c r="E67" s="148">
+      <c r="D67" s="115"/>
+      <c r="E67" s="114">
         <f>SUM(E68)</f>
         <v>4</v>
       </c>
-      <c r="F67" s="149"/>
+      <c r="F67" s="115"/>
       <c r="G67" s="31"/>
       <c r="H67" s="32"/>
       <c r="I67" s="32"/>
@@ -5408,7 +5408,7 @@
       <c r="AT67" s="33"/>
     </row>
     <row r="68" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A68" s="124" t="s">
+      <c r="A68" s="116" t="s">
         <v>43</v>
       </c>
       <c r="B68" s="109"/>
@@ -5465,7 +5465,7 @@
       <c r="AU68" s="38"/>
     </row>
     <row r="69" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A69" s="152"/>
+      <c r="A69" s="117"/>
       <c r="B69" s="111"/>
       <c r="C69" s="110"/>
       <c r="D69" s="111"/>
@@ -5514,20 +5514,20 @@
       <c r="AU69" s="39"/>
     </row>
     <row r="70" spans="1:59" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="171" t="s">
+      <c r="A70" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="B70" s="172"/>
-      <c r="C70" s="173">
+      <c r="B70" s="125"/>
+      <c r="C70" s="126">
         <f>SUM(C71:D76)</f>
         <v>18</v>
       </c>
-      <c r="D70" s="174"/>
-      <c r="E70" s="148">
+      <c r="D70" s="127"/>
+      <c r="E70" s="114">
         <f>SUM(E71:F76)</f>
         <v>18</v>
       </c>
-      <c r="F70" s="149"/>
+      <c r="F70" s="115"/>
       <c r="G70" s="40"/>
       <c r="H70" s="41"/>
       <c r="I70" s="41"/>
@@ -5571,7 +5571,7 @@
       <c r="AU70" s="3"/>
     </row>
     <row r="71" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A71" s="124" t="s">
+      <c r="A71" s="116" t="s">
         <v>46</v>
       </c>
       <c r="B71" s="109"/>
@@ -5626,7 +5626,7 @@
       <c r="AU71" s="3"/>
     </row>
     <row r="72" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A72" s="152"/>
+      <c r="A72" s="117"/>
       <c r="B72" s="111"/>
       <c r="C72" s="110"/>
       <c r="D72" s="111"/>
@@ -5687,7 +5687,7 @@
       <c r="BG72" s="38"/>
     </row>
     <row r="73" spans="1:59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="124" t="s">
+      <c r="A73" s="116" t="s">
         <v>47</v>
       </c>
       <c r="B73" s="109"/>
@@ -5756,7 +5756,7 @@
       <c r="BG73" s="38"/>
     </row>
     <row r="74" spans="1:59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="152"/>
+      <c r="A74" s="117"/>
       <c r="B74" s="111"/>
       <c r="C74" s="110"/>
       <c r="D74" s="111"/>
@@ -5817,7 +5817,7 @@
       <c r="BG74" s="38"/>
     </row>
     <row r="75" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A75" s="124" t="s">
+      <c r="A75" s="116" t="s">
         <v>82</v>
       </c>
       <c r="B75" s="109"/>
@@ -5884,7 +5884,7 @@
       <c r="BG75" s="39"/>
     </row>
     <row r="76" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A76" s="152"/>
+      <c r="A76" s="117"/>
       <c r="B76" s="111"/>
       <c r="C76" s="110"/>
       <c r="D76" s="111"/>
@@ -6006,20 +6006,20 @@
       <c r="BG77" s="3"/>
     </row>
     <row r="78" spans="1:59" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="165" t="s">
+      <c r="A78" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="B78" s="166"/>
-      <c r="C78" s="167">
+      <c r="B78" s="119"/>
+      <c r="C78" s="120">
         <f>SUM(C14+C17+C29+C42+C47+C64+C67+C26 + C70)</f>
         <v>80</v>
       </c>
-      <c r="D78" s="168"/>
-      <c r="E78" s="169">
+      <c r="D78" s="121"/>
+      <c r="E78" s="122">
         <f>SUM(E14+E17+E29+E42+E47+E64+E67+E26+E70)</f>
-        <v>80</v>
-      </c>
-      <c r="F78" s="170"/>
+        <v>89</v>
+      </c>
+      <c r="F78" s="123"/>
       <c r="G78" s="39"/>
       <c r="H78" s="39"/>
       <c r="I78" s="39"/>
@@ -6137,107 +6137,6 @@
     </row>
   </sheetData>
   <mergeCells count="125">
-    <mergeCell ref="A60:B61"/>
-    <mergeCell ref="C60:D61"/>
-    <mergeCell ref="E60:F61"/>
-    <mergeCell ref="A62:B63"/>
-    <mergeCell ref="C62:D63"/>
-    <mergeCell ref="E62:F63"/>
-    <mergeCell ref="A56:B57"/>
-    <mergeCell ref="C56:D57"/>
-    <mergeCell ref="E56:F57"/>
-    <mergeCell ref="A58:B59"/>
-    <mergeCell ref="C58:D59"/>
-    <mergeCell ref="E58:F59"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="A68:B69"/>
-    <mergeCell ref="C68:D69"/>
-    <mergeCell ref="E68:F69"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="A65:B66"/>
-    <mergeCell ref="C65:D66"/>
-    <mergeCell ref="E65:F66"/>
-    <mergeCell ref="A75:B76"/>
-    <mergeCell ref="C75:D76"/>
-    <mergeCell ref="E75:F76"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="A71:B72"/>
-    <mergeCell ref="C71:D72"/>
-    <mergeCell ref="E71:F72"/>
-    <mergeCell ref="A73:B74"/>
-    <mergeCell ref="C73:D74"/>
-    <mergeCell ref="E73:F74"/>
-    <mergeCell ref="A52:B53"/>
-    <mergeCell ref="C52:D53"/>
-    <mergeCell ref="E52:F53"/>
-    <mergeCell ref="A54:B55"/>
-    <mergeCell ref="C54:D55"/>
-    <mergeCell ref="E54:F55"/>
-    <mergeCell ref="A48:B49"/>
-    <mergeCell ref="C48:D49"/>
-    <mergeCell ref="E48:F49"/>
-    <mergeCell ref="A50:B51"/>
-    <mergeCell ref="C50:D51"/>
-    <mergeCell ref="E50:F51"/>
-    <mergeCell ref="A45:B46"/>
-    <mergeCell ref="C45:D46"/>
-    <mergeCell ref="E45:F46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="A40:B41"/>
-    <mergeCell ref="C40:D41"/>
-    <mergeCell ref="E40:F41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="C43:D44"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="A38:B39"/>
-    <mergeCell ref="C38:D39"/>
-    <mergeCell ref="E38:F39"/>
-    <mergeCell ref="A34:B35"/>
-    <mergeCell ref="C34:D35"/>
-    <mergeCell ref="E34:F35"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="E36:F37"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="E30:F31"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:F28"/>
-    <mergeCell ref="C22:D23"/>
-    <mergeCell ref="E22:F23"/>
-    <mergeCell ref="A24:B25"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="E24:F25"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="E20:F21"/>
     <mergeCell ref="A32:B33"/>
     <mergeCell ref="C32:D33"/>
     <mergeCell ref="E32:F33"/>
@@ -6262,6 +6161,107 @@
     <mergeCell ref="C11:D13"/>
     <mergeCell ref="A11:B13"/>
     <mergeCell ref="A22:B23"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="E22:F23"/>
+    <mergeCell ref="A24:B25"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="E24:F25"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="E20:F21"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="E30:F31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:F28"/>
+    <mergeCell ref="A38:B39"/>
+    <mergeCell ref="C38:D39"/>
+    <mergeCell ref="E38:F39"/>
+    <mergeCell ref="A34:B35"/>
+    <mergeCell ref="C34:D35"/>
+    <mergeCell ref="E34:F35"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="E36:F37"/>
+    <mergeCell ref="A45:B46"/>
+    <mergeCell ref="C45:D46"/>
+    <mergeCell ref="E45:F46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="A40:B41"/>
+    <mergeCell ref="C40:D41"/>
+    <mergeCell ref="E40:F41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="C43:D44"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="A52:B53"/>
+    <mergeCell ref="C52:D53"/>
+    <mergeCell ref="E52:F53"/>
+    <mergeCell ref="A54:B55"/>
+    <mergeCell ref="C54:D55"/>
+    <mergeCell ref="E54:F55"/>
+    <mergeCell ref="A48:B49"/>
+    <mergeCell ref="C48:D49"/>
+    <mergeCell ref="E48:F49"/>
+    <mergeCell ref="A50:B51"/>
+    <mergeCell ref="C50:D51"/>
+    <mergeCell ref="E50:F51"/>
+    <mergeCell ref="A75:B76"/>
+    <mergeCell ref="C75:D76"/>
+    <mergeCell ref="E75:F76"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="A71:B72"/>
+    <mergeCell ref="C71:D72"/>
+    <mergeCell ref="E71:F72"/>
+    <mergeCell ref="A73:B74"/>
+    <mergeCell ref="C73:D74"/>
+    <mergeCell ref="E73:F74"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="A68:B69"/>
+    <mergeCell ref="C68:D69"/>
+    <mergeCell ref="E68:F69"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="A65:B66"/>
+    <mergeCell ref="C65:D66"/>
+    <mergeCell ref="E65:F66"/>
+    <mergeCell ref="A60:B61"/>
+    <mergeCell ref="C60:D61"/>
+    <mergeCell ref="E60:F61"/>
+    <mergeCell ref="A62:B63"/>
+    <mergeCell ref="C62:D63"/>
+    <mergeCell ref="E62:F63"/>
+    <mergeCell ref="A56:B57"/>
+    <mergeCell ref="C56:D57"/>
+    <mergeCell ref="E56:F57"/>
+    <mergeCell ref="A58:B59"/>
+    <mergeCell ref="C58:D59"/>
+    <mergeCell ref="E58:F59"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
started documentation of tests
</commit_message>
<xml_diff>
--- a/documentation/Zeitplan.xlsx
+++ b/documentation/Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp8\htdocs\IPA\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35F1886-52A4-4191-AB86-B5BFD85363CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15911069-6BAD-4E50-B48E-33030EE5587A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1267,6 +1267,54 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1277,6 +1325,66 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1303,9 +1411,6 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1318,13 +1423,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1356,105 +1455,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1745,8 +1745,8 @@
   </sheetPr>
   <dimension ref="A1:BG79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="AI63" sqref="AI63:AJ63"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,27 +1759,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:59" ht="44.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="153" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="153"/>
+      <c r="J1" s="153"/>
+      <c r="K1" s="153"/>
+      <c r="L1" s="153"/>
+      <c r="M1" s="153"/>
+      <c r="N1" s="153"/>
+      <c r="O1" s="153"/>
+      <c r="P1" s="153"/>
+      <c r="Q1" s="153"/>
+      <c r="R1" s="153"/>
+      <c r="S1" s="153"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
@@ -2355,86 +2355,86 @@
       <c r="BG10" s="3"/>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A11" s="138" t="s">
+      <c r="A11" s="171" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="139"/>
-      <c r="C11" s="133" t="s">
+      <c r="B11" s="172"/>
+      <c r="C11" s="166" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="134"/>
-      <c r="E11" s="133" t="s">
+      <c r="D11" s="167"/>
+      <c r="E11" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="134"/>
-      <c r="G11" s="118" t="s">
+      <c r="F11" s="167"/>
+      <c r="G11" s="154" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="119"/>
-      <c r="I11" s="119"/>
-      <c r="J11" s="120"/>
-      <c r="K11" s="118" t="s">
+      <c r="H11" s="155"/>
+      <c r="I11" s="155"/>
+      <c r="J11" s="156"/>
+      <c r="K11" s="154" t="s">
         <v>58</v>
       </c>
-      <c r="L11" s="119"/>
-      <c r="M11" s="119"/>
-      <c r="N11" s="120"/>
-      <c r="O11" s="118" t="s">
+      <c r="L11" s="155"/>
+      <c r="M11" s="155"/>
+      <c r="N11" s="156"/>
+      <c r="O11" s="154" t="s">
         <v>59</v>
       </c>
-      <c r="P11" s="119"/>
-      <c r="Q11" s="119"/>
-      <c r="R11" s="120"/>
-      <c r="S11" s="118" t="s">
+      <c r="P11" s="155"/>
+      <c r="Q11" s="155"/>
+      <c r="R11" s="156"/>
+      <c r="S11" s="154" t="s">
         <v>60</v>
       </c>
-      <c r="T11" s="119"/>
-      <c r="U11" s="119"/>
-      <c r="V11" s="120"/>
-      <c r="W11" s="118" t="s">
+      <c r="T11" s="155"/>
+      <c r="U11" s="155"/>
+      <c r="V11" s="156"/>
+      <c r="W11" s="154" t="s">
         <v>61</v>
       </c>
-      <c r="X11" s="119"/>
-      <c r="Y11" s="119"/>
-      <c r="Z11" s="120"/>
-      <c r="AA11" s="118" t="s">
+      <c r="X11" s="155"/>
+      <c r="Y11" s="155"/>
+      <c r="Z11" s="156"/>
+      <c r="AA11" s="154" t="s">
         <v>62</v>
       </c>
-      <c r="AB11" s="119"/>
-      <c r="AC11" s="119"/>
-      <c r="AD11" s="120"/>
-      <c r="AE11" s="118" t="s">
+      <c r="AB11" s="155"/>
+      <c r="AC11" s="155"/>
+      <c r="AD11" s="156"/>
+      <c r="AE11" s="154" t="s">
         <v>63</v>
       </c>
-      <c r="AF11" s="119"/>
-      <c r="AG11" s="119"/>
-      <c r="AH11" s="120"/>
-      <c r="AI11" s="118" t="s">
+      <c r="AF11" s="155"/>
+      <c r="AG11" s="155"/>
+      <c r="AH11" s="156"/>
+      <c r="AI11" s="154" t="s">
         <v>64</v>
       </c>
-      <c r="AJ11" s="119"/>
-      <c r="AK11" s="119"/>
-      <c r="AL11" s="120"/>
-      <c r="AM11" s="118" t="s">
+      <c r="AJ11" s="155"/>
+      <c r="AK11" s="155"/>
+      <c r="AL11" s="156"/>
+      <c r="AM11" s="154" t="s">
         <v>65</v>
       </c>
-      <c r="AN11" s="119"/>
-      <c r="AO11" s="119"/>
-      <c r="AP11" s="120"/>
-      <c r="AQ11" s="118" t="s">
+      <c r="AN11" s="155"/>
+      <c r="AO11" s="155"/>
+      <c r="AP11" s="156"/>
+      <c r="AQ11" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="AR11" s="119"/>
-      <c r="AS11" s="119"/>
-      <c r="AT11" s="120"/>
+      <c r="AR11" s="155"/>
+      <c r="AS11" s="155"/>
+      <c r="AT11" s="156"/>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A12" s="140"/>
-      <c r="B12" s="139"/>
-      <c r="C12" s="135"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="135"/>
-      <c r="F12" s="134"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="172"/>
+      <c r="C12" s="168"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="168"/>
+      <c r="F12" s="167"/>
       <c r="G12" s="10">
         <v>1</v>
       </c>
@@ -2557,12 +2557,12 @@
       </c>
     </row>
     <row r="13" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="141"/>
-      <c r="B13" s="142"/>
-      <c r="C13" s="136"/>
-      <c r="D13" s="137"/>
-      <c r="E13" s="136"/>
-      <c r="F13" s="137"/>
+      <c r="A13" s="174"/>
+      <c r="B13" s="175"/>
+      <c r="C13" s="169"/>
+      <c r="D13" s="170"/>
+      <c r="E13" s="169"/>
+      <c r="F13" s="170"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
@@ -2605,20 +2605,20 @@
       <c r="AT13" s="16"/>
     </row>
     <row r="14" spans="1:59" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="157" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="122"/>
-      <c r="C14" s="123">
+      <c r="B14" s="158"/>
+      <c r="C14" s="159">
         <f>SUM(C15:D16)</f>
         <v>6</v>
       </c>
-      <c r="D14" s="124"/>
-      <c r="E14" s="123">
+      <c r="D14" s="160"/>
+      <c r="E14" s="159">
         <f>SUM(E15)</f>
         <v>6</v>
       </c>
-      <c r="F14" s="124"/>
+      <c r="F14" s="160"/>
       <c r="G14" s="18"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
@@ -2661,18 +2661,18 @@
       <c r="AT14" s="20"/>
     </row>
     <row r="15" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="125" t="s">
+      <c r="A15" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="126"/>
-      <c r="C15" s="129">
+      <c r="B15" s="161"/>
+      <c r="C15" s="164">
         <v>6</v>
       </c>
-      <c r="D15" s="130"/>
-      <c r="E15" s="129">
+      <c r="D15" s="137"/>
+      <c r="E15" s="164">
         <v>6</v>
       </c>
-      <c r="F15" s="130"/>
+      <c r="F15" s="137"/>
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
       <c r="I15" s="26"/>
@@ -2715,12 +2715,12 @@
       <c r="AT15" s="50"/>
     </row>
     <row r="16" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="127"/>
-      <c r="B16" s="128"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="132"/>
+      <c r="A16" s="162"/>
+      <c r="B16" s="163"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="139"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="139"/>
       <c r="G16" s="30"/>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
@@ -2756,20 +2756,20 @@
       <c r="AT16" s="54"/>
     </row>
     <row r="17" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="147" t="s">
+      <c r="A17" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="148"/>
-      <c r="C17" s="149">
+      <c r="B17" s="114"/>
+      <c r="C17" s="115">
         <f>SUM(C18:D25)</f>
         <v>12</v>
       </c>
-      <c r="D17" s="150"/>
-      <c r="E17" s="151">
+      <c r="D17" s="116"/>
+      <c r="E17" s="147">
         <f>SUM(E18:F25)</f>
         <v>10</v>
       </c>
-      <c r="F17" s="152"/>
+      <c r="F17" s="148"/>
       <c r="G17" s="31"/>
       <c r="H17" s="32"/>
       <c r="I17" s="32"/>
@@ -2812,7 +2812,7 @@
       <c r="AT17" s="33"/>
     </row>
     <row r="18" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="125" t="s">
+      <c r="A18" s="117" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="110"/>
@@ -2866,7 +2866,7 @@
       <c r="AT18" s="35"/>
     </row>
     <row r="19" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="153"/>
+      <c r="A19" s="118"/>
       <c r="B19" s="112"/>
       <c r="C19" s="111"/>
       <c r="D19" s="112"/>
@@ -2914,7 +2914,7 @@
       <c r="AT19" s="35"/>
     </row>
     <row r="20" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="125" t="s">
+      <c r="A20" s="117" t="s">
         <v>67</v>
       </c>
       <c r="B20" s="110"/>
@@ -2968,7 +2968,7 @@
       <c r="AT20" s="35"/>
     </row>
     <row r="21" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="153"/>
+      <c r="A21" s="118"/>
       <c r="B21" s="112"/>
       <c r="C21" s="111"/>
       <c r="D21" s="112"/>
@@ -3125,10 +3125,10 @@
         <v>2</v>
       </c>
       <c r="D24" s="110"/>
-      <c r="E24" s="143">
+      <c r="E24" s="149">
         <v>2</v>
       </c>
-      <c r="F24" s="144"/>
+      <c r="F24" s="150"/>
       <c r="G24" s="25"/>
       <c r="H24" s="81"/>
       <c r="I24" s="26"/>
@@ -3177,8 +3177,8 @@
       <c r="B25" s="108"/>
       <c r="C25" s="111"/>
       <c r="D25" s="112"/>
-      <c r="E25" s="145"/>
-      <c r="F25" s="146"/>
+      <c r="E25" s="151"/>
+      <c r="F25" s="152"/>
       <c r="G25" s="25"/>
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
@@ -3223,20 +3223,20 @@
       <c r="AT25" s="35"/>
     </row>
     <row r="26" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="147" t="s">
+      <c r="A26" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="148"/>
-      <c r="C26" s="149">
+      <c r="B26" s="114"/>
+      <c r="C26" s="115">
         <f>SUM(C27)</f>
         <v>2</v>
       </c>
-      <c r="D26" s="150"/>
-      <c r="E26" s="151">
+      <c r="D26" s="116"/>
+      <c r="E26" s="147">
         <f>SUM(E27)</f>
         <v>3</v>
       </c>
-      <c r="F26" s="152"/>
+      <c r="F26" s="148"/>
       <c r="G26" s="31"/>
       <c r="H26" s="32"/>
       <c r="I26" s="32"/>
@@ -3279,7 +3279,7 @@
       <c r="AT26" s="33"/>
     </row>
     <row r="27" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="125" t="s">
+      <c r="A27" s="117" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="110"/>
@@ -3334,7 +3334,7 @@
       <c r="AT27" s="35"/>
     </row>
     <row r="28" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="153"/>
+      <c r="A28" s="118"/>
       <c r="B28" s="112"/>
       <c r="C28" s="111"/>
       <c r="D28" s="112"/>
@@ -3384,20 +3384,20 @@
       <c r="AT28" s="35"/>
     </row>
     <row r="29" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="147" t="s">
+      <c r="A29" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="148"/>
-      <c r="C29" s="149">
+      <c r="B29" s="114"/>
+      <c r="C29" s="115">
         <f>SUM(C30:D41)</f>
         <v>12</v>
       </c>
-      <c r="D29" s="150"/>
-      <c r="E29" s="149">
+      <c r="D29" s="116"/>
+      <c r="E29" s="115">
         <f>SUM(E30:F41)</f>
         <v>25</v>
       </c>
-      <c r="F29" s="150"/>
+      <c r="F29" s="116"/>
       <c r="G29" s="31"/>
       <c r="H29" s="32"/>
       <c r="I29" s="32"/>
@@ -3448,10 +3448,10 @@
         <v>2</v>
       </c>
       <c r="D30" s="110"/>
-      <c r="E30" s="113">
+      <c r="E30" s="129">
         <v>1</v>
       </c>
-      <c r="F30" s="114"/>
+      <c r="F30" s="130"/>
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
@@ -3498,8 +3498,8 @@
       <c r="B31" s="108"/>
       <c r="C31" s="111"/>
       <c r="D31" s="112"/>
-      <c r="E31" s="115"/>
-      <c r="F31" s="116"/>
+      <c r="E31" s="131"/>
+      <c r="F31" s="132"/>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
@@ -3550,10 +3550,10 @@
         <v>2</v>
       </c>
       <c r="D32" s="110"/>
-      <c r="E32" s="113">
+      <c r="E32" s="129">
         <v>2</v>
       </c>
-      <c r="F32" s="114"/>
+      <c r="F32" s="130"/>
       <c r="G32" s="25"/>
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
@@ -3600,8 +3600,8 @@
       <c r="B33" s="108"/>
       <c r="C33" s="111"/>
       <c r="D33" s="112"/>
-      <c r="E33" s="115"/>
-      <c r="F33" s="116"/>
+      <c r="E33" s="131"/>
+      <c r="F33" s="132"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3848,7 +3848,7 @@
       <c r="AT37" s="35"/>
     </row>
     <row r="38" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="125" t="s">
+      <c r="A38" s="117" t="s">
         <v>31</v>
       </c>
       <c r="B38" s="110"/>
@@ -3902,7 +3902,7 @@
       <c r="AT38" s="35"/>
     </row>
     <row r="39" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="153"/>
+      <c r="A39" s="118"/>
       <c r="B39" s="112"/>
       <c r="C39" s="111"/>
       <c r="D39" s="112"/>
@@ -4056,20 +4056,20 @@
       <c r="AT41" s="35"/>
     </row>
     <row r="42" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="147" t="s">
+      <c r="A42" s="113" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="148"/>
-      <c r="C42" s="149">
+      <c r="B42" s="114"/>
+      <c r="C42" s="115">
         <f>SUM(C43:C45)</f>
         <v>3</v>
       </c>
-      <c r="D42" s="150"/>
-      <c r="E42" s="149">
+      <c r="D42" s="116"/>
+      <c r="E42" s="115">
         <f>SUM(E45+E43)</f>
         <v>2</v>
       </c>
-      <c r="F42" s="150"/>
+      <c r="F42" s="116"/>
       <c r="G42" s="31"/>
       <c r="H42" s="32"/>
       <c r="I42" s="32"/>
@@ -4112,18 +4112,18 @@
       <c r="AT42" s="33"/>
     </row>
     <row r="43" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="155" t="s">
+      <c r="A43" s="140" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="156"/>
-      <c r="C43" s="155">
+      <c r="B43" s="141"/>
+      <c r="C43" s="140">
         <v>2</v>
       </c>
-      <c r="D43" s="159"/>
-      <c r="E43" s="155">
+      <c r="D43" s="144"/>
+      <c r="E43" s="140">
         <v>1</v>
       </c>
-      <c r="F43" s="159"/>
+      <c r="F43" s="144"/>
       <c r="G43" s="84"/>
       <c r="H43" s="81"/>
       <c r="I43" s="81"/>
@@ -4166,12 +4166,12 @@
       <c r="AT43" s="54"/>
     </row>
     <row r="44" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="157"/>
-      <c r="B44" s="158"/>
-      <c r="C44" s="160"/>
-      <c r="D44" s="161"/>
-      <c r="E44" s="160"/>
-      <c r="F44" s="161"/>
+      <c r="A44" s="142"/>
+      <c r="B44" s="143"/>
+      <c r="C44" s="145"/>
+      <c r="D44" s="146"/>
+      <c r="E44" s="145"/>
+      <c r="F44" s="146"/>
       <c r="G44" s="84"/>
       <c r="H44" s="81"/>
       <c r="I44" s="81"/>
@@ -4214,10 +4214,10 @@
       <c r="AT44" s="54"/>
     </row>
     <row r="45" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="125" t="s">
+      <c r="A45" s="117" t="s">
         <v>69</v>
       </c>
-      <c r="B45" s="130"/>
+      <c r="B45" s="137"/>
       <c r="C45" s="109">
         <v>1</v>
       </c>
@@ -4270,8 +4270,8 @@
       <c r="AT45" s="35"/>
     </row>
     <row r="46" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="154"/>
-      <c r="B46" s="132"/>
+      <c r="A46" s="138"/>
+      <c r="B46" s="139"/>
       <c r="C46" s="111"/>
       <c r="D46" s="112"/>
       <c r="E46" s="111"/>
@@ -4320,20 +4320,20 @@
       <c r="AT46" s="35"/>
     </row>
     <row r="47" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="147" t="s">
+      <c r="A47" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="148"/>
-      <c r="C47" s="149">
+      <c r="B47" s="114"/>
+      <c r="C47" s="115">
         <f>SUM(C48:D63)</f>
         <v>19</v>
       </c>
-      <c r="D47" s="150"/>
-      <c r="E47" s="149">
+      <c r="D47" s="116"/>
+      <c r="E47" s="115">
         <f>SUM(E48:F63)</f>
-        <v>17</v>
-      </c>
-      <c r="F47" s="150"/>
+        <v>14</v>
+      </c>
+      <c r="F47" s="116"/>
       <c r="G47" s="31"/>
       <c r="H47" s="32"/>
       <c r="I47" s="32"/>
@@ -4376,10 +4376,10 @@
       <c r="AT47" s="33"/>
     </row>
     <row r="48" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="162" t="s">
+      <c r="A48" s="133" t="s">
         <v>74</v>
       </c>
-      <c r="B48" s="163"/>
+      <c r="B48" s="134"/>
       <c r="C48" s="109">
         <v>0.5</v>
       </c>
@@ -4430,8 +4430,8 @@
       <c r="AT48" s="35"/>
     </row>
     <row r="49" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="164"/>
-      <c r="B49" s="165"/>
+      <c r="A49" s="135"/>
+      <c r="B49" s="136"/>
       <c r="C49" s="111"/>
       <c r="D49" s="112"/>
       <c r="E49" s="111"/>
@@ -4478,7 +4478,7 @@
       <c r="AT49" s="35"/>
     </row>
     <row r="50" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A50" s="125" t="s">
+      <c r="A50" s="117" t="s">
         <v>75</v>
       </c>
       <c r="B50" s="110"/>
@@ -4486,10 +4486,10 @@
         <v>0.5</v>
       </c>
       <c r="D50" s="110"/>
-      <c r="E50" s="113">
+      <c r="E50" s="129">
         <v>0.5</v>
       </c>
-      <c r="F50" s="114"/>
+      <c r="F50" s="130"/>
       <c r="G50" s="25"/>
       <c r="H50" s="26"/>
       <c r="I50" s="26"/>
@@ -4532,12 +4532,12 @@
       <c r="AT50" s="35"/>
     </row>
     <row r="51" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="153"/>
+      <c r="A51" s="118"/>
       <c r="B51" s="112"/>
       <c r="C51" s="111"/>
       <c r="D51" s="112"/>
-      <c r="E51" s="115"/>
-      <c r="F51" s="116"/>
+      <c r="E51" s="131"/>
+      <c r="F51" s="132"/>
       <c r="G51" s="25"/>
       <c r="H51" s="26"/>
       <c r="I51" s="26"/>
@@ -4580,7 +4580,7 @@
       <c r="AT51" s="35"/>
     </row>
     <row r="52" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A52" s="125" t="s">
+      <c r="A52" s="117" t="s">
         <v>76</v>
       </c>
       <c r="B52" s="110"/>
@@ -4588,10 +4588,10 @@
         <v>2</v>
       </c>
       <c r="D52" s="110"/>
-      <c r="E52" s="113">
+      <c r="E52" s="129">
         <v>1.5</v>
       </c>
-      <c r="F52" s="114"/>
+      <c r="F52" s="130"/>
       <c r="G52" s="25"/>
       <c r="H52" s="26"/>
       <c r="I52" s="26"/>
@@ -4634,12 +4634,12 @@
       <c r="AT52" s="35"/>
     </row>
     <row r="53" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="153"/>
+      <c r="A53" s="118"/>
       <c r="B53" s="112"/>
       <c r="C53" s="111"/>
       <c r="D53" s="112"/>
-      <c r="E53" s="115"/>
-      <c r="F53" s="116"/>
+      <c r="E53" s="131"/>
+      <c r="F53" s="132"/>
       <c r="G53" s="25"/>
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
@@ -4682,7 +4682,7 @@
       <c r="AT53" s="35"/>
     </row>
     <row r="54" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="125" t="s">
+      <c r="A54" s="117" t="s">
         <v>78</v>
       </c>
       <c r="B54" s="110"/>
@@ -4690,10 +4690,10 @@
         <v>2</v>
       </c>
       <c r="D54" s="110"/>
-      <c r="E54" s="113">
+      <c r="E54" s="129">
         <v>1.5</v>
       </c>
-      <c r="F54" s="114"/>
+      <c r="F54" s="130"/>
       <c r="G54" s="25"/>
       <c r="H54" s="26"/>
       <c r="I54" s="26"/>
@@ -4736,12 +4736,12 @@
       <c r="AT54" s="35"/>
     </row>
     <row r="55" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="153"/>
+      <c r="A55" s="118"/>
       <c r="B55" s="112"/>
       <c r="C55" s="111"/>
       <c r="D55" s="112"/>
-      <c r="E55" s="115"/>
-      <c r="F55" s="116"/>
+      <c r="E55" s="131"/>
+      <c r="F55" s="132"/>
       <c r="G55" s="25"/>
       <c r="H55" s="26"/>
       <c r="I55" s="26"/>
@@ -4792,7 +4792,7 @@
       </c>
       <c r="D56" s="110"/>
       <c r="E56" s="109">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F56" s="110"/>
       <c r="G56" s="25"/>
@@ -4894,7 +4894,7 @@
       </c>
       <c r="D58" s="110"/>
       <c r="E58" s="109">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F58" s="110"/>
       <c r="G58" s="25"/>
@@ -4996,7 +4996,7 @@
       </c>
       <c r="D60" s="110"/>
       <c r="E60" s="109">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F60" s="110"/>
       <c r="G60" s="25"/>
@@ -5193,20 +5193,20 @@
       <c r="AT63" s="35"/>
     </row>
     <row r="64" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="147" t="s">
+      <c r="A64" s="113" t="s">
         <v>39</v>
       </c>
-      <c r="B64" s="148"/>
-      <c r="C64" s="149">
+      <c r="B64" s="114"/>
+      <c r="C64" s="115">
         <f>SUM(C65:D66)</f>
         <v>4</v>
       </c>
-      <c r="D64" s="150"/>
-      <c r="E64" s="149">
+      <c r="D64" s="116"/>
+      <c r="E64" s="115">
         <f>SUM(E65)</f>
         <v>4</v>
       </c>
-      <c r="F64" s="150"/>
+      <c r="F64" s="116"/>
       <c r="G64" s="31"/>
       <c r="H64" s="32"/>
       <c r="I64" s="32"/>
@@ -5249,7 +5249,7 @@
       <c r="AT64" s="33"/>
     </row>
     <row r="65" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="125" t="s">
+      <c r="A65" s="117" t="s">
         <v>40</v>
       </c>
       <c r="B65" s="110"/>
@@ -5305,7 +5305,7 @@
       <c r="AT65" s="35"/>
     </row>
     <row r="66" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="153"/>
+      <c r="A66" s="118"/>
       <c r="B66" s="112"/>
       <c r="C66" s="111"/>
       <c r="D66" s="112"/>
@@ -5341,8 +5341,8 @@
       <c r="AH66" s="58"/>
       <c r="AI66" s="86"/>
       <c r="AJ66" s="26"/>
-      <c r="AK66" s="26"/>
-      <c r="AL66" s="56"/>
+      <c r="AK66" s="55"/>
+      <c r="AL66" s="70"/>
       <c r="AM66" s="27"/>
       <c r="AN66" s="26"/>
       <c r="AO66" s="26"/>
@@ -5353,20 +5353,20 @@
       <c r="AT66" s="35"/>
     </row>
     <row r="67" spans="1:59" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="147" t="s">
+      <c r="A67" s="113" t="s">
         <v>42</v>
       </c>
-      <c r="B67" s="148"/>
-      <c r="C67" s="149">
+      <c r="B67" s="114"/>
+      <c r="C67" s="115">
         <f>SUM(C68:D69)</f>
         <v>4</v>
       </c>
-      <c r="D67" s="150"/>
-      <c r="E67" s="149">
+      <c r="D67" s="116"/>
+      <c r="E67" s="115">
         <f>SUM(E68)</f>
         <v>4</v>
       </c>
-      <c r="F67" s="150"/>
+      <c r="F67" s="116"/>
       <c r="G67" s="31"/>
       <c r="H67" s="32"/>
       <c r="I67" s="32"/>
@@ -5409,7 +5409,7 @@
       <c r="AT67" s="33"/>
     </row>
     <row r="68" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A68" s="125" t="s">
+      <c r="A68" s="117" t="s">
         <v>43</v>
       </c>
       <c r="B68" s="110"/>
@@ -5466,7 +5466,7 @@
       <c r="AU68" s="38"/>
     </row>
     <row r="69" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A69" s="153"/>
+      <c r="A69" s="118"/>
       <c r="B69" s="112"/>
       <c r="C69" s="111"/>
       <c r="D69" s="112"/>
@@ -5515,20 +5515,20 @@
       <c r="AU69" s="39"/>
     </row>
     <row r="70" spans="1:59" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="172" t="s">
+      <c r="A70" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="B70" s="173"/>
-      <c r="C70" s="174">
+      <c r="B70" s="126"/>
+      <c r="C70" s="127">
         <f>SUM(C71:D76)</f>
         <v>18</v>
       </c>
-      <c r="D70" s="175"/>
-      <c r="E70" s="149">
+      <c r="D70" s="128"/>
+      <c r="E70" s="115">
         <f>SUM(E71:F76)</f>
         <v>18</v>
       </c>
-      <c r="F70" s="150"/>
+      <c r="F70" s="116"/>
       <c r="G70" s="40"/>
       <c r="H70" s="41"/>
       <c r="I70" s="41"/>
@@ -5572,7 +5572,7 @@
       <c r="AU70" s="3"/>
     </row>
     <row r="71" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A71" s="125" t="s">
+      <c r="A71" s="117" t="s">
         <v>46</v>
       </c>
       <c r="B71" s="110"/>
@@ -5627,7 +5627,7 @@
       <c r="AU71" s="3"/>
     </row>
     <row r="72" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A72" s="153"/>
+      <c r="A72" s="118"/>
       <c r="B72" s="112"/>
       <c r="C72" s="111"/>
       <c r="D72" s="112"/>
@@ -5688,7 +5688,7 @@
       <c r="BG72" s="38"/>
     </row>
     <row r="73" spans="1:59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="125" t="s">
+      <c r="A73" s="117" t="s">
         <v>47</v>
       </c>
       <c r="B73" s="110"/>
@@ -5757,7 +5757,7 @@
       <c r="BG73" s="38"/>
     </row>
     <row r="74" spans="1:59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="153"/>
+      <c r="A74" s="118"/>
       <c r="B74" s="112"/>
       <c r="C74" s="111"/>
       <c r="D74" s="112"/>
@@ -5818,7 +5818,7 @@
       <c r="BG74" s="38"/>
     </row>
     <row r="75" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A75" s="125" t="s">
+      <c r="A75" s="117" t="s">
         <v>82</v>
       </c>
       <c r="B75" s="110"/>
@@ -5885,7 +5885,7 @@
       <c r="BG75" s="39"/>
     </row>
     <row r="76" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A76" s="153"/>
+      <c r="A76" s="118"/>
       <c r="B76" s="112"/>
       <c r="C76" s="111"/>
       <c r="D76" s="112"/>
@@ -6007,20 +6007,20 @@
       <c r="BG77" s="3"/>
     </row>
     <row r="78" spans="1:59" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="166" t="s">
+      <c r="A78" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="B78" s="167"/>
-      <c r="C78" s="168">
+      <c r="B78" s="120"/>
+      <c r="C78" s="121">
         <f>SUM(C14+C17+C29+C42+C47+C64+C67+C26 + C70)</f>
         <v>80</v>
       </c>
-      <c r="D78" s="169"/>
-      <c r="E78" s="170">
+      <c r="D78" s="122"/>
+      <c r="E78" s="123">
         <f>SUM(E14+E17+E29+E42+E47+E64+E67+E26+E70)</f>
-        <v>89</v>
-      </c>
-      <c r="F78" s="171"/>
+        <v>86</v>
+      </c>
+      <c r="F78" s="124"/>
       <c r="G78" s="39"/>
       <c r="H78" s="39"/>
       <c r="I78" s="39"/>
@@ -6138,107 +6138,6 @@
     </row>
   </sheetData>
   <mergeCells count="125">
-    <mergeCell ref="A60:B61"/>
-    <mergeCell ref="C60:D61"/>
-    <mergeCell ref="E60:F61"/>
-    <mergeCell ref="A62:B63"/>
-    <mergeCell ref="C62:D63"/>
-    <mergeCell ref="E62:F63"/>
-    <mergeCell ref="A56:B57"/>
-    <mergeCell ref="C56:D57"/>
-    <mergeCell ref="E56:F57"/>
-    <mergeCell ref="A58:B59"/>
-    <mergeCell ref="C58:D59"/>
-    <mergeCell ref="E58:F59"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="A68:B69"/>
-    <mergeCell ref="C68:D69"/>
-    <mergeCell ref="E68:F69"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="A65:B66"/>
-    <mergeCell ref="C65:D66"/>
-    <mergeCell ref="E65:F66"/>
-    <mergeCell ref="A75:B76"/>
-    <mergeCell ref="C75:D76"/>
-    <mergeCell ref="E75:F76"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="A71:B72"/>
-    <mergeCell ref="C71:D72"/>
-    <mergeCell ref="E71:F72"/>
-    <mergeCell ref="A73:B74"/>
-    <mergeCell ref="C73:D74"/>
-    <mergeCell ref="E73:F74"/>
-    <mergeCell ref="A52:B53"/>
-    <mergeCell ref="C52:D53"/>
-    <mergeCell ref="E52:F53"/>
-    <mergeCell ref="A54:B55"/>
-    <mergeCell ref="C54:D55"/>
-    <mergeCell ref="E54:F55"/>
-    <mergeCell ref="A48:B49"/>
-    <mergeCell ref="C48:D49"/>
-    <mergeCell ref="E48:F49"/>
-    <mergeCell ref="A50:B51"/>
-    <mergeCell ref="C50:D51"/>
-    <mergeCell ref="E50:F51"/>
-    <mergeCell ref="A45:B46"/>
-    <mergeCell ref="C45:D46"/>
-    <mergeCell ref="E45:F46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="A40:B41"/>
-    <mergeCell ref="C40:D41"/>
-    <mergeCell ref="E40:F41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="C43:D44"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="A38:B39"/>
-    <mergeCell ref="C38:D39"/>
-    <mergeCell ref="E38:F39"/>
-    <mergeCell ref="A34:B35"/>
-    <mergeCell ref="C34:D35"/>
-    <mergeCell ref="E34:F35"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="E36:F37"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="E30:F31"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:F28"/>
-    <mergeCell ref="C22:D23"/>
-    <mergeCell ref="E22:F23"/>
-    <mergeCell ref="A24:B25"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="E24:F25"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="E20:F21"/>
     <mergeCell ref="A32:B33"/>
     <mergeCell ref="C32:D33"/>
     <mergeCell ref="E32:F33"/>
@@ -6263,6 +6162,107 @@
     <mergeCell ref="C11:D13"/>
     <mergeCell ref="A11:B13"/>
     <mergeCell ref="A22:B23"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="E22:F23"/>
+    <mergeCell ref="A24:B25"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="E24:F25"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="E20:F21"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="E30:F31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:F28"/>
+    <mergeCell ref="A38:B39"/>
+    <mergeCell ref="C38:D39"/>
+    <mergeCell ref="E38:F39"/>
+    <mergeCell ref="A34:B35"/>
+    <mergeCell ref="C34:D35"/>
+    <mergeCell ref="E34:F35"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="E36:F37"/>
+    <mergeCell ref="A45:B46"/>
+    <mergeCell ref="C45:D46"/>
+    <mergeCell ref="E45:F46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="A40:B41"/>
+    <mergeCell ref="C40:D41"/>
+    <mergeCell ref="E40:F41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="C43:D44"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="A52:B53"/>
+    <mergeCell ref="C52:D53"/>
+    <mergeCell ref="E52:F53"/>
+    <mergeCell ref="A54:B55"/>
+    <mergeCell ref="C54:D55"/>
+    <mergeCell ref="E54:F55"/>
+    <mergeCell ref="A48:B49"/>
+    <mergeCell ref="C48:D49"/>
+    <mergeCell ref="E48:F49"/>
+    <mergeCell ref="A50:B51"/>
+    <mergeCell ref="C50:D51"/>
+    <mergeCell ref="E50:F51"/>
+    <mergeCell ref="A75:B76"/>
+    <mergeCell ref="C75:D76"/>
+    <mergeCell ref="E75:F76"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="A71:B72"/>
+    <mergeCell ref="C71:D72"/>
+    <mergeCell ref="E71:F72"/>
+    <mergeCell ref="A73:B74"/>
+    <mergeCell ref="C73:D74"/>
+    <mergeCell ref="E73:F74"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="A68:B69"/>
+    <mergeCell ref="C68:D69"/>
+    <mergeCell ref="E68:F69"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="A65:B66"/>
+    <mergeCell ref="C65:D66"/>
+    <mergeCell ref="E65:F66"/>
+    <mergeCell ref="A60:B61"/>
+    <mergeCell ref="C60:D61"/>
+    <mergeCell ref="E60:F61"/>
+    <mergeCell ref="A62:B63"/>
+    <mergeCell ref="C62:D63"/>
+    <mergeCell ref="E62:F63"/>
+    <mergeCell ref="A56:B57"/>
+    <mergeCell ref="C56:D57"/>
+    <mergeCell ref="E56:F57"/>
+    <mergeCell ref="A58:B59"/>
+    <mergeCell ref="C58:D59"/>
+    <mergeCell ref="E58:F59"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
set up project on laptop
</commit_message>
<xml_diff>
--- a/documentation/Zeitplan.xlsx
+++ b/documentation/Zeitplan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp8\htdocs\IPA\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IPA\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9936B52C-7074-42B4-BE63-C9E202F35F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1F22A4-9D1B-4123-91BB-BF740B9C6899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -107,9 +107,6 @@
     <t>Zeitplan erstellen</t>
   </si>
   <si>
-    <t>Ist Meolenstein</t>
-  </si>
-  <si>
     <t>Vorbereitung dokumentieren</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
     <t>Klassendiagramm erstellen</t>
   </si>
   <si>
-    <t>Larvel-Projekt vorbereiten</t>
-  </si>
-  <si>
     <t>API-Routen erstellen</t>
   </si>
   <si>
@@ -288,6 +282,12 @@
   </si>
   <si>
     <t>Aktivitätsdiagramm erstellen</t>
+  </si>
+  <si>
+    <t>Ist Meilenstein</t>
+  </si>
+  <si>
+    <t>Laravel-Projekt vorbereiten</t>
   </si>
 </sst>
 </file>
@@ -1242,6 +1242,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="2" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1266,6 +1267,54 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1276,6 +1325,66 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1302,9 +1411,6 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1317,13 +1423,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1356,113 +1456,13 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Eingabe" xfId="4" builtinId="20"/>
-    <cellStyle name="Gut" xfId="2" builtinId="26"/>
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1745,11 +1745,11 @@
   </sheetPr>
   <dimension ref="A1:BG79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="AL61" sqref="AL61"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="80.7109375" customWidth="1"/>
@@ -1759,27 +1759,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:59" ht="44.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116"/>
-      <c r="N1" s="116"/>
-      <c r="O1" s="116"/>
-      <c r="P1" s="116"/>
-      <c r="Q1" s="116"/>
-      <c r="R1" s="116"/>
-      <c r="S1" s="116"/>
+      <c r="A1" s="153" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="153"/>
+      <c r="J1" s="153"/>
+      <c r="K1" s="153"/>
+      <c r="L1" s="153"/>
+      <c r="M1" s="153"/>
+      <c r="N1" s="153"/>
+      <c r="O1" s="153"/>
+      <c r="P1" s="153"/>
+      <c r="Q1" s="153"/>
+      <c r="R1" s="153"/>
+      <c r="S1" s="153"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="4" t="s">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G6" s="44"/>
       <c r="H6" s="44"/>
@@ -2121,7 +2121,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="4" t="s">
@@ -2166,7 +2166,7 @@
         <v>20</v>
       </c>
       <c r="AO7" s="28" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="AT7" s="29"/>
       <c r="AV7" s="3"/>
@@ -2187,15 +2187,15 @@
         <v>10</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -2283,7 +2283,7 @@
       <c r="AL9" s="3"/>
       <c r="AN9" s="68"/>
       <c r="AO9" s="69" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AP9" s="36"/>
       <c r="AQ9" s="36"/>
@@ -2355,86 +2355,86 @@
       <c r="BG10" s="3"/>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A11" s="137" t="s">
+      <c r="A11" s="171" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="138"/>
-      <c r="C11" s="132" t="s">
+      <c r="B11" s="172"/>
+      <c r="C11" s="166" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="133"/>
-      <c r="E11" s="132" t="s">
+      <c r="D11" s="167"/>
+      <c r="E11" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="133"/>
-      <c r="G11" s="117" t="s">
+      <c r="F11" s="167"/>
+      <c r="G11" s="154" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="155"/>
+      <c r="I11" s="155"/>
+      <c r="J11" s="156"/>
+      <c r="K11" s="154" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="118"/>
-      <c r="I11" s="118"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="117" t="s">
+      <c r="L11" s="155"/>
+      <c r="M11" s="155"/>
+      <c r="N11" s="156"/>
+      <c r="O11" s="154" t="s">
         <v>58</v>
       </c>
-      <c r="L11" s="118"/>
-      <c r="M11" s="118"/>
-      <c r="N11" s="119"/>
-      <c r="O11" s="117" t="s">
+      <c r="P11" s="155"/>
+      <c r="Q11" s="155"/>
+      <c r="R11" s="156"/>
+      <c r="S11" s="154" t="s">
         <v>59</v>
       </c>
-      <c r="P11" s="118"/>
-      <c r="Q11" s="118"/>
-      <c r="R11" s="119"/>
-      <c r="S11" s="117" t="s">
+      <c r="T11" s="155"/>
+      <c r="U11" s="155"/>
+      <c r="V11" s="156"/>
+      <c r="W11" s="154" t="s">
         <v>60</v>
       </c>
-      <c r="T11" s="118"/>
-      <c r="U11" s="118"/>
-      <c r="V11" s="119"/>
-      <c r="W11" s="117" t="s">
+      <c r="X11" s="155"/>
+      <c r="Y11" s="155"/>
+      <c r="Z11" s="156"/>
+      <c r="AA11" s="154" t="s">
         <v>61</v>
       </c>
-      <c r="X11" s="118"/>
-      <c r="Y11" s="118"/>
-      <c r="Z11" s="119"/>
-      <c r="AA11" s="117" t="s">
+      <c r="AB11" s="155"/>
+      <c r="AC11" s="155"/>
+      <c r="AD11" s="156"/>
+      <c r="AE11" s="154" t="s">
         <v>62</v>
       </c>
-      <c r="AB11" s="118"/>
-      <c r="AC11" s="118"/>
-      <c r="AD11" s="119"/>
-      <c r="AE11" s="117" t="s">
+      <c r="AF11" s="155"/>
+      <c r="AG11" s="155"/>
+      <c r="AH11" s="156"/>
+      <c r="AI11" s="154" t="s">
         <v>63</v>
       </c>
-      <c r="AF11" s="118"/>
-      <c r="AG11" s="118"/>
-      <c r="AH11" s="119"/>
-      <c r="AI11" s="117" t="s">
+      <c r="AJ11" s="155"/>
+      <c r="AK11" s="155"/>
+      <c r="AL11" s="156"/>
+      <c r="AM11" s="154" t="s">
         <v>64</v>
       </c>
-      <c r="AJ11" s="118"/>
-      <c r="AK11" s="118"/>
-      <c r="AL11" s="119"/>
-      <c r="AM11" s="117" t="s">
+      <c r="AN11" s="155"/>
+      <c r="AO11" s="155"/>
+      <c r="AP11" s="156"/>
+      <c r="AQ11" s="154" t="s">
         <v>65</v>
       </c>
-      <c r="AN11" s="118"/>
-      <c r="AO11" s="118"/>
-      <c r="AP11" s="119"/>
-      <c r="AQ11" s="117" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR11" s="118"/>
-      <c r="AS11" s="118"/>
-      <c r="AT11" s="119"/>
+      <c r="AR11" s="155"/>
+      <c r="AS11" s="155"/>
+      <c r="AT11" s="156"/>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A12" s="139"/>
-      <c r="B12" s="138"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="133"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="172"/>
+      <c r="C12" s="168"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="168"/>
+      <c r="F12" s="167"/>
       <c r="G12" s="10">
         <v>1</v>
       </c>
@@ -2557,12 +2557,12 @@
       </c>
     </row>
     <row r="13" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="140"/>
-      <c r="B13" s="141"/>
-      <c r="C13" s="135"/>
-      <c r="D13" s="136"/>
-      <c r="E13" s="135"/>
-      <c r="F13" s="136"/>
+      <c r="A13" s="174"/>
+      <c r="B13" s="175"/>
+      <c r="C13" s="169"/>
+      <c r="D13" s="170"/>
+      <c r="E13" s="169"/>
+      <c r="F13" s="170"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
@@ -2605,20 +2605,20 @@
       <c r="AT13" s="16"/>
     </row>
     <row r="14" spans="1:59" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="120" t="s">
+      <c r="A14" s="157" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="121"/>
-      <c r="C14" s="122">
+      <c r="B14" s="158"/>
+      <c r="C14" s="159">
         <f>SUM(C15:D16)</f>
         <v>6</v>
       </c>
-      <c r="D14" s="123"/>
-      <c r="E14" s="122">
+      <c r="D14" s="160"/>
+      <c r="E14" s="159">
         <f>SUM(E15)</f>
         <v>6</v>
       </c>
-      <c r="F14" s="123"/>
+      <c r="F14" s="160"/>
       <c r="G14" s="18"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
@@ -2661,18 +2661,18 @@
       <c r="AT14" s="20"/>
     </row>
     <row r="15" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="124" t="s">
+      <c r="A15" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="125"/>
-      <c r="C15" s="128">
+      <c r="B15" s="161"/>
+      <c r="C15" s="164">
         <v>6</v>
       </c>
-      <c r="D15" s="129"/>
-      <c r="E15" s="128">
+      <c r="D15" s="137"/>
+      <c r="E15" s="164">
         <v>6</v>
       </c>
-      <c r="F15" s="129"/>
+      <c r="F15" s="137"/>
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
       <c r="I15" s="26"/>
@@ -2715,12 +2715,12 @@
       <c r="AT15" s="50"/>
     </row>
     <row r="16" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="126"/>
-      <c r="B16" s="127"/>
-      <c r="C16" s="130"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="130"/>
-      <c r="F16" s="131"/>
+      <c r="A16" s="162"/>
+      <c r="B16" s="163"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="139"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="139"/>
       <c r="G16" s="30"/>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
@@ -2756,20 +2756,20 @@
       <c r="AT16" s="54"/>
     </row>
     <row r="17" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="146" t="s">
+      <c r="A17" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="147"/>
-      <c r="C17" s="148">
+      <c r="B17" s="114"/>
+      <c r="C17" s="115">
         <f>SUM(C18:D25)</f>
         <v>12</v>
       </c>
-      <c r="D17" s="149"/>
-      <c r="E17" s="150">
+      <c r="D17" s="116"/>
+      <c r="E17" s="147">
         <f>SUM(E18:F25)</f>
         <v>10</v>
       </c>
-      <c r="F17" s="151"/>
+      <c r="F17" s="148"/>
       <c r="G17" s="31"/>
       <c r="H17" s="32"/>
       <c r="I17" s="32"/>
@@ -2812,18 +2812,18 @@
       <c r="AT17" s="33"/>
     </row>
     <row r="18" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="124" t="s">
+      <c r="A18" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="109"/>
-      <c r="C18" s="108">
+      <c r="B18" s="110"/>
+      <c r="C18" s="109">
         <v>6</v>
       </c>
-      <c r="D18" s="109"/>
-      <c r="E18" s="108">
+      <c r="D18" s="110"/>
+      <c r="E18" s="109">
         <v>6</v>
       </c>
-      <c r="F18" s="109"/>
+      <c r="F18" s="110"/>
       <c r="G18" s="77"/>
       <c r="H18" s="78"/>
       <c r="I18" s="78"/>
@@ -2866,12 +2866,12 @@
       <c r="AT18" s="35"/>
     </row>
     <row r="19" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="152"/>
-      <c r="B19" s="111"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="111"/>
+      <c r="A19" s="118"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="111"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="112"/>
       <c r="G19" s="101"/>
       <c r="H19" s="55"/>
       <c r="I19" s="55"/>
@@ -2914,18 +2914,18 @@
       <c r="AT19" s="35"/>
     </row>
     <row r="20" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="124" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="109"/>
-      <c r="C20" s="108">
+      <c r="A20" s="117" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="110"/>
+      <c r="C20" s="109">
         <v>2</v>
       </c>
-      <c r="D20" s="109"/>
-      <c r="E20" s="108">
+      <c r="D20" s="110"/>
+      <c r="E20" s="109">
         <v>1</v>
       </c>
-      <c r="F20" s="109"/>
+      <c r="F20" s="110"/>
       <c r="G20" s="86"/>
       <c r="H20" s="81"/>
       <c r="I20" s="81"/>
@@ -2968,12 +2968,12 @@
       <c r="AT20" s="35"/>
     </row>
     <row r="21" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="152"/>
-      <c r="B21" s="111"/>
-      <c r="C21" s="110"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="110"/>
-      <c r="F21" s="111"/>
+      <c r="A21" s="118"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="111"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="111"/>
+      <c r="F21" s="112"/>
       <c r="G21" s="86"/>
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
@@ -3016,18 +3016,18 @@
       <c r="AT21" s="35"/>
     </row>
     <row r="22" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="104" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="105"/>
-      <c r="C22" s="108">
+      <c r="A22" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="106"/>
+      <c r="C22" s="109">
         <v>2</v>
       </c>
-      <c r="D22" s="109"/>
-      <c r="E22" s="108">
+      <c r="D22" s="110"/>
+      <c r="E22" s="109">
         <v>1</v>
       </c>
-      <c r="F22" s="109"/>
+      <c r="F22" s="110"/>
       <c r="G22" s="79"/>
       <c r="H22" s="80"/>
       <c r="I22" s="80"/>
@@ -3069,12 +3069,12 @@
       <c r="AT22" s="35"/>
     </row>
     <row r="23" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="106"/>
-      <c r="B23" s="107"/>
-      <c r="C23" s="110"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="111"/>
+      <c r="A23" s="107"/>
+      <c r="B23" s="108"/>
+      <c r="C23" s="111"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="111"/>
+      <c r="F23" s="112"/>
       <c r="G23" s="25"/>
       <c r="H23" s="81"/>
       <c r="I23" s="81"/>
@@ -3117,24 +3117,24 @@
       <c r="AT23" s="35"/>
     </row>
     <row r="24" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="104" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="105"/>
-      <c r="C24" s="108">
+      <c r="A24" s="105" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="106"/>
+      <c r="C24" s="109">
         <v>2</v>
       </c>
-      <c r="D24" s="109"/>
-      <c r="E24" s="142">
+      <c r="D24" s="110"/>
+      <c r="E24" s="149">
         <v>2</v>
       </c>
-      <c r="F24" s="143"/>
+      <c r="F24" s="150"/>
       <c r="G24" s="25"/>
       <c r="H24" s="81"/>
       <c r="I24" s="26"/>
       <c r="J24" s="54"/>
       <c r="L24" s="63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N24" s="35"/>
       <c r="O24" s="25"/>
@@ -3159,7 +3159,7 @@
       <c r="AH24" s="59"/>
       <c r="AI24" s="25"/>
       <c r="AJ24" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AK24" s="26"/>
       <c r="AL24" s="35"/>
@@ -3173,18 +3173,18 @@
       <c r="AT24" s="35"/>
     </row>
     <row r="25" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="106"/>
-      <c r="B25" s="107"/>
-      <c r="C25" s="110"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="144"/>
-      <c r="F25" s="145"/>
+      <c r="A25" s="107"/>
+      <c r="B25" s="108"/>
+      <c r="C25" s="111"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="151"/>
+      <c r="F25" s="152"/>
       <c r="G25" s="25"/>
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
       <c r="J25" s="82"/>
       <c r="K25" s="71" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L25" s="26"/>
       <c r="M25" s="26"/>
@@ -3223,20 +3223,20 @@
       <c r="AT25" s="35"/>
     </row>
     <row r="26" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="146" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="147"/>
-      <c r="C26" s="148">
+      <c r="A26" s="113" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="114"/>
+      <c r="C26" s="115">
         <f>SUM(C27)</f>
         <v>2</v>
       </c>
-      <c r="D26" s="149"/>
-      <c r="E26" s="150">
+      <c r="D26" s="116"/>
+      <c r="E26" s="147">
         <f>SUM(E27)</f>
         <v>3</v>
       </c>
-      <c r="F26" s="151"/>
+      <c r="F26" s="148"/>
       <c r="G26" s="31"/>
       <c r="H26" s="32"/>
       <c r="I26" s="32"/>
@@ -3279,18 +3279,18 @@
       <c r="AT26" s="33"/>
     </row>
     <row r="27" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="124" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="109"/>
-      <c r="C27" s="108">
+      <c r="A27" s="117" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="110"/>
+      <c r="C27" s="109">
         <v>2</v>
       </c>
-      <c r="D27" s="109"/>
-      <c r="E27" s="108">
+      <c r="D27" s="110"/>
+      <c r="E27" s="109">
         <v>3</v>
       </c>
-      <c r="F27" s="109"/>
+      <c r="F27" s="110"/>
       <c r="G27" s="25"/>
       <c r="H27" s="26"/>
       <c r="I27" s="26"/>
@@ -3298,7 +3298,7 @@
       <c r="K27" s="84"/>
       <c r="L27" s="81"/>
       <c r="M27" s="63" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N27" s="35"/>
       <c r="P27" s="26"/>
@@ -3334,12 +3334,12 @@
       <c r="AT27" s="35"/>
     </row>
     <row r="28" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="152"/>
-      <c r="B28" s="111"/>
-      <c r="C28" s="110"/>
-      <c r="D28" s="111"/>
-      <c r="E28" s="110"/>
-      <c r="F28" s="111"/>
+      <c r="A28" s="118"/>
+      <c r="B28" s="112"/>
+      <c r="C28" s="111"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="112"/>
       <c r="G28" s="25"/>
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
@@ -3347,7 +3347,7 @@
       <c r="K28" s="84"/>
       <c r="L28" s="72"/>
       <c r="M28" s="72" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N28" s="35"/>
       <c r="O28" s="25"/>
@@ -3384,20 +3384,20 @@
       <c r="AT28" s="35"/>
     </row>
     <row r="29" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="146" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="147"/>
-      <c r="C29" s="148">
+      <c r="A29" s="113" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="114"/>
+      <c r="C29" s="115">
         <f>SUM(C30:D41)</f>
         <v>12</v>
       </c>
-      <c r="D29" s="149"/>
-      <c r="E29" s="148">
+      <c r="D29" s="116"/>
+      <c r="E29" s="115">
         <f>SUM(E30:F41)</f>
         <v>25</v>
       </c>
-      <c r="F29" s="149"/>
+      <c r="F29" s="116"/>
       <c r="G29" s="31"/>
       <c r="H29" s="32"/>
       <c r="I29" s="32"/>
@@ -3440,18 +3440,18 @@
       <c r="AT29" s="33"/>
     </row>
     <row r="30" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="104" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="105"/>
-      <c r="C30" s="108">
+      <c r="A30" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="106"/>
+      <c r="C30" s="109">
         <v>2</v>
       </c>
-      <c r="D30" s="109"/>
-      <c r="E30" s="112">
+      <c r="D30" s="110"/>
+      <c r="E30" s="129">
         <v>1</v>
       </c>
-      <c r="F30" s="113"/>
+      <c r="F30" s="130"/>
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
@@ -3494,12 +3494,12 @@
       <c r="AT30" s="35"/>
     </row>
     <row r="31" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="106"/>
-      <c r="B31" s="107"/>
-      <c r="C31" s="110"/>
-      <c r="D31" s="111"/>
-      <c r="E31" s="114"/>
-      <c r="F31" s="115"/>
+      <c r="A31" s="107"/>
+      <c r="B31" s="108"/>
+      <c r="C31" s="111"/>
+      <c r="D31" s="112"/>
+      <c r="E31" s="131"/>
+      <c r="F31" s="132"/>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
@@ -3542,18 +3542,18 @@
       <c r="AT31" s="35"/>
     </row>
     <row r="32" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="104" t="s">
-        <v>83</v>
-      </c>
-      <c r="B32" s="105"/>
-      <c r="C32" s="108">
+      <c r="A32" s="105" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="106"/>
+      <c r="C32" s="109">
         <v>2</v>
       </c>
-      <c r="D32" s="109"/>
-      <c r="E32" s="112">
+      <c r="D32" s="110"/>
+      <c r="E32" s="129">
         <v>2</v>
       </c>
-      <c r="F32" s="113"/>
+      <c r="F32" s="130"/>
       <c r="G32" s="25"/>
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
@@ -3596,12 +3596,12 @@
       <c r="AT32" s="35"/>
     </row>
     <row r="33" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="106"/>
-      <c r="B33" s="107"/>
-      <c r="C33" s="110"/>
-      <c r="D33" s="111"/>
-      <c r="E33" s="114"/>
-      <c r="F33" s="115"/>
+      <c r="A33" s="107"/>
+      <c r="B33" s="108"/>
+      <c r="C33" s="111"/>
+      <c r="D33" s="112"/>
+      <c r="E33" s="131"/>
+      <c r="F33" s="132"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3644,18 +3644,18 @@
       <c r="AT33" s="35"/>
     </row>
     <row r="34" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="104" t="s">
-        <v>73</v>
-      </c>
-      <c r="B34" s="105"/>
-      <c r="C34" s="108">
+      <c r="A34" s="105" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="106"/>
+      <c r="C34" s="109">
         <v>2</v>
       </c>
-      <c r="D34" s="109"/>
-      <c r="E34" s="108">
+      <c r="D34" s="110"/>
+      <c r="E34" s="109">
         <v>2</v>
       </c>
-      <c r="F34" s="109"/>
+      <c r="F34" s="110"/>
       <c r="G34" s="25"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3698,12 +3698,12 @@
       <c r="AT34" s="35"/>
     </row>
     <row r="35" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="106"/>
-      <c r="B35" s="107"/>
-      <c r="C35" s="110"/>
-      <c r="D35" s="111"/>
-      <c r="E35" s="110"/>
-      <c r="F35" s="111"/>
+      <c r="A35" s="107"/>
+      <c r="B35" s="108"/>
+      <c r="C35" s="111"/>
+      <c r="D35" s="112"/>
+      <c r="E35" s="111"/>
+      <c r="F35" s="112"/>
       <c r="G35" s="25"/>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3746,18 +3746,18 @@
       <c r="AT35" s="35"/>
     </row>
     <row r="36" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="104" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="105"/>
-      <c r="C36" s="108">
+      <c r="A36" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="106"/>
+      <c r="C36" s="109">
         <v>2</v>
       </c>
-      <c r="D36" s="109"/>
-      <c r="E36" s="108">
+      <c r="D36" s="110"/>
+      <c r="E36" s="109">
         <v>4</v>
       </c>
-      <c r="F36" s="109"/>
+      <c r="F36" s="110"/>
       <c r="G36" s="25"/>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3800,12 +3800,12 @@
       <c r="AT36" s="35"/>
     </row>
     <row r="37" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A37" s="106"/>
-      <c r="B37" s="107"/>
-      <c r="C37" s="110"/>
-      <c r="D37" s="111"/>
-      <c r="E37" s="110"/>
-      <c r="F37" s="111"/>
+      <c r="A37" s="107"/>
+      <c r="B37" s="108"/>
+      <c r="C37" s="111"/>
+      <c r="D37" s="112"/>
+      <c r="E37" s="111"/>
+      <c r="F37" s="112"/>
       <c r="G37" s="25"/>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3848,18 +3848,18 @@
       <c r="AT37" s="35"/>
     </row>
     <row r="38" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="124" t="s">
-        <v>31</v>
-      </c>
-      <c r="B38" s="109"/>
-      <c r="C38" s="108">
+      <c r="A38" s="117" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="110"/>
+      <c r="C38" s="109">
         <v>2</v>
       </c>
-      <c r="D38" s="109"/>
-      <c r="E38" s="108">
+      <c r="D38" s="110"/>
+      <c r="E38" s="109">
         <v>5</v>
       </c>
-      <c r="F38" s="109"/>
+      <c r="F38" s="110"/>
       <c r="G38" s="25"/>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3902,12 +3902,12 @@
       <c r="AT38" s="35"/>
     </row>
     <row r="39" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="152"/>
-      <c r="B39" s="111"/>
-      <c r="C39" s="110"/>
-      <c r="D39" s="111"/>
-      <c r="E39" s="110"/>
-      <c r="F39" s="111"/>
+      <c r="A39" s="118"/>
+      <c r="B39" s="112"/>
+      <c r="C39" s="111"/>
+      <c r="D39" s="112"/>
+      <c r="E39" s="111"/>
+      <c r="F39" s="112"/>
       <c r="G39" s="25"/>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3950,18 +3950,18 @@
       <c r="AT39" s="35"/>
     </row>
     <row r="40" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A40" s="104" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" s="105"/>
-      <c r="C40" s="108">
+      <c r="A40" s="105" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="106"/>
+      <c r="C40" s="109">
         <v>2</v>
       </c>
-      <c r="D40" s="109"/>
-      <c r="E40" s="108">
+      <c r="D40" s="110"/>
+      <c r="E40" s="109">
         <v>11</v>
       </c>
-      <c r="F40" s="109"/>
+      <c r="F40" s="110"/>
       <c r="G40" s="25"/>
       <c r="H40" s="26"/>
       <c r="I40" s="26"/>
@@ -3976,7 +3976,7 @@
       <c r="R40" s="59"/>
       <c r="S40" s="92"/>
       <c r="T40" s="63" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U40" s="26"/>
       <c r="V40" s="35"/>
@@ -4006,12 +4006,12 @@
       <c r="AT40" s="35"/>
     </row>
     <row r="41" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="106"/>
-      <c r="B41" s="107"/>
-      <c r="C41" s="110"/>
-      <c r="D41" s="111"/>
-      <c r="E41" s="110"/>
-      <c r="F41" s="111"/>
+      <c r="A41" s="107"/>
+      <c r="B41" s="108"/>
+      <c r="C41" s="111"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="111"/>
+      <c r="F41" s="112"/>
       <c r="G41" s="25"/>
       <c r="H41" s="26"/>
       <c r="I41" s="26"/>
@@ -4032,7 +4032,7 @@
       <c r="X41" s="55"/>
       <c r="Y41" s="55"/>
       <c r="Z41" s="102" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA41" s="25"/>
       <c r="AB41" s="26"/>
@@ -4056,20 +4056,20 @@
       <c r="AT41" s="35"/>
     </row>
     <row r="42" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="146" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42" s="147"/>
-      <c r="C42" s="148">
+      <c r="A42" s="113" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="114"/>
+      <c r="C42" s="115">
         <f>SUM(C43:C45)</f>
         <v>3</v>
       </c>
-      <c r="D42" s="149"/>
-      <c r="E42" s="148">
+      <c r="D42" s="116"/>
+      <c r="E42" s="115">
         <f>SUM(E45+E43)</f>
         <v>2</v>
       </c>
-      <c r="F42" s="149"/>
+      <c r="F42" s="116"/>
       <c r="G42" s="31"/>
       <c r="H42" s="32"/>
       <c r="I42" s="32"/>
@@ -4112,18 +4112,18 @@
       <c r="AT42" s="33"/>
     </row>
     <row r="43" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="154" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="155"/>
-      <c r="C43" s="154">
+      <c r="A43" s="140" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="141"/>
+      <c r="C43" s="140">
         <v>2</v>
       </c>
-      <c r="D43" s="158"/>
-      <c r="E43" s="154">
+      <c r="D43" s="144"/>
+      <c r="E43" s="140">
         <v>1</v>
       </c>
-      <c r="F43" s="158"/>
+      <c r="F43" s="144"/>
       <c r="G43" s="84"/>
       <c r="H43" s="81"/>
       <c r="I43" s="81"/>
@@ -4166,12 +4166,12 @@
       <c r="AT43" s="54"/>
     </row>
     <row r="44" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="156"/>
-      <c r="B44" s="157"/>
-      <c r="C44" s="159"/>
-      <c r="D44" s="160"/>
-      <c r="E44" s="159"/>
-      <c r="F44" s="160"/>
+      <c r="A44" s="142"/>
+      <c r="B44" s="143"/>
+      <c r="C44" s="145"/>
+      <c r="D44" s="146"/>
+      <c r="E44" s="145"/>
+      <c r="F44" s="146"/>
       <c r="G44" s="84"/>
       <c r="H44" s="81"/>
       <c r="I44" s="81"/>
@@ -4214,18 +4214,18 @@
       <c r="AT44" s="54"/>
     </row>
     <row r="45" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="124" t="s">
-        <v>69</v>
-      </c>
-      <c r="B45" s="129"/>
-      <c r="C45" s="108">
+      <c r="A45" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="137"/>
+      <c r="C45" s="109">
         <v>1</v>
       </c>
-      <c r="D45" s="109"/>
-      <c r="E45" s="108">
+      <c r="D45" s="110"/>
+      <c r="E45" s="109">
         <v>1</v>
       </c>
-      <c r="F45" s="109"/>
+      <c r="F45" s="110"/>
       <c r="G45" s="25"/>
       <c r="H45" s="26"/>
       <c r="I45" s="26"/>
@@ -4242,7 +4242,7 @@
       <c r="T45" s="26"/>
       <c r="U45" s="81"/>
       <c r="V45" s="95" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W45" s="25"/>
       <c r="X45" s="26"/>
@@ -4270,12 +4270,12 @@
       <c r="AT45" s="35"/>
     </row>
     <row r="46" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="153"/>
-      <c r="B46" s="131"/>
-      <c r="C46" s="110"/>
-      <c r="D46" s="111"/>
-      <c r="E46" s="110"/>
-      <c r="F46" s="111"/>
+      <c r="A46" s="138"/>
+      <c r="B46" s="139"/>
+      <c r="C46" s="111"/>
+      <c r="D46" s="112"/>
+      <c r="E46" s="111"/>
+      <c r="F46" s="112"/>
       <c r="G46" s="25"/>
       <c r="H46" s="26"/>
       <c r="I46" s="26"/>
@@ -4297,7 +4297,7 @@
       <c r="Y46" s="26"/>
       <c r="Z46" s="35"/>
       <c r="AA46" s="103" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB46" s="26"/>
       <c r="AC46" s="26"/>
@@ -4320,20 +4320,20 @@
       <c r="AT46" s="35"/>
     </row>
     <row r="47" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="146" t="s">
-        <v>36</v>
-      </c>
-      <c r="B47" s="147"/>
-      <c r="C47" s="148">
+      <c r="A47" s="113" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="114"/>
+      <c r="C47" s="115">
         <f>SUM(C48:D63)</f>
         <v>19</v>
       </c>
-      <c r="D47" s="149"/>
-      <c r="E47" s="148">
+      <c r="D47" s="116"/>
+      <c r="E47" s="115">
         <f>SUM(E48:F63)</f>
         <v>17</v>
       </c>
-      <c r="F47" s="149"/>
+      <c r="F47" s="116"/>
       <c r="G47" s="31"/>
       <c r="H47" s="32"/>
       <c r="I47" s="32"/>
@@ -4376,18 +4376,18 @@
       <c r="AT47" s="33"/>
     </row>
     <row r="48" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="161" t="s">
-        <v>74</v>
-      </c>
-      <c r="B48" s="162"/>
-      <c r="C48" s="108">
+      <c r="A48" s="133" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" s="134"/>
+      <c r="C48" s="109">
         <v>0.5</v>
       </c>
-      <c r="D48" s="109"/>
-      <c r="E48" s="108">
+      <c r="D48" s="110"/>
+      <c r="E48" s="109">
         <v>0.5</v>
       </c>
-      <c r="F48" s="109"/>
+      <c r="F48" s="110"/>
       <c r="G48" s="25"/>
       <c r="H48" s="26"/>
       <c r="I48" s="26"/>
@@ -4430,12 +4430,12 @@
       <c r="AT48" s="35"/>
     </row>
     <row r="49" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="163"/>
-      <c r="B49" s="164"/>
-      <c r="C49" s="110"/>
-      <c r="D49" s="111"/>
-      <c r="E49" s="110"/>
-      <c r="F49" s="111"/>
+      <c r="A49" s="135"/>
+      <c r="B49" s="136"/>
+      <c r="C49" s="111"/>
+      <c r="D49" s="112"/>
+      <c r="E49" s="111"/>
+      <c r="F49" s="112"/>
       <c r="G49" s="25"/>
       <c r="H49" s="26"/>
       <c r="I49" s="26"/>
@@ -4478,18 +4478,18 @@
       <c r="AT49" s="35"/>
     </row>
     <row r="50" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A50" s="124" t="s">
-        <v>75</v>
-      </c>
-      <c r="B50" s="109"/>
-      <c r="C50" s="108">
+      <c r="A50" s="117" t="s">
+        <v>73</v>
+      </c>
+      <c r="B50" s="110"/>
+      <c r="C50" s="109">
         <v>0.5</v>
       </c>
-      <c r="D50" s="109"/>
-      <c r="E50" s="112">
+      <c r="D50" s="110"/>
+      <c r="E50" s="129">
         <v>0.5</v>
       </c>
-      <c r="F50" s="113"/>
+      <c r="F50" s="130"/>
       <c r="G50" s="25"/>
       <c r="H50" s="26"/>
       <c r="I50" s="26"/>
@@ -4532,12 +4532,12 @@
       <c r="AT50" s="35"/>
     </row>
     <row r="51" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="152"/>
-      <c r="B51" s="111"/>
-      <c r="C51" s="110"/>
-      <c r="D51" s="111"/>
-      <c r="E51" s="114"/>
-      <c r="F51" s="115"/>
+      <c r="A51" s="118"/>
+      <c r="B51" s="112"/>
+      <c r="C51" s="111"/>
+      <c r="D51" s="112"/>
+      <c r="E51" s="131"/>
+      <c r="F51" s="132"/>
       <c r="G51" s="25"/>
       <c r="H51" s="26"/>
       <c r="I51" s="26"/>
@@ -4580,18 +4580,18 @@
       <c r="AT51" s="35"/>
     </row>
     <row r="52" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A52" s="124" t="s">
-        <v>76</v>
-      </c>
-      <c r="B52" s="109"/>
-      <c r="C52" s="108">
+      <c r="A52" s="117" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" s="110"/>
+      <c r="C52" s="109">
         <v>2</v>
       </c>
-      <c r="D52" s="109"/>
-      <c r="E52" s="112">
+      <c r="D52" s="110"/>
+      <c r="E52" s="129">
         <v>1.5</v>
       </c>
-      <c r="F52" s="113"/>
+      <c r="F52" s="130"/>
       <c r="G52" s="25"/>
       <c r="H52" s="26"/>
       <c r="I52" s="26"/>
@@ -4634,12 +4634,12 @@
       <c r="AT52" s="35"/>
     </row>
     <row r="53" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="152"/>
-      <c r="B53" s="111"/>
-      <c r="C53" s="110"/>
-      <c r="D53" s="111"/>
-      <c r="E53" s="114"/>
-      <c r="F53" s="115"/>
+      <c r="A53" s="118"/>
+      <c r="B53" s="112"/>
+      <c r="C53" s="111"/>
+      <c r="D53" s="112"/>
+      <c r="E53" s="131"/>
+      <c r="F53" s="132"/>
       <c r="G53" s="25"/>
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
@@ -4682,18 +4682,18 @@
       <c r="AT53" s="35"/>
     </row>
     <row r="54" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="124" t="s">
-        <v>78</v>
-      </c>
-      <c r="B54" s="109"/>
-      <c r="C54" s="108">
+      <c r="A54" s="117" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="110"/>
+      <c r="C54" s="109">
         <v>2</v>
       </c>
-      <c r="D54" s="109"/>
-      <c r="E54" s="112">
+      <c r="D54" s="110"/>
+      <c r="E54" s="129">
         <v>1.5</v>
       </c>
-      <c r="F54" s="113"/>
+      <c r="F54" s="130"/>
       <c r="G54" s="25"/>
       <c r="H54" s="26"/>
       <c r="I54" s="26"/>
@@ -4736,12 +4736,12 @@
       <c r="AT54" s="35"/>
     </row>
     <row r="55" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="152"/>
-      <c r="B55" s="111"/>
-      <c r="C55" s="110"/>
-      <c r="D55" s="111"/>
-      <c r="E55" s="114"/>
-      <c r="F55" s="115"/>
+      <c r="A55" s="118"/>
+      <c r="B55" s="112"/>
+      <c r="C55" s="111"/>
+      <c r="D55" s="112"/>
+      <c r="E55" s="131"/>
+      <c r="F55" s="132"/>
       <c r="G55" s="25"/>
       <c r="H55" s="26"/>
       <c r="I55" s="26"/>
@@ -4783,18 +4783,18 @@
       <c r="AT55" s="35"/>
     </row>
     <row r="56" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="104" t="s">
-        <v>77</v>
-      </c>
-      <c r="B56" s="105"/>
-      <c r="C56" s="108">
+      <c r="A56" s="105" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" s="106"/>
+      <c r="C56" s="109">
         <v>2</v>
       </c>
-      <c r="D56" s="109"/>
-      <c r="E56" s="108">
+      <c r="D56" s="110"/>
+      <c r="E56" s="109">
         <v>1.5</v>
       </c>
-      <c r="F56" s="109"/>
+      <c r="F56" s="110"/>
       <c r="G56" s="25"/>
       <c r="H56" s="26"/>
       <c r="I56" s="26"/>
@@ -4837,12 +4837,12 @@
       <c r="AT56" s="35"/>
     </row>
     <row r="57" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A57" s="106"/>
-      <c r="B57" s="107"/>
-      <c r="C57" s="110"/>
-      <c r="D57" s="111"/>
-      <c r="E57" s="110"/>
-      <c r="F57" s="111"/>
+      <c r="A57" s="107"/>
+      <c r="B57" s="108"/>
+      <c r="C57" s="111"/>
+      <c r="D57" s="112"/>
+      <c r="E57" s="111"/>
+      <c r="F57" s="112"/>
       <c r="G57" s="25"/>
       <c r="H57" s="26"/>
       <c r="I57" s="26"/>
@@ -4885,18 +4885,18 @@
       <c r="AT57" s="35"/>
     </row>
     <row r="58" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A58" s="104" t="s">
-        <v>79</v>
-      </c>
-      <c r="B58" s="105"/>
-      <c r="C58" s="108">
+      <c r="A58" s="105" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" s="106"/>
+      <c r="C58" s="109">
         <v>2</v>
       </c>
-      <c r="D58" s="109"/>
-      <c r="E58" s="108">
+      <c r="D58" s="110"/>
+      <c r="E58" s="109">
         <v>1.5</v>
       </c>
-      <c r="F58" s="109"/>
+      <c r="F58" s="110"/>
       <c r="G58" s="25"/>
       <c r="H58" s="26"/>
       <c r="I58" s="26"/>
@@ -4939,12 +4939,12 @@
       <c r="AT58" s="35"/>
     </row>
     <row r="59" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A59" s="106"/>
-      <c r="B59" s="107"/>
-      <c r="C59" s="110"/>
-      <c r="D59" s="111"/>
-      <c r="E59" s="110"/>
-      <c r="F59" s="111"/>
+      <c r="A59" s="107"/>
+      <c r="B59" s="108"/>
+      <c r="C59" s="111"/>
+      <c r="D59" s="112"/>
+      <c r="E59" s="111"/>
+      <c r="F59" s="112"/>
       <c r="G59" s="25"/>
       <c r="H59" s="26"/>
       <c r="I59" s="26"/>
@@ -4987,18 +4987,18 @@
       <c r="AT59" s="35"/>
     </row>
     <row r="60" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A60" s="104" t="s">
-        <v>37</v>
-      </c>
-      <c r="B60" s="105"/>
-      <c r="C60" s="108">
+      <c r="A60" s="105" t="s">
+        <v>36</v>
+      </c>
+      <c r="B60" s="106"/>
+      <c r="C60" s="109">
         <v>6</v>
       </c>
-      <c r="D60" s="109"/>
-      <c r="E60" s="108">
+      <c r="D60" s="110"/>
+      <c r="E60" s="109">
         <v>6</v>
       </c>
-      <c r="F60" s="109"/>
+      <c r="F60" s="110"/>
       <c r="G60" s="25"/>
       <c r="H60" s="26"/>
       <c r="I60" s="26"/>
@@ -5041,12 +5041,12 @@
       <c r="AT60" s="35"/>
     </row>
     <row r="61" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A61" s="106"/>
-      <c r="B61" s="107"/>
-      <c r="C61" s="110"/>
-      <c r="D61" s="111"/>
-      <c r="E61" s="110"/>
-      <c r="F61" s="111"/>
+      <c r="A61" s="107"/>
+      <c r="B61" s="108"/>
+      <c r="C61" s="111"/>
+      <c r="D61" s="112"/>
+      <c r="E61" s="111"/>
+      <c r="F61" s="112"/>
       <c r="G61" s="25"/>
       <c r="H61" s="26"/>
       <c r="I61" s="26"/>
@@ -5089,18 +5089,18 @@
       <c r="AT61" s="35"/>
     </row>
     <row r="62" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A62" s="104" t="s">
-        <v>80</v>
-      </c>
-      <c r="B62" s="105"/>
-      <c r="C62" s="108">
+      <c r="A62" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" s="106"/>
+      <c r="C62" s="109">
         <v>4</v>
       </c>
-      <c r="D62" s="109"/>
-      <c r="E62" s="108">
+      <c r="D62" s="110"/>
+      <c r="E62" s="109">
         <v>4</v>
       </c>
-      <c r="F62" s="109"/>
+      <c r="F62" s="110"/>
       <c r="G62" s="25"/>
       <c r="H62" s="26"/>
       <c r="I62" s="26"/>
@@ -5126,7 +5126,7 @@
       <c r="AC62" s="81"/>
       <c r="AD62" s="96"/>
       <c r="AE62" s="98" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AF62" s="90"/>
       <c r="AG62" s="59"/>
@@ -5145,12 +5145,12 @@
       <c r="AT62" s="35"/>
     </row>
     <row r="63" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A63" s="106"/>
-      <c r="B63" s="107"/>
-      <c r="C63" s="110"/>
-      <c r="D63" s="111"/>
-      <c r="E63" s="110"/>
-      <c r="F63" s="111"/>
+      <c r="A63" s="107"/>
+      <c r="B63" s="108"/>
+      <c r="C63" s="111"/>
+      <c r="D63" s="112"/>
+      <c r="E63" s="111"/>
+      <c r="F63" s="112"/>
       <c r="G63" s="25"/>
       <c r="H63" s="26"/>
       <c r="I63" s="26"/>
@@ -5176,7 +5176,7 @@
       <c r="AC63" s="26"/>
       <c r="AD63" s="56"/>
       <c r="AE63" s="101"/>
-      <c r="AF63" s="175"/>
+      <c r="AF63" s="104"/>
       <c r="AG63" s="59"/>
       <c r="AH63" s="59"/>
       <c r="AI63" s="25"/>
@@ -5193,20 +5193,20 @@
       <c r="AT63" s="35"/>
     </row>
     <row r="64" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="146" t="s">
-        <v>39</v>
-      </c>
-      <c r="B64" s="147"/>
-      <c r="C64" s="148">
+      <c r="A64" s="113" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" s="114"/>
+      <c r="C64" s="115">
         <f>SUM(C65:D66)</f>
         <v>4</v>
       </c>
-      <c r="D64" s="149"/>
-      <c r="E64" s="148">
+      <c r="D64" s="116"/>
+      <c r="E64" s="115">
         <f>SUM(E65)</f>
         <v>4</v>
       </c>
-      <c r="F64" s="149"/>
+      <c r="F64" s="116"/>
       <c r="G64" s="31"/>
       <c r="H64" s="32"/>
       <c r="I64" s="32"/>
@@ -5249,18 +5249,18 @@
       <c r="AT64" s="33"/>
     </row>
     <row r="65" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="124" t="s">
-        <v>40</v>
-      </c>
-      <c r="B65" s="109"/>
-      <c r="C65" s="108">
+      <c r="A65" s="117" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65" s="110"/>
+      <c r="C65" s="109">
         <v>4</v>
       </c>
-      <c r="D65" s="109"/>
-      <c r="E65" s="108">
+      <c r="D65" s="110"/>
+      <c r="E65" s="109">
         <v>4</v>
       </c>
-      <c r="F65" s="109"/>
+      <c r="F65" s="110"/>
       <c r="G65" s="25"/>
       <c r="H65" s="26"/>
       <c r="I65" s="26"/>
@@ -5290,7 +5290,7 @@
       <c r="AG65" s="59"/>
       <c r="AH65" s="58"/>
       <c r="AI65" s="64" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AJ65" s="26"/>
       <c r="AK65" s="81"/>
@@ -5305,12 +5305,12 @@
       <c r="AT65" s="35"/>
     </row>
     <row r="66" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="152"/>
-      <c r="B66" s="111"/>
-      <c r="C66" s="110"/>
-      <c r="D66" s="111"/>
-      <c r="E66" s="110"/>
-      <c r="F66" s="111"/>
+      <c r="A66" s="118"/>
+      <c r="B66" s="112"/>
+      <c r="C66" s="111"/>
+      <c r="D66" s="112"/>
+      <c r="E66" s="111"/>
+      <c r="F66" s="112"/>
       <c r="G66" s="25"/>
       <c r="H66" s="26"/>
       <c r="I66" s="26"/>
@@ -5353,20 +5353,20 @@
       <c r="AT66" s="35"/>
     </row>
     <row r="67" spans="1:59" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="146" t="s">
-        <v>42</v>
-      </c>
-      <c r="B67" s="147"/>
-      <c r="C67" s="148">
+      <c r="A67" s="113" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" s="114"/>
+      <c r="C67" s="115">
         <f>SUM(C68:D69)</f>
         <v>4</v>
       </c>
-      <c r="D67" s="149"/>
-      <c r="E67" s="148">
+      <c r="D67" s="116"/>
+      <c r="E67" s="115">
         <f>SUM(E68)</f>
         <v>4</v>
       </c>
-      <c r="F67" s="149"/>
+      <c r="F67" s="116"/>
       <c r="G67" s="31"/>
       <c r="H67" s="32"/>
       <c r="I67" s="32"/>
@@ -5409,18 +5409,18 @@
       <c r="AT67" s="33"/>
     </row>
     <row r="68" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A68" s="124" t="s">
-        <v>43</v>
-      </c>
-      <c r="B68" s="109"/>
-      <c r="C68" s="108">
+      <c r="A68" s="117" t="s">
+        <v>42</v>
+      </c>
+      <c r="B68" s="110"/>
+      <c r="C68" s="109">
         <v>4</v>
       </c>
-      <c r="D68" s="109"/>
-      <c r="E68" s="108">
+      <c r="D68" s="110"/>
+      <c r="E68" s="109">
         <v>4</v>
       </c>
-      <c r="F68" s="109"/>
+      <c r="F68" s="110"/>
       <c r="G68" s="25"/>
       <c r="H68" s="26"/>
       <c r="I68" s="26"/>
@@ -5452,7 +5452,7 @@
       <c r="AI68" s="86"/>
       <c r="AJ68" s="87"/>
       <c r="AK68" s="63" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AL68" s="56"/>
       <c r="AM68" s="86"/>
@@ -5466,12 +5466,12 @@
       <c r="AU68" s="38"/>
     </row>
     <row r="69" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A69" s="152"/>
-      <c r="B69" s="111"/>
-      <c r="C69" s="110"/>
-      <c r="D69" s="111"/>
-      <c r="E69" s="110"/>
-      <c r="F69" s="111"/>
+      <c r="A69" s="118"/>
+      <c r="B69" s="112"/>
+      <c r="C69" s="111"/>
+      <c r="D69" s="112"/>
+      <c r="E69" s="111"/>
+      <c r="F69" s="112"/>
       <c r="G69" s="25"/>
       <c r="H69" s="26"/>
       <c r="I69" s="26"/>
@@ -5515,20 +5515,20 @@
       <c r="AU69" s="39"/>
     </row>
     <row r="70" spans="1:59" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="171" t="s">
-        <v>45</v>
-      </c>
-      <c r="B70" s="172"/>
-      <c r="C70" s="173">
+      <c r="A70" s="125" t="s">
+        <v>44</v>
+      </c>
+      <c r="B70" s="126"/>
+      <c r="C70" s="127">
         <f>SUM(C71:D76)</f>
         <v>18</v>
       </c>
-      <c r="D70" s="174"/>
-      <c r="E70" s="148">
+      <c r="D70" s="128"/>
+      <c r="E70" s="115">
         <f>SUM(E71:F76)</f>
         <v>18</v>
       </c>
-      <c r="F70" s="149"/>
+      <c r="F70" s="116"/>
       <c r="G70" s="40"/>
       <c r="H70" s="41"/>
       <c r="I70" s="41"/>
@@ -5572,18 +5572,18 @@
       <c r="AU70" s="3"/>
     </row>
     <row r="71" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A71" s="124" t="s">
-        <v>46</v>
-      </c>
-      <c r="B71" s="109"/>
-      <c r="C71" s="108">
+      <c r="A71" s="117" t="s">
+        <v>45</v>
+      </c>
+      <c r="B71" s="110"/>
+      <c r="C71" s="109">
         <v>6</v>
       </c>
-      <c r="D71" s="109"/>
-      <c r="E71" s="108">
+      <c r="D71" s="110"/>
+      <c r="E71" s="109">
         <v>6</v>
       </c>
-      <c r="F71" s="109"/>
+      <c r="F71" s="110"/>
       <c r="G71" s="25"/>
       <c r="H71" s="26"/>
       <c r="I71" s="26"/>
@@ -5627,12 +5627,12 @@
       <c r="AU71" s="3"/>
     </row>
     <row r="72" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A72" s="152"/>
-      <c r="B72" s="111"/>
-      <c r="C72" s="110"/>
-      <c r="D72" s="111"/>
-      <c r="E72" s="110"/>
-      <c r="F72" s="111"/>
+      <c r="A72" s="118"/>
+      <c r="B72" s="112"/>
+      <c r="C72" s="111"/>
+      <c r="D72" s="112"/>
+      <c r="E72" s="111"/>
+      <c r="F72" s="112"/>
       <c r="G72" s="25"/>
       <c r="H72" s="26"/>
       <c r="I72" s="26"/>
@@ -5688,18 +5688,18 @@
       <c r="BG72" s="38"/>
     </row>
     <row r="73" spans="1:59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="124" t="s">
-        <v>47</v>
-      </c>
-      <c r="B73" s="109"/>
-      <c r="C73" s="108">
+      <c r="A73" s="117" t="s">
+        <v>46</v>
+      </c>
+      <c r="B73" s="110"/>
+      <c r="C73" s="109">
         <v>6</v>
       </c>
-      <c r="D73" s="109"/>
-      <c r="E73" s="108">
+      <c r="D73" s="110"/>
+      <c r="E73" s="109">
         <v>6</v>
       </c>
-      <c r="F73" s="109"/>
+      <c r="F73" s="110"/>
       <c r="G73" s="25"/>
       <c r="H73" s="26"/>
       <c r="I73" s="26"/>
@@ -5737,7 +5737,7 @@
       <c r="AO73" s="87"/>
       <c r="AP73" s="100"/>
       <c r="AQ73" s="98" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AR73" s="26"/>
       <c r="AS73" s="26"/>
@@ -5757,12 +5757,12 @@
       <c r="BG73" s="38"/>
     </row>
     <row r="74" spans="1:59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="152"/>
-      <c r="B74" s="111"/>
-      <c r="C74" s="110"/>
-      <c r="D74" s="111"/>
-      <c r="E74" s="110"/>
-      <c r="F74" s="111"/>
+      <c r="A74" s="118"/>
+      <c r="B74" s="112"/>
+      <c r="C74" s="111"/>
+      <c r="D74" s="112"/>
+      <c r="E74" s="111"/>
+      <c r="F74" s="112"/>
       <c r="G74" s="25"/>
       <c r="H74" s="26"/>
       <c r="I74" s="26"/>
@@ -5818,18 +5818,18 @@
       <c r="BG74" s="38"/>
     </row>
     <row r="75" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A75" s="124" t="s">
-        <v>82</v>
-      </c>
-      <c r="B75" s="109"/>
-      <c r="C75" s="108">
+      <c r="A75" s="117" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" s="110"/>
+      <c r="C75" s="109">
         <v>6</v>
       </c>
-      <c r="D75" s="109"/>
-      <c r="E75" s="108">
+      <c r="D75" s="110"/>
+      <c r="E75" s="109">
         <v>6</v>
       </c>
-      <c r="F75" s="109"/>
+      <c r="F75" s="110"/>
       <c r="G75" s="25"/>
       <c r="H75" s="26"/>
       <c r="I75" s="26"/>
@@ -5885,12 +5885,12 @@
       <c r="BG75" s="39"/>
     </row>
     <row r="76" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A76" s="152"/>
-      <c r="B76" s="111"/>
-      <c r="C76" s="110"/>
-      <c r="D76" s="111"/>
-      <c r="E76" s="110"/>
-      <c r="F76" s="111"/>
+      <c r="A76" s="118"/>
+      <c r="B76" s="112"/>
+      <c r="C76" s="111"/>
+      <c r="D76" s="112"/>
+      <c r="E76" s="111"/>
+      <c r="F76" s="112"/>
       <c r="G76" s="25"/>
       <c r="H76" s="26"/>
       <c r="I76" s="26"/>
@@ -6007,20 +6007,20 @@
       <c r="BG77" s="3"/>
     </row>
     <row r="78" spans="1:59" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="165" t="s">
-        <v>49</v>
-      </c>
-      <c r="B78" s="166"/>
-      <c r="C78" s="167">
+      <c r="A78" s="119" t="s">
+        <v>48</v>
+      </c>
+      <c r="B78" s="120"/>
+      <c r="C78" s="121">
         <f>SUM(C14+C17+C29+C42+C47+C64+C67+C26 + C70)</f>
         <v>80</v>
       </c>
-      <c r="D78" s="168"/>
-      <c r="E78" s="169">
+      <c r="D78" s="122"/>
+      <c r="E78" s="123">
         <f>SUM(E14+E17+E29+E42+E47+E64+E67+E26+E70)</f>
         <v>89</v>
       </c>
-      <c r="F78" s="170"/>
+      <c r="F78" s="124"/>
       <c r="G78" s="39"/>
       <c r="H78" s="39"/>
       <c r="I78" s="39"/>
@@ -6138,107 +6138,6 @@
     </row>
   </sheetData>
   <mergeCells count="125">
-    <mergeCell ref="A60:B61"/>
-    <mergeCell ref="C60:D61"/>
-    <mergeCell ref="E60:F61"/>
-    <mergeCell ref="A62:B63"/>
-    <mergeCell ref="C62:D63"/>
-    <mergeCell ref="E62:F63"/>
-    <mergeCell ref="A56:B57"/>
-    <mergeCell ref="C56:D57"/>
-    <mergeCell ref="E56:F57"/>
-    <mergeCell ref="A58:B59"/>
-    <mergeCell ref="C58:D59"/>
-    <mergeCell ref="E58:F59"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="A68:B69"/>
-    <mergeCell ref="C68:D69"/>
-    <mergeCell ref="E68:F69"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="A65:B66"/>
-    <mergeCell ref="C65:D66"/>
-    <mergeCell ref="E65:F66"/>
-    <mergeCell ref="A75:B76"/>
-    <mergeCell ref="C75:D76"/>
-    <mergeCell ref="E75:F76"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="A71:B72"/>
-    <mergeCell ref="C71:D72"/>
-    <mergeCell ref="E71:F72"/>
-    <mergeCell ref="A73:B74"/>
-    <mergeCell ref="C73:D74"/>
-    <mergeCell ref="E73:F74"/>
-    <mergeCell ref="A52:B53"/>
-    <mergeCell ref="C52:D53"/>
-    <mergeCell ref="E52:F53"/>
-    <mergeCell ref="A54:B55"/>
-    <mergeCell ref="C54:D55"/>
-    <mergeCell ref="E54:F55"/>
-    <mergeCell ref="A48:B49"/>
-    <mergeCell ref="C48:D49"/>
-    <mergeCell ref="E48:F49"/>
-    <mergeCell ref="A50:B51"/>
-    <mergeCell ref="C50:D51"/>
-    <mergeCell ref="E50:F51"/>
-    <mergeCell ref="A45:B46"/>
-    <mergeCell ref="C45:D46"/>
-    <mergeCell ref="E45:F46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="A40:B41"/>
-    <mergeCell ref="C40:D41"/>
-    <mergeCell ref="E40:F41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="C43:D44"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="A38:B39"/>
-    <mergeCell ref="C38:D39"/>
-    <mergeCell ref="E38:F39"/>
-    <mergeCell ref="A34:B35"/>
-    <mergeCell ref="C34:D35"/>
-    <mergeCell ref="E34:F35"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="E36:F37"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="E30:F31"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:F28"/>
-    <mergeCell ref="C22:D23"/>
-    <mergeCell ref="E22:F23"/>
-    <mergeCell ref="A24:B25"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="E24:F25"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="E20:F21"/>
     <mergeCell ref="A32:B33"/>
     <mergeCell ref="C32:D33"/>
     <mergeCell ref="E32:F33"/>
@@ -6263,6 +6162,107 @@
     <mergeCell ref="C11:D13"/>
     <mergeCell ref="A11:B13"/>
     <mergeCell ref="A22:B23"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="E22:F23"/>
+    <mergeCell ref="A24:B25"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="E24:F25"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="E20:F21"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="E30:F31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:F28"/>
+    <mergeCell ref="A38:B39"/>
+    <mergeCell ref="C38:D39"/>
+    <mergeCell ref="E38:F39"/>
+    <mergeCell ref="A34:B35"/>
+    <mergeCell ref="C34:D35"/>
+    <mergeCell ref="E34:F35"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="E36:F37"/>
+    <mergeCell ref="A45:B46"/>
+    <mergeCell ref="C45:D46"/>
+    <mergeCell ref="E45:F46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="A40:B41"/>
+    <mergeCell ref="C40:D41"/>
+    <mergeCell ref="E40:F41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="C43:D44"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="A52:B53"/>
+    <mergeCell ref="C52:D53"/>
+    <mergeCell ref="E52:F53"/>
+    <mergeCell ref="A54:B55"/>
+    <mergeCell ref="C54:D55"/>
+    <mergeCell ref="E54:F55"/>
+    <mergeCell ref="A48:B49"/>
+    <mergeCell ref="C48:D49"/>
+    <mergeCell ref="E48:F49"/>
+    <mergeCell ref="A50:B51"/>
+    <mergeCell ref="C50:D51"/>
+    <mergeCell ref="E50:F51"/>
+    <mergeCell ref="A75:B76"/>
+    <mergeCell ref="C75:D76"/>
+    <mergeCell ref="E75:F76"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="A71:B72"/>
+    <mergeCell ref="C71:D72"/>
+    <mergeCell ref="E71:F72"/>
+    <mergeCell ref="A73:B74"/>
+    <mergeCell ref="C73:D74"/>
+    <mergeCell ref="E73:F74"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="A68:B69"/>
+    <mergeCell ref="C68:D69"/>
+    <mergeCell ref="E68:F69"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="A65:B66"/>
+    <mergeCell ref="C65:D66"/>
+    <mergeCell ref="E65:F66"/>
+    <mergeCell ref="A60:B61"/>
+    <mergeCell ref="C60:D61"/>
+    <mergeCell ref="E60:F61"/>
+    <mergeCell ref="A62:B63"/>
+    <mergeCell ref="C62:D63"/>
+    <mergeCell ref="E62:F63"/>
+    <mergeCell ref="A56:B57"/>
+    <mergeCell ref="C56:D57"/>
+    <mergeCell ref="E56:F57"/>
+    <mergeCell ref="A58:B59"/>
+    <mergeCell ref="C58:D59"/>
+    <mergeCell ref="E58:F59"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
table and graphic names in documentation
</commit_message>
<xml_diff>
--- a/documentation/Zeitplan.xlsx
+++ b/documentation/Zeitplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp8\htdocs\IPA\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0F5A95-5F16-4A1E-820A-9A240E1E952D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CB44F3-5838-4DC9-A846-F81B8734603B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-5530" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
   <si>
     <t>Projekttitel</t>
   </si>
@@ -200,9 +200,6 @@
     <t>Granularität</t>
   </si>
   <si>
-    <t>0.5 Stunde</t>
-  </si>
-  <si>
     <t>Mo 13.03.2023</t>
   </si>
   <si>
@@ -288,6 +285,9 @@
   </si>
   <si>
     <t>Laravel-Aufbaudiagramm erstellen</t>
+  </si>
+  <si>
+    <t>0.5 Stunden</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1039,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1300,6 +1300,108 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1312,11 +1414,50 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1348,147 +1489,16 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Eingabe" xfId="4" builtinId="20"/>
@@ -1778,8 +1788,8 @@
   </sheetPr>
   <dimension ref="A1:BG79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="N72" sqref="N72"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,27 +1802,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:59" ht="44.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="120" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156"/>
-      <c r="F1" s="156"/>
-      <c r="G1" s="156"/>
-      <c r="H1" s="156"/>
-      <c r="I1" s="156"/>
-      <c r="J1" s="156"/>
-      <c r="K1" s="156"/>
-      <c r="L1" s="156"/>
-      <c r="M1" s="156"/>
-      <c r="N1" s="156"/>
-      <c r="O1" s="156"/>
-      <c r="P1" s="156"/>
-      <c r="Q1" s="156"/>
-      <c r="R1" s="156"/>
-      <c r="S1" s="156"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="120"/>
+      <c r="O1" s="120"/>
+      <c r="P1" s="120"/>
+      <c r="Q1" s="120"/>
+      <c r="R1" s="120"/>
+      <c r="S1" s="120"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
@@ -2199,7 +2209,7 @@
         <v>20</v>
       </c>
       <c r="AO7" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AT7" s="29"/>
       <c r="AV7" s="3"/>
@@ -2228,7 +2238,7 @@
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="5" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -2316,7 +2326,7 @@
       <c r="AL9" s="3"/>
       <c r="AN9" s="68"/>
       <c r="AO9" s="69" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AP9" s="36"/>
       <c r="AQ9" s="36"/>
@@ -2388,86 +2398,86 @@
       <c r="BG10" s="3"/>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A11" s="174" t="s">
+      <c r="A11" s="141" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="175"/>
-      <c r="C11" s="169" t="s">
+      <c r="B11" s="142"/>
+      <c r="C11" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="170"/>
-      <c r="E11" s="169" t="s">
+      <c r="D11" s="137"/>
+      <c r="E11" s="136" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="170"/>
-      <c r="G11" s="157" t="s">
+      <c r="F11" s="137"/>
+      <c r="G11" s="121" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="122"/>
+      <c r="I11" s="122"/>
+      <c r="J11" s="123"/>
+      <c r="K11" s="121" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="158"/>
-      <c r="I11" s="158"/>
-      <c r="J11" s="159"/>
-      <c r="K11" s="157" t="s">
+      <c r="L11" s="122"/>
+      <c r="M11" s="122"/>
+      <c r="N11" s="123"/>
+      <c r="O11" s="121" t="s">
         <v>56</v>
       </c>
-      <c r="L11" s="158"/>
-      <c r="M11" s="158"/>
-      <c r="N11" s="159"/>
-      <c r="O11" s="157" t="s">
+      <c r="P11" s="122"/>
+      <c r="Q11" s="122"/>
+      <c r="R11" s="123"/>
+      <c r="S11" s="121" t="s">
         <v>57</v>
       </c>
-      <c r="P11" s="158"/>
-      <c r="Q11" s="158"/>
-      <c r="R11" s="159"/>
-      <c r="S11" s="157" t="s">
+      <c r="T11" s="122"/>
+      <c r="U11" s="122"/>
+      <c r="V11" s="123"/>
+      <c r="W11" s="121" t="s">
         <v>58</v>
       </c>
-      <c r="T11" s="158"/>
-      <c r="U11" s="158"/>
-      <c r="V11" s="159"/>
-      <c r="W11" s="157" t="s">
+      <c r="X11" s="122"/>
+      <c r="Y11" s="122"/>
+      <c r="Z11" s="123"/>
+      <c r="AA11" s="121" t="s">
         <v>59</v>
       </c>
-      <c r="X11" s="158"/>
-      <c r="Y11" s="158"/>
-      <c r="Z11" s="159"/>
-      <c r="AA11" s="157" t="s">
+      <c r="AB11" s="122"/>
+      <c r="AC11" s="122"/>
+      <c r="AD11" s="123"/>
+      <c r="AE11" s="121" t="s">
         <v>60</v>
       </c>
-      <c r="AB11" s="158"/>
-      <c r="AC11" s="158"/>
-      <c r="AD11" s="159"/>
-      <c r="AE11" s="157" t="s">
+      <c r="AF11" s="122"/>
+      <c r="AG11" s="122"/>
+      <c r="AH11" s="123"/>
+      <c r="AI11" s="121" t="s">
         <v>61</v>
       </c>
-      <c r="AF11" s="158"/>
-      <c r="AG11" s="158"/>
-      <c r="AH11" s="159"/>
-      <c r="AI11" s="157" t="s">
+      <c r="AJ11" s="122"/>
+      <c r="AK11" s="122"/>
+      <c r="AL11" s="123"/>
+      <c r="AM11" s="121" t="s">
         <v>62</v>
       </c>
-      <c r="AJ11" s="158"/>
-      <c r="AK11" s="158"/>
-      <c r="AL11" s="159"/>
-      <c r="AM11" s="157" t="s">
+      <c r="AN11" s="122"/>
+      <c r="AO11" s="122"/>
+      <c r="AP11" s="123"/>
+      <c r="AQ11" s="121" t="s">
         <v>63</v>
       </c>
-      <c r="AN11" s="158"/>
-      <c r="AO11" s="158"/>
-      <c r="AP11" s="159"/>
-      <c r="AQ11" s="157" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR11" s="158"/>
-      <c r="AS11" s="158"/>
-      <c r="AT11" s="159"/>
+      <c r="AR11" s="122"/>
+      <c r="AS11" s="122"/>
+      <c r="AT11" s="123"/>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A12" s="176"/>
-      <c r="B12" s="175"/>
-      <c r="C12" s="171"/>
-      <c r="D12" s="170"/>
-      <c r="E12" s="171"/>
-      <c r="F12" s="170"/>
+      <c r="A12" s="143"/>
+      <c r="B12" s="142"/>
+      <c r="C12" s="138"/>
+      <c r="D12" s="137"/>
+      <c r="E12" s="138"/>
+      <c r="F12" s="137"/>
       <c r="G12" s="10">
         <v>1</v>
       </c>
@@ -2590,12 +2600,12 @@
       </c>
     </row>
     <row r="13" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="177"/>
-      <c r="B13" s="178"/>
-      <c r="C13" s="172"/>
-      <c r="D13" s="173"/>
-      <c r="E13" s="172"/>
-      <c r="F13" s="173"/>
+      <c r="A13" s="144"/>
+      <c r="B13" s="145"/>
+      <c r="C13" s="139"/>
+      <c r="D13" s="140"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="140"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
@@ -2638,20 +2648,20 @@
       <c r="AT13" s="16"/>
     </row>
     <row r="14" spans="1:59" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="160" t="s">
+      <c r="A14" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="161"/>
-      <c r="C14" s="162">
+      <c r="B14" s="125"/>
+      <c r="C14" s="126">
         <f>SUM(C15:D16)</f>
         <v>6</v>
       </c>
-      <c r="D14" s="163"/>
-      <c r="E14" s="162">
+      <c r="D14" s="127"/>
+      <c r="E14" s="126">
         <f>SUM(E15)</f>
         <v>6</v>
       </c>
-      <c r="F14" s="163"/>
+      <c r="F14" s="127"/>
       <c r="G14" s="18"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
@@ -2694,18 +2704,18 @@
       <c r="AT14" s="20"/>
     </row>
     <row r="15" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="120" t="s">
+      <c r="A15" s="128" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="164"/>
-      <c r="C15" s="167">
+      <c r="B15" s="129"/>
+      <c r="C15" s="132">
         <v>6</v>
       </c>
-      <c r="D15" s="140"/>
-      <c r="E15" s="167">
+      <c r="D15" s="133"/>
+      <c r="E15" s="132">
         <v>6</v>
       </c>
-      <c r="F15" s="140"/>
+      <c r="F15" s="133"/>
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
       <c r="I15" s="26"/>
@@ -2748,12 +2758,12 @@
       <c r="AT15" s="50"/>
     </row>
     <row r="16" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="165"/>
-      <c r="B16" s="166"/>
-      <c r="C16" s="168"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="168"/>
-      <c r="F16" s="142"/>
+      <c r="A16" s="130"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="134"/>
+      <c r="D16" s="135"/>
+      <c r="E16" s="134"/>
+      <c r="F16" s="135"/>
       <c r="G16" s="30"/>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
@@ -2789,20 +2799,20 @@
       <c r="AT16" s="54"/>
     </row>
     <row r="17" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="116" t="s">
+      <c r="A17" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="117"/>
-      <c r="C17" s="118">
+      <c r="B17" s="151"/>
+      <c r="C17" s="152">
         <f>SUM(C18:D25)</f>
         <v>12</v>
       </c>
-      <c r="D17" s="119"/>
-      <c r="E17" s="150">
+      <c r="D17" s="153"/>
+      <c r="E17" s="154">
         <f>SUM(E18:F25)</f>
         <v>10</v>
       </c>
-      <c r="F17" s="151"/>
+      <c r="F17" s="155"/>
       <c r="G17" s="31"/>
       <c r="H17" s="32"/>
       <c r="I17" s="32"/>
@@ -2845,7 +2855,7 @@
       <c r="AT17" s="33"/>
     </row>
     <row r="18" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="120" t="s">
+      <c r="A18" s="128" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="113"/>
@@ -2899,7 +2909,7 @@
       <c r="AT18" s="35"/>
     </row>
     <row r="19" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="121"/>
+      <c r="A19" s="156"/>
       <c r="B19" s="115"/>
       <c r="C19" s="114"/>
       <c r="D19" s="115"/>
@@ -2947,8 +2957,8 @@
       <c r="AT19" s="35"/>
     </row>
     <row r="20" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="120" t="s">
-        <v>65</v>
+      <c r="A20" s="128" t="s">
+        <v>64</v>
       </c>
       <c r="B20" s="113"/>
       <c r="C20" s="112">
@@ -3001,7 +3011,7 @@
       <c r="AT20" s="35"/>
     </row>
     <row r="21" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="121"/>
+      <c r="A21" s="156"/>
       <c r="B21" s="115"/>
       <c r="C21" s="114"/>
       <c r="D21" s="115"/>
@@ -3050,7 +3060,7 @@
     </row>
     <row r="22" spans="1:46" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="108" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" s="109"/>
       <c r="C22" s="112">
@@ -3151,17 +3161,17 @@
     </row>
     <row r="24" spans="1:46" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="108" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B24" s="109"/>
       <c r="C24" s="112">
         <v>2</v>
       </c>
       <c r="D24" s="113"/>
-      <c r="E24" s="152">
+      <c r="E24" s="146">
         <v>2</v>
       </c>
-      <c r="F24" s="153"/>
+      <c r="F24" s="147"/>
       <c r="G24" s="25"/>
       <c r="H24" s="81"/>
       <c r="I24" s="26"/>
@@ -3210,8 +3220,8 @@
       <c r="B25" s="111"/>
       <c r="C25" s="114"/>
       <c r="D25" s="115"/>
-      <c r="E25" s="154"/>
-      <c r="F25" s="155"/>
+      <c r="E25" s="148"/>
+      <c r="F25" s="149"/>
       <c r="G25" s="25"/>
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
@@ -3256,20 +3266,20 @@
       <c r="AT25" s="35"/>
     </row>
     <row r="26" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="116" t="s">
+      <c r="A26" s="150" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="117"/>
-      <c r="C26" s="118">
+      <c r="B26" s="151"/>
+      <c r="C26" s="152">
         <f>SUM(C27)</f>
         <v>2</v>
       </c>
-      <c r="D26" s="119"/>
-      <c r="E26" s="150">
+      <c r="D26" s="153"/>
+      <c r="E26" s="154">
         <f>SUM(E27)</f>
         <v>3</v>
       </c>
-      <c r="F26" s="151"/>
+      <c r="F26" s="155"/>
       <c r="G26" s="31"/>
       <c r="H26" s="32"/>
       <c r="I26" s="32"/>
@@ -3312,7 +3322,7 @@
       <c r="AT26" s="33"/>
     </row>
     <row r="27" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="120" t="s">
+      <c r="A27" s="128" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="113"/>
@@ -3367,7 +3377,7 @@
       <c r="AT27" s="35"/>
     </row>
     <row r="28" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="121"/>
+      <c r="A28" s="156"/>
       <c r="B28" s="115"/>
       <c r="C28" s="114"/>
       <c r="D28" s="115"/>
@@ -3417,20 +3427,20 @@
       <c r="AT28" s="35"/>
     </row>
     <row r="29" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="116" t="s">
+      <c r="A29" s="150" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="117"/>
-      <c r="C29" s="118">
+      <c r="B29" s="151"/>
+      <c r="C29" s="152">
         <f>SUM(C30:D41)</f>
         <v>12</v>
       </c>
-      <c r="D29" s="119"/>
-      <c r="E29" s="118">
+      <c r="D29" s="153"/>
+      <c r="E29" s="152">
         <f>SUM(E30:F41)</f>
         <v>25</v>
       </c>
-      <c r="F29" s="119"/>
+      <c r="F29" s="153"/>
       <c r="G29" s="31"/>
       <c r="H29" s="32"/>
       <c r="I29" s="32"/>
@@ -3474,17 +3484,17 @@
     </row>
     <row r="30" spans="1:46" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="108" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B30" s="109"/>
       <c r="C30" s="112">
         <v>2</v>
       </c>
       <c r="D30" s="113"/>
-      <c r="E30" s="132">
+      <c r="E30" s="116">
         <v>1</v>
       </c>
-      <c r="F30" s="133"/>
+      <c r="F30" s="117"/>
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
@@ -3531,8 +3541,8 @@
       <c r="B31" s="111"/>
       <c r="C31" s="114"/>
       <c r="D31" s="115"/>
-      <c r="E31" s="134"/>
-      <c r="F31" s="135"/>
+      <c r="E31" s="118"/>
+      <c r="F31" s="119"/>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
@@ -3576,17 +3586,17 @@
     </row>
     <row r="32" spans="1:46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="108" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" s="109"/>
       <c r="C32" s="112">
         <v>2</v>
       </c>
       <c r="D32" s="113"/>
-      <c r="E32" s="132">
+      <c r="E32" s="116">
         <v>2</v>
       </c>
-      <c r="F32" s="133"/>
+      <c r="F32" s="117"/>
       <c r="G32" s="25"/>
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
@@ -3633,8 +3643,8 @@
       <c r="B33" s="111"/>
       <c r="C33" s="114"/>
       <c r="D33" s="115"/>
-      <c r="E33" s="134"/>
-      <c r="F33" s="135"/>
+      <c r="E33" s="118"/>
+      <c r="F33" s="119"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3678,7 +3688,7 @@
     </row>
     <row r="34" spans="1:46" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="108" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B34" s="109"/>
       <c r="C34" s="112">
@@ -3780,7 +3790,7 @@
     </row>
     <row r="36" spans="1:46" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="108" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B36" s="109"/>
       <c r="C36" s="112">
@@ -3881,7 +3891,7 @@
       <c r="AT37" s="35"/>
     </row>
     <row r="38" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="120" t="s">
+      <c r="A38" s="128" t="s">
         <v>29</v>
       </c>
       <c r="B38" s="113"/>
@@ -3935,7 +3945,7 @@
       <c r="AT38" s="35"/>
     </row>
     <row r="39" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="121"/>
+      <c r="A39" s="156"/>
       <c r="B39" s="115"/>
       <c r="C39" s="114"/>
       <c r="D39" s="115"/>
@@ -4064,7 +4074,7 @@
       <c r="W41" s="103"/>
       <c r="X41" s="55"/>
       <c r="Y41" s="55"/>
-      <c r="Z41" s="102" t="s">
+      <c r="Z41" s="181" t="s">
         <v>31</v>
       </c>
       <c r="AA41" s="25"/>
@@ -4089,20 +4099,20 @@
       <c r="AT41" s="35"/>
     </row>
     <row r="42" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="116" t="s">
+      <c r="A42" s="150" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="117"/>
-      <c r="C42" s="118">
+      <c r="B42" s="151"/>
+      <c r="C42" s="152">
         <f>SUM(C43:C45)</f>
         <v>3</v>
       </c>
-      <c r="D42" s="119"/>
-      <c r="E42" s="118">
+      <c r="D42" s="153"/>
+      <c r="E42" s="152">
         <f>SUM(E45+E43)</f>
         <v>2</v>
       </c>
-      <c r="F42" s="119"/>
+      <c r="F42" s="153"/>
       <c r="G42" s="31"/>
       <c r="H42" s="32"/>
       <c r="I42" s="32"/>
@@ -4145,18 +4155,18 @@
       <c r="AT42" s="33"/>
     </row>
     <row r="43" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="143" t="s">
-        <v>66</v>
-      </c>
-      <c r="B43" s="144"/>
-      <c r="C43" s="143">
+      <c r="A43" s="158" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="159"/>
+      <c r="C43" s="158">
         <v>2</v>
       </c>
-      <c r="D43" s="147"/>
-      <c r="E43" s="143">
+      <c r="D43" s="162"/>
+      <c r="E43" s="158">
         <v>1</v>
       </c>
-      <c r="F43" s="147"/>
+      <c r="F43" s="162"/>
       <c r="G43" s="84"/>
       <c r="H43" s="81"/>
       <c r="I43" s="81"/>
@@ -4199,12 +4209,12 @@
       <c r="AT43" s="54"/>
     </row>
     <row r="44" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="145"/>
-      <c r="B44" s="146"/>
-      <c r="C44" s="148"/>
-      <c r="D44" s="149"/>
-      <c r="E44" s="148"/>
-      <c r="F44" s="149"/>
+      <c r="A44" s="160"/>
+      <c r="B44" s="161"/>
+      <c r="C44" s="163"/>
+      <c r="D44" s="164"/>
+      <c r="E44" s="163"/>
+      <c r="F44" s="164"/>
       <c r="G44" s="84"/>
       <c r="H44" s="81"/>
       <c r="I44" s="81"/>
@@ -4247,10 +4257,10 @@
       <c r="AT44" s="54"/>
     </row>
     <row r="45" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="120" t="s">
-        <v>67</v>
-      </c>
-      <c r="B45" s="140"/>
+      <c r="A45" s="128" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="133"/>
       <c r="C45" s="112">
         <v>1</v>
       </c>
@@ -4303,8 +4313,8 @@
       <c r="AT45" s="35"/>
     </row>
     <row r="46" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="141"/>
-      <c r="B46" s="142"/>
+      <c r="A46" s="157"/>
+      <c r="B46" s="135"/>
       <c r="C46" s="114"/>
       <c r="D46" s="115"/>
       <c r="E46" s="114"/>
@@ -4329,7 +4339,7 @@
       <c r="X46" s="26"/>
       <c r="Y46" s="26"/>
       <c r="Z46" s="35"/>
-      <c r="AA46" s="103" t="s">
+      <c r="AA46" s="71" t="s">
         <v>33</v>
       </c>
       <c r="AB46" s="26"/>
@@ -4353,20 +4363,20 @@
       <c r="AT46" s="35"/>
     </row>
     <row r="47" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="116" t="s">
+      <c r="A47" s="150" t="s">
         <v>34</v>
       </c>
-      <c r="B47" s="117"/>
-      <c r="C47" s="118">
+      <c r="B47" s="151"/>
+      <c r="C47" s="152">
         <f>SUM(C48:D63)</f>
         <v>19</v>
       </c>
-      <c r="D47" s="119"/>
-      <c r="E47" s="118">
+      <c r="D47" s="153"/>
+      <c r="E47" s="152">
         <f>SUM(E48:F63)</f>
         <v>15</v>
       </c>
-      <c r="F47" s="119"/>
+      <c r="F47" s="153"/>
       <c r="G47" s="31"/>
       <c r="H47" s="32"/>
       <c r="I47" s="32"/>
@@ -4409,10 +4419,10 @@
       <c r="AT47" s="33"/>
     </row>
     <row r="48" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="136" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" s="137"/>
+      <c r="A48" s="165" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="166"/>
       <c r="C48" s="112">
         <v>0.5</v>
       </c>
@@ -4463,8 +4473,8 @@
       <c r="AT48" s="35"/>
     </row>
     <row r="49" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="138"/>
-      <c r="B49" s="139"/>
+      <c r="A49" s="167"/>
+      <c r="B49" s="168"/>
       <c r="C49" s="114"/>
       <c r="D49" s="115"/>
       <c r="E49" s="114"/>
@@ -4511,18 +4521,18 @@
       <c r="AT49" s="35"/>
     </row>
     <row r="50" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A50" s="120" t="s">
-        <v>70</v>
+      <c r="A50" s="128" t="s">
+        <v>69</v>
       </c>
       <c r="B50" s="113"/>
       <c r="C50" s="112">
         <v>0.5</v>
       </c>
       <c r="D50" s="113"/>
-      <c r="E50" s="132">
+      <c r="E50" s="116">
         <v>0.5</v>
       </c>
-      <c r="F50" s="133"/>
+      <c r="F50" s="117"/>
       <c r="G50" s="25"/>
       <c r="H50" s="26"/>
       <c r="I50" s="26"/>
@@ -4565,12 +4575,12 @@
       <c r="AT50" s="35"/>
     </row>
     <row r="51" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="121"/>
+      <c r="A51" s="156"/>
       <c r="B51" s="115"/>
       <c r="C51" s="114"/>
       <c r="D51" s="115"/>
-      <c r="E51" s="134"/>
-      <c r="F51" s="135"/>
+      <c r="E51" s="118"/>
+      <c r="F51" s="119"/>
       <c r="G51" s="25"/>
       <c r="H51" s="26"/>
       <c r="I51" s="26"/>
@@ -4613,18 +4623,18 @@
       <c r="AT51" s="35"/>
     </row>
     <row r="52" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A52" s="120" t="s">
-        <v>71</v>
+      <c r="A52" s="128" t="s">
+        <v>70</v>
       </c>
       <c r="B52" s="113"/>
       <c r="C52" s="112">
         <v>2</v>
       </c>
       <c r="D52" s="113"/>
-      <c r="E52" s="132">
+      <c r="E52" s="116">
         <v>1.5</v>
       </c>
-      <c r="F52" s="133"/>
+      <c r="F52" s="117"/>
       <c r="G52" s="25"/>
       <c r="H52" s="26"/>
       <c r="I52" s="26"/>
@@ -4667,12 +4677,12 @@
       <c r="AT52" s="35"/>
     </row>
     <row r="53" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="121"/>
+      <c r="A53" s="156"/>
       <c r="B53" s="115"/>
       <c r="C53" s="114"/>
       <c r="D53" s="115"/>
-      <c r="E53" s="134"/>
-      <c r="F53" s="135"/>
+      <c r="E53" s="118"/>
+      <c r="F53" s="119"/>
       <c r="G53" s="25"/>
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
@@ -4715,18 +4725,18 @@
       <c r="AT53" s="35"/>
     </row>
     <row r="54" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="120" t="s">
-        <v>73</v>
+      <c r="A54" s="128" t="s">
+        <v>72</v>
       </c>
       <c r="B54" s="113"/>
       <c r="C54" s="112">
         <v>2</v>
       </c>
       <c r="D54" s="113"/>
-      <c r="E54" s="132">
+      <c r="E54" s="116">
         <v>1.5</v>
       </c>
-      <c r="F54" s="133"/>
+      <c r="F54" s="117"/>
       <c r="G54" s="25"/>
       <c r="H54" s="26"/>
       <c r="I54" s="26"/>
@@ -4769,12 +4779,12 @@
       <c r="AT54" s="35"/>
     </row>
     <row r="55" spans="1:46" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="121"/>
+      <c r="A55" s="156"/>
       <c r="B55" s="115"/>
       <c r="C55" s="114"/>
       <c r="D55" s="115"/>
-      <c r="E55" s="134"/>
-      <c r="F55" s="135"/>
+      <c r="E55" s="118"/>
+      <c r="F55" s="119"/>
       <c r="G55" s="25"/>
       <c r="H55" s="26"/>
       <c r="I55" s="26"/>
@@ -4817,7 +4827,7 @@
     </row>
     <row r="56" spans="1:46" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="108" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B56" s="109"/>
       <c r="C56" s="112">
@@ -4919,7 +4929,7 @@
     </row>
     <row r="58" spans="1:46" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="108" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B58" s="109"/>
       <c r="C58" s="112">
@@ -5123,7 +5133,7 @@
     </row>
     <row r="62" spans="1:46" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="108" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B62" s="109"/>
       <c r="C62" s="112">
@@ -5213,7 +5223,7 @@
       <c r="AG63" s="59"/>
       <c r="AH63" s="59"/>
       <c r="AI63" s="103"/>
-      <c r="AJ63" s="55" t="s">
+      <c r="AJ63" s="72" t="s">
         <v>36</v>
       </c>
       <c r="AK63" s="26"/>
@@ -5228,20 +5238,20 @@
       <c r="AT63" s="35"/>
     </row>
     <row r="64" spans="1:46" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="116" t="s">
+      <c r="A64" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="B64" s="117"/>
-      <c r="C64" s="118">
+      <c r="B64" s="151"/>
+      <c r="C64" s="152">
         <f>SUM(C65:D66)</f>
         <v>4</v>
       </c>
-      <c r="D64" s="119"/>
-      <c r="E64" s="118">
+      <c r="D64" s="153"/>
+      <c r="E64" s="152">
         <f>SUM(E65)</f>
         <v>8</v>
       </c>
-      <c r="F64" s="119"/>
+      <c r="F64" s="153"/>
       <c r="G64" s="31"/>
       <c r="H64" s="32"/>
       <c r="I64" s="32"/>
@@ -5284,7 +5294,7 @@
       <c r="AT64" s="33"/>
     </row>
     <row r="65" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="120" t="s">
+      <c r="A65" s="128" t="s">
         <v>38</v>
       </c>
       <c r="B65" s="113"/>
@@ -5340,7 +5350,7 @@
       <c r="AT65" s="35"/>
     </row>
     <row r="66" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="121"/>
+      <c r="A66" s="156"/>
       <c r="B66" s="115"/>
       <c r="C66" s="114"/>
       <c r="D66" s="115"/>
@@ -5377,7 +5387,7 @@
       <c r="AI66" s="106"/>
       <c r="AJ66" s="26"/>
       <c r="AK66" s="55"/>
-      <c r="AL66" s="70" t="s">
+      <c r="AL66" s="180" t="s">
         <v>39</v>
       </c>
       <c r="AM66" s="27"/>
@@ -5390,20 +5400,20 @@
       <c r="AT66" s="35"/>
     </row>
     <row r="67" spans="1:59" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="116" t="s">
+      <c r="A67" s="150" t="s">
         <v>40</v>
       </c>
-      <c r="B67" s="117"/>
-      <c r="C67" s="118">
+      <c r="B67" s="151"/>
+      <c r="C67" s="152">
         <f>SUM(C68:D69)</f>
         <v>4</v>
       </c>
-      <c r="D67" s="119"/>
-      <c r="E67" s="118">
+      <c r="D67" s="153"/>
+      <c r="E67" s="152">
         <f>SUM(E68)</f>
         <v>2</v>
       </c>
-      <c r="F67" s="119"/>
+      <c r="F67" s="153"/>
       <c r="G67" s="31"/>
       <c r="H67" s="32"/>
       <c r="I67" s="32"/>
@@ -5446,7 +5456,7 @@
       <c r="AT67" s="33"/>
     </row>
     <row r="68" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A68" s="120" t="s">
+      <c r="A68" s="128" t="s">
         <v>41</v>
       </c>
       <c r="B68" s="113"/>
@@ -5503,7 +5513,7 @@
       <c r="AU68" s="38"/>
     </row>
     <row r="69" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A69" s="121"/>
+      <c r="A69" s="156"/>
       <c r="B69" s="115"/>
       <c r="C69" s="114"/>
       <c r="D69" s="115"/>
@@ -5541,7 +5551,7 @@
       <c r="AJ69" s="81"/>
       <c r="AK69" s="81"/>
       <c r="AL69" s="56"/>
-      <c r="AM69" s="73" t="s">
+      <c r="AM69" s="179" t="s">
         <v>42</v>
       </c>
       <c r="AN69" s="26"/>
@@ -5554,20 +5564,20 @@
       <c r="AU69" s="39"/>
     </row>
     <row r="70" spans="1:59" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="128" t="s">
+      <c r="A70" s="175" t="s">
         <v>43</v>
       </c>
-      <c r="B70" s="129"/>
-      <c r="C70" s="130">
+      <c r="B70" s="176"/>
+      <c r="C70" s="177">
         <f>SUM(C71:D76)</f>
         <v>18</v>
       </c>
-      <c r="D70" s="131"/>
-      <c r="E70" s="118">
+      <c r="D70" s="178"/>
+      <c r="E70" s="152">
         <f>SUM(E71:F76)</f>
         <v>14</v>
       </c>
-      <c r="F70" s="119"/>
+      <c r="F70" s="153"/>
       <c r="G70" s="40"/>
       <c r="H70" s="41"/>
       <c r="I70" s="41"/>
@@ -5611,7 +5621,7 @@
       <c r="AU70" s="3"/>
     </row>
     <row r="71" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A71" s="120" t="s">
+      <c r="A71" s="128" t="s">
         <v>44</v>
       </c>
       <c r="B71" s="113"/>
@@ -5666,7 +5676,7 @@
       <c r="AU71" s="3"/>
     </row>
     <row r="72" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A72" s="121"/>
+      <c r="A72" s="156"/>
       <c r="B72" s="115"/>
       <c r="C72" s="114"/>
       <c r="D72" s="115"/>
@@ -5727,7 +5737,7 @@
       <c r="BG72" s="38"/>
     </row>
     <row r="73" spans="1:59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="120" t="s">
+      <c r="A73" s="128" t="s">
         <v>45</v>
       </c>
       <c r="B73" s="113"/>
@@ -5736,7 +5746,7 @@
       </c>
       <c r="D73" s="113"/>
       <c r="E73" s="112">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F73" s="113"/>
       <c r="G73" s="25"/>
@@ -5796,7 +5806,7 @@
       <c r="BG73" s="38"/>
     </row>
     <row r="74" spans="1:59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="121"/>
+      <c r="A74" s="156"/>
       <c r="B74" s="115"/>
       <c r="C74" s="114"/>
       <c r="D74" s="115"/>
@@ -5836,10 +5846,12 @@
       <c r="AL74" s="54"/>
       <c r="AM74" s="86"/>
       <c r="AN74" s="81"/>
-      <c r="AO74" s="81"/>
-      <c r="AP74" s="56"/>
-      <c r="AQ74" s="27"/>
-      <c r="AR74" s="26"/>
+      <c r="AO74" s="83"/>
+      <c r="AP74" s="70"/>
+      <c r="AQ74" s="73"/>
+      <c r="AR74" s="72" t="s">
+        <v>46</v>
+      </c>
       <c r="AS74" s="26"/>
       <c r="AT74" s="56"/>
       <c r="AU74" s="3"/>
@@ -5857,8 +5869,8 @@
       <c r="BG74" s="38"/>
     </row>
     <row r="75" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A75" s="120" t="s">
-        <v>77</v>
+      <c r="A75" s="128" t="s">
+        <v>76</v>
       </c>
       <c r="B75" s="113"/>
       <c r="C75" s="112">
@@ -5866,7 +5878,7 @@
       </c>
       <c r="D75" s="113"/>
       <c r="E75" s="112">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F75" s="113"/>
       <c r="G75" s="25"/>
@@ -5924,7 +5936,7 @@
       <c r="BG75" s="39"/>
     </row>
     <row r="76" spans="1:59" ht="18" x14ac:dyDescent="0.25">
-      <c r="A76" s="121"/>
+      <c r="A76" s="156"/>
       <c r="B76" s="115"/>
       <c r="C76" s="114"/>
       <c r="D76" s="115"/>
@@ -5968,8 +5980,8 @@
       <c r="AP76" s="54"/>
       <c r="AQ76" s="86"/>
       <c r="AR76" s="81"/>
-      <c r="AS76" s="81"/>
-      <c r="AT76" s="54"/>
+      <c r="AS76" s="83"/>
+      <c r="AT76" s="182"/>
       <c r="AU76" s="3"/>
       <c r="AV76" s="3"/>
       <c r="AW76" s="3"/>
@@ -6046,20 +6058,20 @@
       <c r="BG77" s="3"/>
     </row>
     <row r="78" spans="1:59" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="122" t="s">
+      <c r="A78" s="169" t="s">
         <v>47</v>
       </c>
-      <c r="B78" s="123"/>
-      <c r="C78" s="124">
+      <c r="B78" s="170"/>
+      <c r="C78" s="171">
         <f>SUM(C14+C17+C29+C42+C47+C64+C67+C26 + C70)</f>
         <v>80</v>
       </c>
-      <c r="D78" s="125"/>
-      <c r="E78" s="126">
+      <c r="D78" s="172"/>
+      <c r="E78" s="173">
         <f>SUM(E14+E17+E29+E42+E47+E64+E67+E26+E70)</f>
         <v>85</v>
       </c>
-      <c r="F78" s="127"/>
+      <c r="F78" s="174"/>
       <c r="G78" s="39"/>
       <c r="H78" s="39"/>
       <c r="I78" s="39"/>
@@ -6177,6 +6189,107 @@
     </row>
   </sheetData>
   <mergeCells count="125">
+    <mergeCell ref="A60:B61"/>
+    <mergeCell ref="C60:D61"/>
+    <mergeCell ref="E60:F61"/>
+    <mergeCell ref="A62:B63"/>
+    <mergeCell ref="C62:D63"/>
+    <mergeCell ref="E62:F63"/>
+    <mergeCell ref="A56:B57"/>
+    <mergeCell ref="C56:D57"/>
+    <mergeCell ref="E56:F57"/>
+    <mergeCell ref="A58:B59"/>
+    <mergeCell ref="C58:D59"/>
+    <mergeCell ref="E58:F59"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="A68:B69"/>
+    <mergeCell ref="C68:D69"/>
+    <mergeCell ref="E68:F69"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="A65:B66"/>
+    <mergeCell ref="C65:D66"/>
+    <mergeCell ref="E65:F66"/>
+    <mergeCell ref="A75:B76"/>
+    <mergeCell ref="C75:D76"/>
+    <mergeCell ref="E75:F76"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="A71:B72"/>
+    <mergeCell ref="C71:D72"/>
+    <mergeCell ref="E71:F72"/>
+    <mergeCell ref="A73:B74"/>
+    <mergeCell ref="C73:D74"/>
+    <mergeCell ref="E73:F74"/>
+    <mergeCell ref="A52:B53"/>
+    <mergeCell ref="C52:D53"/>
+    <mergeCell ref="E52:F53"/>
+    <mergeCell ref="A54:B55"/>
+    <mergeCell ref="C54:D55"/>
+    <mergeCell ref="E54:F55"/>
+    <mergeCell ref="A48:B49"/>
+    <mergeCell ref="C48:D49"/>
+    <mergeCell ref="E48:F49"/>
+    <mergeCell ref="A50:B51"/>
+    <mergeCell ref="C50:D51"/>
+    <mergeCell ref="E50:F51"/>
+    <mergeCell ref="A45:B46"/>
+    <mergeCell ref="C45:D46"/>
+    <mergeCell ref="E45:F46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="A40:B41"/>
+    <mergeCell ref="C40:D41"/>
+    <mergeCell ref="E40:F41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="C43:D44"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="A38:B39"/>
+    <mergeCell ref="C38:D39"/>
+    <mergeCell ref="E38:F39"/>
+    <mergeCell ref="A34:B35"/>
+    <mergeCell ref="C34:D35"/>
+    <mergeCell ref="E34:F35"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="E36:F37"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="E30:F31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:F28"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="E22:F23"/>
+    <mergeCell ref="A24:B25"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="E24:F25"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="E20:F21"/>
     <mergeCell ref="A32:B33"/>
     <mergeCell ref="C32:D33"/>
     <mergeCell ref="E32:F33"/>
@@ -6201,107 +6314,6 @@
     <mergeCell ref="C11:D13"/>
     <mergeCell ref="A11:B13"/>
     <mergeCell ref="A22:B23"/>
-    <mergeCell ref="C22:D23"/>
-    <mergeCell ref="E22:F23"/>
-    <mergeCell ref="A24:B25"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="E24:F25"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="E20:F21"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="E30:F31"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:F28"/>
-    <mergeCell ref="A38:B39"/>
-    <mergeCell ref="C38:D39"/>
-    <mergeCell ref="E38:F39"/>
-    <mergeCell ref="A34:B35"/>
-    <mergeCell ref="C34:D35"/>
-    <mergeCell ref="E34:F35"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="E36:F37"/>
-    <mergeCell ref="A45:B46"/>
-    <mergeCell ref="C45:D46"/>
-    <mergeCell ref="E45:F46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="A40:B41"/>
-    <mergeCell ref="C40:D41"/>
-    <mergeCell ref="E40:F41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="C43:D44"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="A52:B53"/>
-    <mergeCell ref="C52:D53"/>
-    <mergeCell ref="E52:F53"/>
-    <mergeCell ref="A54:B55"/>
-    <mergeCell ref="C54:D55"/>
-    <mergeCell ref="E54:F55"/>
-    <mergeCell ref="A48:B49"/>
-    <mergeCell ref="C48:D49"/>
-    <mergeCell ref="E48:F49"/>
-    <mergeCell ref="A50:B51"/>
-    <mergeCell ref="C50:D51"/>
-    <mergeCell ref="E50:F51"/>
-    <mergeCell ref="A75:B76"/>
-    <mergeCell ref="C75:D76"/>
-    <mergeCell ref="E75:F76"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="A71:B72"/>
-    <mergeCell ref="C71:D72"/>
-    <mergeCell ref="E71:F72"/>
-    <mergeCell ref="A73:B74"/>
-    <mergeCell ref="C73:D74"/>
-    <mergeCell ref="E73:F74"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="A68:B69"/>
-    <mergeCell ref="C68:D69"/>
-    <mergeCell ref="E68:F69"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="A65:B66"/>
-    <mergeCell ref="C65:D66"/>
-    <mergeCell ref="E65:F66"/>
-    <mergeCell ref="A60:B61"/>
-    <mergeCell ref="C60:D61"/>
-    <mergeCell ref="E60:F61"/>
-    <mergeCell ref="A62:B63"/>
-    <mergeCell ref="C62:D63"/>
-    <mergeCell ref="E62:F63"/>
-    <mergeCell ref="A56:B57"/>
-    <mergeCell ref="C56:D57"/>
-    <mergeCell ref="E56:F57"/>
-    <mergeCell ref="A58:B59"/>
-    <mergeCell ref="C58:D59"/>
-    <mergeCell ref="E58:F59"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>